<commit_message>
change over to quarto
</commit_message>
<xml_diff>
--- a/scoring/EDGI_exercise_scoresheet.xlsx
+++ b/scoring/EDGI_exercise_scoresheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kschaumberg/Dropbox/Wisconsin/Papers (External)/EDGI Exercise/Analyses/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kschaumberg/Dropbox/Wisconsin/Papers (External)/EDGI Exercise/Analyses/scoring/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{134BD0B6-424E-4441-B84A-9C8C3E743E15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F8A35A-FAA8-B540-B326-4C5F2E0536F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="16400" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ED100k" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2756" uniqueCount="640">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2756" uniqueCount="638">
   <si>
     <t>raw_vars</t>
   </si>
@@ -1091,9 +1091,6 @@
     <t>&gt;1 month of psychologically driven exercise every day or nearly every day</t>
   </si>
   <si>
-    <t xml:space="preserve">Reports exercised excessively (compulsively) in a way that was 'more often/became a habit' OR any exercise that is compensatory </t>
-  </si>
-  <si>
     <t>Compulsive/Driven Exercise that lasted for at least one month</t>
   </si>
   <si>
@@ -1109,9 +1106,6 @@
     <t>ED100k_ex_compulsive</t>
   </si>
   <si>
-    <t>ED100k_ex_maladaptive_any</t>
-  </si>
-  <si>
     <t>ED100k_ex_compulsive_1mo, ED100k_ex_compensatory</t>
   </si>
   <si>
@@ -1583,12 +1577,6 @@
     <t>ED100k_vomit_icb == 0</t>
   </si>
   <si>
-    <t>ED100k_exercise_icb, ED100k_ex_compensatory</t>
-  </si>
-  <si>
-    <t>ED100k_exercise_icb == 0 ~ 0, ED100k_ex_compensatory == 0 ~ 0 , ED100k_exercise_icb== 1 | ED100k_ex_compensatory == 1 ~ 1</t>
-  </si>
-  <si>
     <t>cet_2_appearance</t>
   </si>
   <si>
@@ -1956,6 +1944,12 @@
   </si>
   <si>
     <t>0=0, 1=1, 2=2, -8 = NaN</t>
+  </si>
+  <si>
+    <t>ED100k_ex_compulsive == 0 ~ 0, ED100k_ex_compensatory == 0 ~ 0, ED100k_ex_compulsive == 1 | ED100k_ex_compensatory ==1 ~ 1</t>
+  </si>
+  <si>
+    <t>ED100k_ex_maladaptive_1</t>
   </si>
 </sst>
 </file>
@@ -3079,10 +3073,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L142"/>
+  <dimension ref="A1:L141"/>
   <sheetViews>
-    <sheetView topLeftCell="A78" zoomScale="136" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="L93" sqref="L93"/>
+    <sheetView tabSelected="1" topLeftCell="A125" zoomScale="119" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B128" sqref="B128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3206,7 +3200,7 @@
     </row>
     <row r="4" spans="1:11" s="15" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>11</v>
@@ -3416,13 +3410,13 @@
     </row>
     <row r="10" spans="1:11" s="28" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="26" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="B10" s="26" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="D10" s="26" t="s">
         <v>11</v>
@@ -3431,7 +3425,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="26" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="G10" s="13" t="s">
         <v>11</v>
@@ -3451,13 +3445,13 @@
     </row>
     <row r="11" spans="1:11" s="28" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="26" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="B11" s="26" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="D11" s="26" t="s">
         <v>11</v>
@@ -3466,7 +3460,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="26" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="G11" s="13" t="s">
         <v>11</v>
@@ -3486,13 +3480,13 @@
     </row>
     <row r="12" spans="1:11" s="28" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="26" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="B12" s="26" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="D12" s="26" t="s">
         <v>12</v>
@@ -3501,7 +3495,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="26" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="G12" s="13" t="s">
         <v>11</v>
@@ -3521,7 +3515,7 @@
     </row>
     <row r="13" spans="1:11" s="15" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="B13" s="13" t="s">
         <v>11</v>
@@ -5587,10 +5581,10 @@
     </row>
     <row r="72" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="9" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C72" s="6" t="s">
         <v>96</v>
@@ -5602,10 +5596,10 @@
         <v>2</v>
       </c>
       <c r="F72" s="9" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="G72" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="H72" s="9" t="s">
         <v>11</v>
@@ -5637,10 +5631,10 @@
         <v>2</v>
       </c>
       <c r="F73" s="9" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="G73" s="9" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="H73" s="9" t="s">
         <v>11</v>
@@ -5672,10 +5666,10 @@
         <v>2</v>
       </c>
       <c r="F74" s="9" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="G74" s="9" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="H74" s="9" t="s">
         <v>11</v>
@@ -5707,10 +5701,10 @@
         <v>2</v>
       </c>
       <c r="F75" s="9" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="G75" s="9" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="H75" s="9" t="s">
         <v>11</v>
@@ -5742,10 +5736,10 @@
         <v>2</v>
       </c>
       <c r="F76" s="9" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="G76" s="9" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="H76" s="9" t="s">
         <v>11</v>
@@ -5777,10 +5771,10 @@
         <v>2</v>
       </c>
       <c r="F77" s="9" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="G77" s="9" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="H77" s="9" t="s">
         <v>11</v>
@@ -5812,10 +5806,10 @@
         <v>2</v>
       </c>
       <c r="F78" s="9" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="G78" s="9" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="H78" s="9" t="s">
         <v>11</v>
@@ -5847,10 +5841,10 @@
         <v>2</v>
       </c>
       <c r="F79" s="9" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="G79" s="9" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="H79" s="9" t="s">
         <v>11</v>
@@ -5870,7 +5864,7 @@
         <v>43</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C80" s="6" t="s">
         <v>101</v>
@@ -5882,10 +5876,10 @@
         <v>2</v>
       </c>
       <c r="F80" s="9" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="G80" s="9" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="H80" s="9" t="s">
         <v>11</v>
@@ -5905,10 +5899,10 @@
         <v>40</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="D81" s="9" t="s">
         <v>14</v>
@@ -5917,10 +5911,10 @@
         <v>2</v>
       </c>
       <c r="F81" s="30" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="G81" s="9" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="H81" s="9" t="s">
         <v>11</v>
@@ -5937,13 +5931,13 @@
     </row>
     <row r="82" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="9" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="D82" s="9" t="s">
         <v>333</v>
@@ -5952,7 +5946,7 @@
         <v>3</v>
       </c>
       <c r="F82" s="9" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="G82" s="9" t="s">
         <v>11</v>
@@ -5967,7 +5961,7 @@
         <v>11</v>
       </c>
       <c r="K82" s="9" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
     </row>
     <row r="83" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -5975,7 +5969,7 @@
         <v>59</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C83" s="6" t="s">
         <v>117</v>
@@ -5993,13 +5987,13 @@
         <v>11</v>
       </c>
       <c r="H83" s="9" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="I83" s="9">
         <v>0</v>
       </c>
       <c r="J83" s="9" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="K83" s="9" t="s">
         <v>11</v>
@@ -6010,7 +6004,7 @@
         <v>42</v>
       </c>
       <c r="B84" s="9" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C84" s="6" t="s">
         <v>100</v>
@@ -6028,13 +6022,13 @@
         <v>11</v>
       </c>
       <c r="H84" s="9" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="I84" s="9">
         <v>0</v>
       </c>
       <c r="J84" s="9" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="K84" s="9" t="s">
         <v>11</v>
@@ -6042,16 +6036,16 @@
     </row>
     <row r="85" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="9" t="s">
-        <v>515</v>
+        <v>30</v>
       </c>
       <c r="B85" s="9" t="s">
-        <v>357</v>
+        <v>328</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>351</v>
+        <v>88</v>
       </c>
       <c r="D85" s="9" t="s">
-        <v>333</v>
+        <v>269</v>
       </c>
       <c r="E85" s="9">
         <v>3</v>
@@ -6063,27 +6057,27 @@
         <v>11</v>
       </c>
       <c r="H85" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="I85" s="9" t="s">
-        <v>11</v>
+        <v>285</v>
+      </c>
+      <c r="I85" s="9">
+        <v>0</v>
       </c>
       <c r="J85" s="9" t="s">
-        <v>11</v>
+        <v>286</v>
       </c>
       <c r="K85" s="9" t="s">
-        <v>516</v>
+        <v>11</v>
       </c>
     </row>
     <row r="86" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B86" s="9" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D86" s="9" t="s">
         <v>269</v>
@@ -6104,7 +6098,7 @@
         <v>0</v>
       </c>
       <c r="J86" s="9" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="K86" s="9" t="s">
         <v>11</v>
@@ -6112,13 +6106,13 @@
     </row>
     <row r="87" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="9" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>329</v>
+        <v>379</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>89</v>
+        <v>120</v>
       </c>
       <c r="D87" s="9" t="s">
         <v>269</v>
@@ -6133,13 +6127,13 @@
         <v>11</v>
       </c>
       <c r="H87" s="9" t="s">
-        <v>285</v>
+        <v>511</v>
       </c>
       <c r="I87" s="9">
         <v>0</v>
       </c>
       <c r="J87" s="9" t="s">
-        <v>287</v>
+        <v>380</v>
       </c>
       <c r="K87" s="9" t="s">
         <v>11</v>
@@ -6147,13 +6141,13 @@
     </row>
     <row r="88" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="9" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B88" s="9" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="D88" s="9" t="s">
         <v>269</v>
@@ -6168,13 +6162,13 @@
         <v>11</v>
       </c>
       <c r="H88" s="9" t="s">
-        <v>513</v>
+        <v>373</v>
       </c>
       <c r="I88" s="9">
         <v>0</v>
       </c>
       <c r="J88" s="9" t="s">
-        <v>382</v>
+        <v>630</v>
       </c>
       <c r="K88" s="9" t="s">
         <v>11</v>
@@ -6182,13 +6176,13 @@
     </row>
     <row r="89" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="9" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="B89" s="9" t="s">
-        <v>370</v>
+        <v>602</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>111</v>
+        <v>236</v>
       </c>
       <c r="D89" s="9" t="s">
         <v>269</v>
@@ -6197,19 +6191,19 @@
         <v>3</v>
       </c>
       <c r="F89" s="9" t="s">
-        <v>11</v>
+        <v>603</v>
       </c>
       <c r="G89" s="9" t="s">
         <v>11</v>
       </c>
       <c r="H89" s="9" t="s">
-        <v>375</v>
+        <v>285</v>
       </c>
       <c r="I89" s="9">
         <v>0</v>
       </c>
       <c r="J89" s="9" t="s">
-        <v>634</v>
+        <v>601</v>
       </c>
       <c r="K89" s="9" t="s">
         <v>11</v>
@@ -6217,13 +6211,13 @@
     </row>
     <row r="90" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="9" t="s">
-        <v>36</v>
+        <v>245</v>
       </c>
       <c r="B90" s="9" t="s">
-        <v>606</v>
+        <v>612</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>236</v>
+        <v>613</v>
       </c>
       <c r="D90" s="9" t="s">
         <v>269</v>
@@ -6232,163 +6226,163 @@
         <v>3</v>
       </c>
       <c r="F90" s="9" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="G90" s="9" t="s">
         <v>11</v>
       </c>
       <c r="H90" s="9" t="s">
-        <v>285</v>
+        <v>373</v>
       </c>
       <c r="I90" s="9">
         <v>0</v>
       </c>
       <c r="J90" s="9" t="s">
-        <v>605</v>
+        <v>629</v>
       </c>
       <c r="K90" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="91" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="B91" s="9" t="s">
-        <v>616</v>
-      </c>
-      <c r="C91" s="6" t="s">
-        <v>617</v>
-      </c>
-      <c r="D91" s="9" t="s">
+      <c r="A91" s="29" t="s">
+        <v>604</v>
+      </c>
+      <c r="B91" s="29" t="s">
+        <v>614</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>615</v>
+      </c>
+      <c r="D91" s="29" t="s">
         <v>269</v>
       </c>
-      <c r="E91" s="9">
-        <v>3</v>
-      </c>
-      <c r="F91" s="9" t="s">
-        <v>607</v>
-      </c>
-      <c r="G91" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="H91" s="9" t="s">
-        <v>375</v>
-      </c>
-      <c r="I91" s="9">
-        <v>0</v>
-      </c>
-      <c r="J91" s="9" t="s">
-        <v>633</v>
-      </c>
-      <c r="K91" s="9" t="s">
+      <c r="E91" s="29">
+        <v>4</v>
+      </c>
+      <c r="F91" s="29" t="s">
+        <v>603</v>
+      </c>
+      <c r="G91" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="H91" s="29" t="s">
+        <v>621</v>
+      </c>
+      <c r="I91" s="29">
+        <v>0</v>
+      </c>
+      <c r="J91" s="29" t="s">
+        <v>628</v>
+      </c>
+      <c r="K91" s="29" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="92" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="29" t="s">
-        <v>608</v>
+        <v>614</v>
       </c>
       <c r="B92" s="29" t="s">
+        <v>632</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>633</v>
+      </c>
+      <c r="D92" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="E92" s="29">
+        <v>5</v>
+      </c>
+      <c r="F92" s="29" t="s">
+        <v>634</v>
+      </c>
+      <c r="G92" s="29" t="s">
+        <v>635</v>
+      </c>
+      <c r="H92" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="I92" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="J92" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="K92" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="L92" s="29"/>
+    </row>
+    <row r="93" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="B93" s="9" t="s">
+        <v>616</v>
+      </c>
+      <c r="C93" s="6" t="s">
+        <v>617</v>
+      </c>
+      <c r="D93" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="E93" s="9">
+        <v>3</v>
+      </c>
+      <c r="F93" s="9" t="s">
+        <v>603</v>
+      </c>
+      <c r="G93" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H93" s="9" t="s">
         <v>618</v>
       </c>
-      <c r="C92" s="2" t="s">
-        <v>619</v>
-      </c>
-      <c r="D92" s="29" t="s">
-        <v>269</v>
-      </c>
-      <c r="E92" s="29">
-        <v>4</v>
-      </c>
-      <c r="F92" s="29" t="s">
-        <v>607</v>
-      </c>
-      <c r="G92" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="H92" s="29" t="s">
-        <v>625</v>
-      </c>
-      <c r="I92" s="29">
-        <v>0</v>
-      </c>
-      <c r="J92" s="29" t="s">
-        <v>632</v>
-      </c>
-      <c r="K92" s="29" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="93" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="29" t="s">
-        <v>618</v>
-      </c>
-      <c r="B93" s="29" t="s">
-        <v>636</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>637</v>
-      </c>
-      <c r="D93" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="E93" s="29">
-        <v>5</v>
-      </c>
-      <c r="F93" s="29" t="s">
-        <v>638</v>
-      </c>
-      <c r="G93" s="29" t="s">
-        <v>639</v>
-      </c>
-      <c r="H93" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="I93" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="J93" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="K93" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="L93" s="29"/>
+      <c r="I93" s="9">
+        <v>0</v>
+      </c>
+      <c r="J93" s="9" t="s">
+        <v>631</v>
+      </c>
+      <c r="K93" s="9" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="94" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="9" t="s">
-        <v>244</v>
+      <c r="A94" s="7" t="s">
+        <v>268</v>
       </c>
       <c r="B94" s="9" t="s">
-        <v>620</v>
+        <v>272</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>621</v>
+        <v>407</v>
       </c>
       <c r="D94" s="9" t="s">
-        <v>269</v>
+        <v>333</v>
       </c>
       <c r="E94" s="9">
         <v>3</v>
       </c>
       <c r="F94" s="9" t="s">
-        <v>607</v>
+        <v>542</v>
       </c>
       <c r="G94" s="9" t="s">
         <v>11</v>
       </c>
       <c r="H94" s="9" t="s">
-        <v>622</v>
-      </c>
-      <c r="I94" s="9">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="I94" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="J94" s="9" t="s">
-        <v>635</v>
+        <v>11</v>
       </c>
       <c r="K94" s="9" t="s">
-        <v>11</v>
+        <v>569</v>
       </c>
     </row>
     <row r="95" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -6396,10 +6390,10 @@
         <v>268</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="D95" s="9" t="s">
         <v>333</v>
@@ -6408,7 +6402,7 @@
         <v>3</v>
       </c>
       <c r="F95" s="9" t="s">
-        <v>546</v>
+        <v>568</v>
       </c>
       <c r="G95" s="9" t="s">
         <v>11</v>
@@ -6423,18 +6417,18 @@
         <v>11</v>
       </c>
       <c r="K95" s="9" t="s">
-        <v>573</v>
+        <v>567</v>
       </c>
     </row>
     <row r="96" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="7" t="s">
-        <v>268</v>
+        <v>17</v>
       </c>
       <c r="B96" s="9" t="s">
-        <v>273</v>
+        <v>585</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>408</v>
+        <v>586</v>
       </c>
       <c r="D96" s="9" t="s">
         <v>333</v>
@@ -6443,7 +6437,7 @@
         <v>3</v>
       </c>
       <c r="F96" s="9" t="s">
-        <v>572</v>
+        <v>587</v>
       </c>
       <c r="G96" s="9" t="s">
         <v>11</v>
@@ -6458,53 +6452,53 @@
         <v>11</v>
       </c>
       <c r="K96" s="9" t="s">
-        <v>571</v>
+        <v>588</v>
       </c>
     </row>
     <row r="97" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="7" t="s">
-        <v>17</v>
+      <c r="A97" s="9" t="s">
+        <v>53</v>
       </c>
       <c r="B97" s="9" t="s">
-        <v>589</v>
+        <v>382</v>
       </c>
       <c r="C97" s="6" t="s">
-        <v>590</v>
+        <v>109</v>
       </c>
       <c r="D97" s="9" t="s">
-        <v>333</v>
+        <v>269</v>
       </c>
       <c r="E97" s="9">
         <v>3</v>
       </c>
       <c r="F97" s="9" t="s">
-        <v>591</v>
+        <v>11</v>
       </c>
       <c r="G97" s="9" t="s">
         <v>11</v>
       </c>
       <c r="H97" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="I97" s="9" t="s">
-        <v>11</v>
+        <v>512</v>
+      </c>
+      <c r="I97" s="9">
+        <v>0</v>
       </c>
       <c r="J97" s="9" t="s">
-        <v>11</v>
+        <v>385</v>
       </c>
       <c r="K97" s="9" t="s">
-        <v>592</v>
+        <v>11</v>
       </c>
     </row>
     <row r="98" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="9" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B98" s="9" t="s">
-        <v>384</v>
+        <v>370</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="D98" s="9" t="s">
         <v>269</v>
@@ -6519,13 +6513,13 @@
         <v>11</v>
       </c>
       <c r="H98" s="9" t="s">
-        <v>514</v>
+        <v>372</v>
       </c>
       <c r="I98" s="9">
         <v>0</v>
       </c>
       <c r="J98" s="9" t="s">
-        <v>387</v>
+        <v>378</v>
       </c>
       <c r="K98" s="9" t="s">
         <v>11</v>
@@ -6533,34 +6527,34 @@
     </row>
     <row r="99" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="9" t="s">
-        <v>56</v>
+        <v>374</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D99" s="9" t="s">
-        <v>269</v>
+        <v>14</v>
       </c>
       <c r="E99" s="9">
-        <v>3</v>
-      </c>
-      <c r="F99" s="9" t="s">
-        <v>11</v>
+        <v>4</v>
+      </c>
+      <c r="F99" s="7" t="s">
+        <v>543</v>
       </c>
       <c r="G99" s="9" t="s">
-        <v>11</v>
+        <v>555</v>
       </c>
       <c r="H99" s="9" t="s">
-        <v>374</v>
-      </c>
-      <c r="I99" s="9">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="I99" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="J99" s="9" t="s">
-        <v>380</v>
+        <v>11</v>
       </c>
       <c r="K99" s="9" t="s">
         <v>11</v>
@@ -6568,13 +6562,13 @@
     </row>
     <row r="100" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="9" t="s">
-        <v>376</v>
+        <v>386</v>
       </c>
       <c r="B100" s="9" t="s">
-        <v>377</v>
+        <v>388</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="D100" s="9" t="s">
         <v>14</v>
@@ -6583,10 +6577,10 @@
         <v>4</v>
       </c>
       <c r="F100" s="7" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="G100" s="9" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="H100" s="9" t="s">
         <v>11</v>
@@ -6601,15 +6595,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="101" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="9" t="s">
-        <v>388</v>
+        <v>328</v>
       </c>
       <c r="B101" s="9" t="s">
-        <v>390</v>
+        <v>336</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="D101" s="9" t="s">
         <v>14</v>
@@ -6617,11 +6611,11 @@
       <c r="E101" s="9">
         <v>4</v>
       </c>
-      <c r="F101" s="7" t="s">
-        <v>548</v>
+      <c r="F101" s="9" t="s">
+        <v>541</v>
       </c>
       <c r="G101" s="9" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="H101" s="9" t="s">
         <v>11</v>
@@ -6636,15 +6630,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="102" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:11" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="9" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B102" s="9" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D102" s="9" t="s">
         <v>14</v>
@@ -6653,10 +6647,10 @@
         <v>4</v>
       </c>
       <c r="F102" s="9" t="s">
-        <v>545</v>
+        <v>589</v>
       </c>
       <c r="G102" s="9" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="H102" s="9" t="s">
         <v>11</v>
@@ -6671,15 +6665,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="103" spans="1:11" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="9" t="s">
-        <v>329</v>
+        <v>379</v>
       </c>
       <c r="B103" s="9" t="s">
-        <v>337</v>
+        <v>381</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>89</v>
+        <v>120</v>
       </c>
       <c r="D103" s="9" t="s">
         <v>14</v>
@@ -6687,11 +6681,11 @@
       <c r="E103" s="9">
         <v>4</v>
       </c>
-      <c r="F103" s="9" t="s">
-        <v>593</v>
+      <c r="F103" s="7" t="s">
+        <v>548</v>
       </c>
       <c r="G103" s="9" t="s">
-        <v>561</v>
+        <v>555</v>
       </c>
       <c r="H103" s="9" t="s">
         <v>11</v>
@@ -6706,15 +6700,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="104" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A104" s="9" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="B104" s="9" t="s">
-        <v>383</v>
+        <v>369</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="D104" s="9" t="s">
         <v>14</v>
@@ -6723,10 +6717,10 @@
         <v>4</v>
       </c>
       <c r="F104" s="7" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="G104" s="9" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="H104" s="9" t="s">
         <v>11</v>
@@ -6741,15 +6735,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="105" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" s="9" t="s">
-        <v>370</v>
+        <v>382</v>
       </c>
       <c r="B105" s="9" t="s">
-        <v>371</v>
+        <v>383</v>
       </c>
       <c r="C105" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D105" s="9" t="s">
         <v>14</v>
@@ -6758,10 +6752,10 @@
         <v>4</v>
       </c>
       <c r="F105" s="7" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="G105" s="9" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
       <c r="H105" s="9" t="s">
         <v>11</v>
@@ -6778,13 +6772,13 @@
     </row>
     <row r="106" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="9" t="s">
-        <v>384</v>
+        <v>370</v>
       </c>
       <c r="B106" s="9" t="s">
-        <v>385</v>
+        <v>371</v>
       </c>
       <c r="C106" s="6" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="D106" s="9" t="s">
         <v>14</v>
@@ -6793,10 +6787,10 @@
         <v>4</v>
       </c>
       <c r="F106" s="7" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="G106" s="9" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="H106" s="9" t="s">
         <v>11</v>
@@ -6811,27 +6805,27 @@
         <v>11</v>
       </c>
     </row>
-    <row r="107" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A107" s="9" t="s">
-        <v>372</v>
+        <v>340</v>
       </c>
       <c r="B107" s="9" t="s">
-        <v>373</v>
+        <v>355</v>
       </c>
       <c r="C107" s="6" t="s">
-        <v>114</v>
+        <v>334</v>
       </c>
       <c r="D107" s="9" t="s">
-        <v>14</v>
+        <v>333</v>
       </c>
       <c r="E107" s="9">
-        <v>4</v>
-      </c>
-      <c r="F107" s="7" t="s">
-        <v>555</v>
+        <v>5</v>
+      </c>
+      <c r="F107" s="9" t="s">
+        <v>541</v>
       </c>
       <c r="G107" s="9" t="s">
-        <v>560</v>
+        <v>11</v>
       </c>
       <c r="H107" s="9" t="s">
         <v>11</v>
@@ -6843,53 +6837,53 @@
         <v>11</v>
       </c>
       <c r="K107" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="108" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A108" s="9" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B108" s="9" t="s">
-        <v>356</v>
-      </c>
-      <c r="C108" s="6" t="s">
-        <v>334</v>
+        <v>343</v>
+      </c>
+      <c r="C108" s="5" t="s">
+        <v>342</v>
       </c>
       <c r="D108" s="9" t="s">
-        <v>333</v>
+        <v>269</v>
       </c>
       <c r="E108" s="9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F108" s="9" t="s">
-        <v>545</v>
+        <v>11</v>
       </c>
       <c r="G108" s="9" t="s">
         <v>11</v>
       </c>
       <c r="H108" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="I108" s="9" t="s">
-        <v>11</v>
+        <v>575</v>
+      </c>
+      <c r="I108" s="9">
+        <v>0</v>
       </c>
       <c r="J108" s="9" t="s">
-        <v>11</v>
+        <v>565</v>
       </c>
       <c r="K108" s="9" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="109" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A109" s="9" t="s">
-        <v>341</v>
+        <v>349</v>
       </c>
       <c r="B109" s="9" t="s">
-        <v>343</v>
-      </c>
-      <c r="C109" s="5" t="s">
-        <v>342</v>
+        <v>330</v>
+      </c>
+      <c r="C109" s="6" t="s">
+        <v>93</v>
       </c>
       <c r="D109" s="9" t="s">
         <v>269</v>
@@ -6904,13 +6898,13 @@
         <v>11</v>
       </c>
       <c r="H109" s="9" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="I109" s="9">
         <v>0</v>
       </c>
       <c r="J109" s="9" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
       <c r="K109" s="9" t="s">
         <v>11</v>
@@ -6918,13 +6912,13 @@
     </row>
     <row r="110" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A110" s="9" t="s">
-        <v>349</v>
+        <v>35</v>
       </c>
       <c r="B110" s="9" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="C110" s="6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D110" s="9" t="s">
         <v>269</v>
@@ -6939,13 +6933,13 @@
         <v>11</v>
       </c>
       <c r="H110" s="9" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="I110" s="9">
         <v>0</v>
       </c>
       <c r="J110" s="9" t="s">
-        <v>568</v>
+        <v>290</v>
       </c>
       <c r="K110" s="9" t="s">
         <v>11</v>
@@ -6953,13 +6947,13 @@
     </row>
     <row r="111" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A111" s="9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B111" s="9" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="C111" s="6" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D111" s="9" t="s">
         <v>269</v>
@@ -6974,13 +6968,13 @@
         <v>11</v>
       </c>
       <c r="H111" s="9" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="I111" s="9">
         <v>0</v>
       </c>
       <c r="J111" s="9" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="K111" s="9" t="s">
         <v>11</v>
@@ -6988,13 +6982,13 @@
     </row>
     <row r="112" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A112" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B112" s="9" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D112" s="9" t="s">
         <v>269</v>
@@ -7009,27 +7003,27 @@
         <v>11</v>
       </c>
       <c r="H112" s="9" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="I112" s="9">
         <v>0</v>
       </c>
       <c r="J112" s="9" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="K112" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="113" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" s="9" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B113" s="9" t="s">
-        <v>331</v>
+        <v>578</v>
       </c>
       <c r="C113" s="6" t="s">
-        <v>91</v>
+        <v>576</v>
       </c>
       <c r="D113" s="9" t="s">
         <v>269</v>
@@ -7044,60 +7038,60 @@
         <v>11</v>
       </c>
       <c r="H113" s="9" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="I113" s="9">
         <v>0</v>
       </c>
       <c r="J113" s="9" t="s">
-        <v>289</v>
-      </c>
-      <c r="K113" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="114" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+        <v>577</v>
+      </c>
+      <c r="K113" s="9"/>
+    </row>
+    <row r="114" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A114" s="9" t="s">
-        <v>36</v>
+        <v>330</v>
       </c>
       <c r="B114" s="9" t="s">
-        <v>582</v>
+        <v>365</v>
       </c>
       <c r="C114" s="6" t="s">
-        <v>580</v>
+        <v>93</v>
       </c>
       <c r="D114" s="9" t="s">
-        <v>269</v>
+        <v>14</v>
       </c>
       <c r="E114" s="9">
         <v>6</v>
       </c>
-      <c r="F114" s="9" t="s">
-        <v>11</v>
+      <c r="F114" s="7" t="s">
+        <v>545</v>
       </c>
       <c r="G114" s="9" t="s">
-        <v>11</v>
+        <v>556</v>
       </c>
       <c r="H114" s="9" t="s">
-        <v>579</v>
-      </c>
-      <c r="I114" s="9">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="I114" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="J114" s="9" t="s">
-        <v>581</v>
-      </c>
-      <c r="K114" s="9"/>
-    </row>
-    <row r="115" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="K114" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="9" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="B115" s="9" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="C115" s="6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D115" s="9" t="s">
         <v>14</v>
@@ -7105,11 +7099,11 @@
       <c r="E115" s="9">
         <v>6</v>
       </c>
-      <c r="F115" s="7" t="s">
-        <v>549</v>
+      <c r="F115" s="9" t="s">
+        <v>546</v>
       </c>
       <c r="G115" s="9" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="H115" s="9" t="s">
         <v>11</v>
@@ -7124,15 +7118,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="116" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="9" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="B116" s="9" t="s">
-        <v>366</v>
+        <v>338</v>
       </c>
       <c r="C116" s="6" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D116" s="9" t="s">
         <v>14</v>
@@ -7141,10 +7135,10 @@
         <v>6</v>
       </c>
       <c r="F116" s="9" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="G116" s="9" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
       <c r="H116" s="9" t="s">
         <v>11</v>
@@ -7159,15 +7153,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="117" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="9" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="B117" s="9" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D117" s="9" t="s">
         <v>14</v>
@@ -7176,10 +7170,10 @@
         <v>6</v>
       </c>
       <c r="F117" s="9" t="s">
-        <v>551</v>
+        <v>541</v>
       </c>
       <c r="G117" s="9" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="H117" s="9" t="s">
         <v>11</v>
@@ -7194,27 +7188,27 @@
         <v>11</v>
       </c>
     </row>
-    <row r="118" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="9" t="s">
-        <v>331</v>
+        <v>343</v>
       </c>
       <c r="B118" s="9" t="s">
-        <v>339</v>
-      </c>
-      <c r="C118" s="6" t="s">
-        <v>91</v>
+        <v>344</v>
+      </c>
+      <c r="C118" s="5" t="s">
+        <v>342</v>
       </c>
       <c r="D118" s="9" t="s">
         <v>14</v>
       </c>
       <c r="E118" s="9">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F118" s="9" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="G118" s="9" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="H118" s="9" t="s">
         <v>11</v>
@@ -7229,27 +7223,27 @@
         <v>11</v>
       </c>
     </row>
-    <row r="119" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="9" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="B119" s="9" t="s">
-        <v>344</v>
-      </c>
-      <c r="C119" s="5" t="s">
-        <v>342</v>
+        <v>360</v>
+      </c>
+      <c r="C119" s="6" t="s">
+        <v>348</v>
       </c>
       <c r="D119" s="9" t="s">
-        <v>14</v>
+        <v>311</v>
       </c>
       <c r="E119" s="9">
         <v>7</v>
       </c>
       <c r="F119" s="9" t="s">
-        <v>545</v>
+        <v>11</v>
       </c>
       <c r="G119" s="9" t="s">
-        <v>561</v>
+        <v>11</v>
       </c>
       <c r="H119" s="9" t="s">
         <v>11</v>
@@ -7264,24 +7258,24 @@
         <v>11</v>
       </c>
     </row>
-    <row r="120" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="9" t="s">
-        <v>345</v>
+        <v>366</v>
       </c>
       <c r="B120" s="9" t="s">
         <v>362</v>
       </c>
       <c r="C120" s="6" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="D120" s="9" t="s">
-        <v>311</v>
+        <v>333</v>
       </c>
       <c r="E120" s="9">
         <v>7</v>
       </c>
       <c r="F120" s="9" t="s">
-        <v>11</v>
+        <v>541</v>
       </c>
       <c r="G120" s="9" t="s">
         <v>11</v>
@@ -7296,18 +7290,18 @@
         <v>11</v>
       </c>
       <c r="K120" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="121" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="9" t="s">
-        <v>368</v>
+        <v>345</v>
       </c>
       <c r="B121" s="9" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="C121" s="6" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="D121" s="9" t="s">
         <v>333</v>
@@ -7316,7 +7310,7 @@
         <v>7</v>
       </c>
       <c r="F121" s="9" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="G121" s="9" t="s">
         <v>11</v>
@@ -7331,27 +7325,27 @@
         <v>11</v>
       </c>
       <c r="K121" s="9" t="s">
-        <v>578</v>
+        <v>347</v>
       </c>
     </row>
     <row r="122" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="9" t="s">
-        <v>345</v>
+        <v>367</v>
       </c>
       <c r="B122" s="9" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="C122" s="6" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="D122" s="9" t="s">
         <v>333</v>
       </c>
       <c r="E122" s="9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F122" s="9" t="s">
-        <v>545</v>
+        <v>11</v>
       </c>
       <c r="G122" s="9" t="s">
         <v>11</v>
@@ -7366,30 +7360,30 @@
         <v>11</v>
       </c>
       <c r="K122" s="9" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="123" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A123" s="9" t="s">
-        <v>369</v>
+        <v>29</v>
       </c>
       <c r="B123" s="9" t="s">
-        <v>360</v>
-      </c>
-      <c r="C123" s="6" t="s">
-        <v>350</v>
+        <v>570</v>
+      </c>
+      <c r="C123" s="9" t="s">
+        <v>571</v>
       </c>
       <c r="D123" s="9" t="s">
-        <v>333</v>
+        <v>14</v>
       </c>
       <c r="E123" s="9">
         <v>8</v>
       </c>
       <c r="F123" s="9" t="s">
-        <v>11</v>
+        <v>541</v>
       </c>
       <c r="G123" s="9" t="s">
-        <v>11</v>
+        <v>572</v>
       </c>
       <c r="H123" s="9" t="s">
         <v>11</v>
@@ -7401,30 +7395,30 @@
         <v>11</v>
       </c>
       <c r="K123" s="9" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="124" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A124" s="9" t="s">
-        <v>29</v>
+        <v>591</v>
       </c>
       <c r="B124" s="9" t="s">
-        <v>574</v>
-      </c>
-      <c r="C124" s="9" t="s">
-        <v>575</v>
+        <v>592</v>
+      </c>
+      <c r="C124" s="6" t="s">
+        <v>590</v>
       </c>
       <c r="D124" s="9" t="s">
-        <v>14</v>
+        <v>333</v>
       </c>
       <c r="E124" s="9">
         <v>8</v>
       </c>
       <c r="F124" s="9" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="G124" s="9" t="s">
-        <v>576</v>
+        <v>11</v>
       </c>
       <c r="H124" s="9" t="s">
         <v>11</v>
@@ -7436,27 +7430,27 @@
         <v>11</v>
       </c>
       <c r="K124" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="125" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="9" t="s">
-        <v>595</v>
+        <v>366</v>
       </c>
       <c r="B125" s="9" t="s">
+        <v>594</v>
+      </c>
+      <c r="C125" s="6" t="s">
         <v>596</v>
-      </c>
-      <c r="C125" s="6" t="s">
-        <v>594</v>
       </c>
       <c r="D125" s="9" t="s">
         <v>333</v>
       </c>
       <c r="E125" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F125" s="9" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="G125" s="9" t="s">
         <v>11</v>
@@ -7471,27 +7465,27 @@
         <v>11</v>
       </c>
       <c r="K125" s="9" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="126" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="9" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="B126" s="9" t="s">
-        <v>598</v>
+        <v>359</v>
       </c>
       <c r="C126" s="6" t="s">
-        <v>600</v>
+        <v>539</v>
       </c>
       <c r="D126" s="9" t="s">
         <v>333</v>
       </c>
       <c r="E126" s="9">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F126" s="9" t="s">
-        <v>545</v>
+        <v>11</v>
       </c>
       <c r="G126" s="9" t="s">
         <v>11</v>
@@ -7506,18 +7500,18 @@
         <v>11</v>
       </c>
       <c r="K126" s="9" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
     </row>
     <row r="127" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="9" t="s">
-        <v>365</v>
+        <v>356</v>
       </c>
       <c r="B127" s="9" t="s">
-        <v>361</v>
+        <v>600</v>
       </c>
       <c r="C127" s="6" t="s">
-        <v>543</v>
+        <v>598</v>
       </c>
       <c r="D127" s="9" t="s">
         <v>333</v>
@@ -7541,18 +7535,18 @@
         <v>11</v>
       </c>
       <c r="K127" s="9" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="128" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="9" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B128" s="9" t="s">
-        <v>604</v>
+        <v>637</v>
       </c>
       <c r="C128" s="6" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="D128" s="9" t="s">
         <v>333</v>
@@ -7576,8 +7570,11 @@
         <v>11</v>
       </c>
       <c r="K128" s="9" t="s">
-        <v>603</v>
-      </c>
+        <v>636</v>
+      </c>
+    </row>
+    <row r="136" spans="2:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="B136" s="9"/>
     </row>
     <row r="137" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B137" s="9"/>
@@ -7594,12 +7591,9 @@
     <row r="141" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B141" s="9"/>
     </row>
-    <row r="142" spans="2:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="B142" s="9"/>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K143">
-    <sortCondition ref="E2:E143"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K142">
+    <sortCondition ref="E2:E142"/>
   </sortState>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7653,13 +7647,13 @@
     </row>
     <row r="2" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
@@ -7668,7 +7662,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="G2" t="s">
         <v>11</v>
@@ -7688,13 +7682,13 @@
     </row>
     <row r="3" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
@@ -7703,7 +7697,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="25" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
@@ -7723,13 +7717,13 @@
     </row>
     <row r="4" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="25" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
@@ -7738,7 +7732,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="25" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="G4" t="s">
         <v>11</v>
@@ -7758,13 +7752,13 @@
     </row>
     <row r="5" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
@@ -7773,7 +7767,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="25" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="G5" t="s">
         <v>11</v>
@@ -7793,13 +7787,13 @@
     </row>
     <row r="6" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
@@ -7808,7 +7802,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="25" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="G6" t="s">
         <v>11</v>
@@ -7828,13 +7822,13 @@
     </row>
     <row r="7" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="25" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="D7" t="s">
         <v>11</v>
@@ -7843,7 +7837,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="25" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="G7" t="s">
         <v>11</v>
@@ -7863,13 +7857,13 @@
     </row>
     <row r="8" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="25" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="D8" t="s">
         <v>11</v>
@@ -7878,7 +7872,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="25" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="G8" t="s">
         <v>11</v>
@@ -7898,13 +7892,13 @@
     </row>
     <row r="9" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -7913,7 +7907,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="25" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="G9" t="s">
         <v>11</v>
@@ -7933,13 +7927,13 @@
     </row>
     <row r="10" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D10" t="s">
         <v>11</v>
@@ -7948,7 +7942,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="25" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="G10" t="s">
         <v>11</v>
@@ -7968,13 +7962,13 @@
     </row>
     <row r="11" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="25" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="D11" t="s">
         <v>11</v>
@@ -7983,7 +7977,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="25" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="G11" t="s">
         <v>11</v>
@@ -8003,13 +7997,13 @@
     </row>
     <row r="12" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="25" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="D12" t="s">
         <v>11</v>
@@ -8018,7 +8012,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="25" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="G12" t="s">
         <v>11</v>
@@ -8038,13 +8032,13 @@
     </row>
     <row r="13" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="25" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="D13" t="s">
         <v>11</v>
@@ -8053,7 +8047,7 @@
         <v>0</v>
       </c>
       <c r="F13" s="25" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="G13" t="s">
         <v>11</v>
@@ -8073,13 +8067,13 @@
     </row>
     <row r="14" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="25" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="D14" t="s">
         <v>11</v>
@@ -8088,7 +8082,7 @@
         <v>0</v>
       </c>
       <c r="F14" s="25" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="G14" t="s">
         <v>11</v>
@@ -8108,13 +8102,13 @@
     </row>
     <row r="15" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="25" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B15" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D15" t="s">
         <v>11</v>
@@ -8123,7 +8117,7 @@
         <v>0</v>
       </c>
       <c r="F15" s="25" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="G15" t="s">
         <v>11</v>
@@ -8143,13 +8137,13 @@
     </row>
     <row r="16" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="25" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B16" t="s">
         <v>11</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D16" t="s">
         <v>11</v>
@@ -8158,7 +8152,7 @@
         <v>0</v>
       </c>
       <c r="F16" s="25" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="G16" t="s">
         <v>11</v>
@@ -8178,13 +8172,13 @@
     </row>
     <row r="17" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="25" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B17" t="s">
         <v>11</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="D17" t="s">
         <v>11</v>
@@ -8193,7 +8187,7 @@
         <v>0</v>
       </c>
       <c r="F17" s="25" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="G17" t="s">
         <v>11</v>
@@ -8213,13 +8207,13 @@
     </row>
     <row r="18" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="25" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B18" t="s">
         <v>11</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D18" t="s">
         <v>11</v>
@@ -8228,7 +8222,7 @@
         <v>0</v>
       </c>
       <c r="F18" s="25" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="G18" t="s">
         <v>11</v>
@@ -8248,13 +8242,13 @@
     </row>
     <row r="19" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="25" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B19" t="s">
         <v>11</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D19" t="s">
         <v>11</v>
@@ -8263,7 +8257,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="25" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="G19" t="s">
         <v>11</v>
@@ -8283,13 +8277,13 @@
     </row>
     <row r="20" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="25" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B20" t="s">
         <v>11</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="D20" t="s">
         <v>11</v>
@@ -8298,7 +8292,7 @@
         <v>0</v>
       </c>
       <c r="F20" s="25" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="G20" t="s">
         <v>11</v>
@@ -8318,13 +8312,13 @@
     </row>
     <row r="21" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="25" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B21" t="s">
         <v>11</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="D21" t="s">
         <v>11</v>
@@ -8353,13 +8347,13 @@
     </row>
     <row r="22" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="25" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B22" t="s">
         <v>11</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D22" t="s">
         <v>11</v>
@@ -8431,8 +8425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A5C7946-155C-C64C-B6E6-9BB8EBA62A76}">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A1:XFD19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8477,13 +8471,13 @@
     </row>
     <row r="2" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
@@ -8492,7 +8486,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="G2" t="s">
         <v>11</v>
@@ -8512,13 +8506,13 @@
     </row>
     <row r="3" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
@@ -8527,7 +8521,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="25" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
@@ -8547,13 +8541,13 @@
     </row>
     <row r="4" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="25" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
@@ -8562,7 +8556,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="25" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="G4" t="s">
         <v>11</v>
@@ -8582,13 +8576,13 @@
     </row>
     <row r="5" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -8597,7 +8591,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="25" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="G5" t="s">
         <v>11</v>
@@ -8617,13 +8611,13 @@
     </row>
     <row r="6" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -8632,7 +8626,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="25" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="G6" t="s">
         <v>11</v>
@@ -8652,13 +8646,13 @@
     </row>
     <row r="7" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="25" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
@@ -8667,7 +8661,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="25" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="G7" t="s">
         <v>11</v>
@@ -8687,13 +8681,13 @@
     </row>
     <row r="8" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="25" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
@@ -8702,7 +8696,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="25" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="G8" t="s">
         <v>11</v>
@@ -8722,13 +8716,13 @@
     </row>
     <row r="9" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="D9" t="s">
         <v>12</v>
@@ -8737,7 +8731,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="25" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="G9" t="s">
         <v>11</v>
@@ -8757,13 +8751,13 @@
     </row>
     <row r="10" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -8772,7 +8766,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="25" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="G10" t="s">
         <v>11</v>
@@ -8792,13 +8786,13 @@
     </row>
     <row r="11" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="25" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
@@ -8807,7 +8801,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="25" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="G11" t="s">
         <v>11</v>
@@ -8827,13 +8821,13 @@
     </row>
     <row r="12" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="25" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="D12" t="s">
         <v>12</v>
@@ -8842,7 +8836,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="25" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="G12" t="s">
         <v>11</v>
@@ -8862,13 +8856,13 @@
     </row>
     <row r="13" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="25" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="D13" t="s">
         <v>12</v>
@@ -8877,7 +8871,7 @@
         <v>0</v>
       </c>
       <c r="F13" s="25" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="G13" t="s">
         <v>11</v>
@@ -8897,13 +8891,13 @@
     </row>
     <row r="14" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="25" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="D14" t="s">
         <v>12</v>
@@ -8912,7 +8906,7 @@
         <v>0</v>
       </c>
       <c r="F14" s="25" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="G14" t="s">
         <v>11</v>
@@ -8932,13 +8926,13 @@
     </row>
     <row r="15" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="25" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B15" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="D15" t="s">
         <v>12</v>
@@ -8967,13 +8961,13 @@
     </row>
     <row r="16" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="25" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B16" t="s">
         <v>11</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D16" t="s">
         <v>12</v>
@@ -9002,13 +8996,13 @@
     </row>
     <row r="17" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="25" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B17" t="s">
         <v>11</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="D17" t="s">
         <v>12</v>
@@ -9073,13 +9067,13 @@
     </row>
     <row r="19" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="25" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B19" t="s">
+        <v>506</v>
+      </c>
+      <c r="C19" s="25" t="s">
         <v>508</v>
-      </c>
-      <c r="C19" s="25" t="s">
-        <v>510</v>
       </c>
       <c r="D19" t="s">
         <v>311</v>
@@ -10180,7 +10174,7 @@
     </row>
     <row r="31" spans="1:11" s="19" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="22" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B31" s="19" t="s">
         <v>11</v>
@@ -10215,16 +10209,16 @@
     </row>
     <row r="32" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="B32" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D32" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="E32">
         <v>2</v>
@@ -10250,16 +10244,16 @@
     </row>
     <row r="33" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="B33" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D33" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="E33">
         <v>2</v>
@@ -10285,16 +10279,16 @@
     </row>
     <row r="34" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="B34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D34" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="E34">
         <v>2</v>
@@ -10320,16 +10314,16 @@
     </row>
     <row r="35" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="B35" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D35" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="E35">
         <v>2</v>
@@ -10358,7 +10352,7 @@
         <v>136</v>
       </c>
       <c r="B36" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>165</v>
@@ -10376,13 +10370,13 @@
         <v>11</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="I36" s="2">
         <v>0</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="K36" s="2" t="s">
         <v>11</v>
@@ -10393,7 +10387,7 @@
         <v>137</v>
       </c>
       <c r="B37" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>166</v>
@@ -10428,7 +10422,7 @@
         <v>138</v>
       </c>
       <c r="B38" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>167</v>
@@ -10463,7 +10457,7 @@
         <v>139</v>
       </c>
       <c r="B39" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>168</v>
@@ -10498,7 +10492,7 @@
         <v>123</v>
       </c>
       <c r="B40" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>152</v>
@@ -10510,7 +10504,7 @@
         <v>3</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>11</v>
@@ -10530,13 +10524,13 @@
     </row>
     <row r="41" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B41" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="D41" t="s">
         <v>269</v>
@@ -10548,13 +10542,13 @@
         <v>11</v>
       </c>
       <c r="H41" s="12" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="I41" s="12" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="J41" s="12" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="K41" s="2" t="s">
         <v>11</v>
@@ -10562,13 +10556,13 @@
     </row>
     <row r="42" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B42" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="D42" t="s">
         <v>269</v>
@@ -10580,13 +10574,13 @@
         <v>11</v>
       </c>
       <c r="H42" s="12" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="I42" s="12" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="J42" s="12" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="K42" s="2" t="s">
         <v>11</v>
@@ -10594,13 +10588,13 @@
     </row>
     <row r="43" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B43" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="D43" t="s">
         <v>269</v>
@@ -10612,13 +10606,13 @@
         <v>11</v>
       </c>
       <c r="H43" s="12" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="I43" s="12" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="J43" s="12" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="K43" s="2" t="s">
         <v>11</v>
@@ -10626,13 +10620,13 @@
     </row>
     <row r="44" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B44" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="D44" t="s">
         <v>269</v>
@@ -10644,13 +10638,13 @@
         <v>11</v>
       </c>
       <c r="H44" s="12" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="I44" s="12" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="J44" s="12" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="K44" s="2" t="s">
         <v>11</v>
@@ -10658,16 +10652,16 @@
     </row>
     <row r="45" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B45" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D45" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="E45">
         <v>5</v>
@@ -11701,7 +11695,7 @@
         <v>185</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="C29" s="12" t="s">
         <v>209</v>
@@ -11911,10 +11905,10 @@
         <v>191</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>14</v>
@@ -11923,7 +11917,7 @@
         <v>2</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>312</v>
@@ -12054,7 +12048,7 @@
         <v>300</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>14</v>
@@ -12063,7 +12057,7 @@
         <v>2</v>
       </c>
       <c r="F39" s="12" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>312</v>
@@ -12156,7 +12150,7 @@
         <v>198</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="C42" s="12" t="s">
         <v>222</v>
@@ -12366,7 +12360,7 @@
         <v>204</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="C48" s="12" t="s">
         <v>228</v>
@@ -12471,7 +12465,7 @@
         <v>207</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="C51" s="12" t="s">
         <v>231</v>
@@ -12503,16 +12497,16 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>314</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="E52" s="5">
         <v>3</v>
@@ -12538,13 +12532,13 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>313</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="D53" s="5" t="s">
         <v>269</v>
@@ -12559,13 +12553,13 @@
         <v>11</v>
       </c>
       <c r="H53" s="12" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="I53" s="12" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="J53" s="12" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="K53" s="12" t="s">
         <v>11</v>
@@ -12573,16 +12567,16 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>316</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="E54" s="5">
         <v>3</v>
@@ -12608,13 +12602,13 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="5" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B55" s="5" t="s">
         <v>315</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="D55" s="5" t="s">
         <v>269</v>
@@ -12629,13 +12623,13 @@
         <v>11</v>
       </c>
       <c r="H55" s="12" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="I55" s="12" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="J55" s="12" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="K55" s="12" t="s">
         <v>11</v>
@@ -12646,13 +12640,13 @@
         <v>317</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>319</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="E56" s="5">
         <v>3</v>
@@ -12678,13 +12672,13 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="5" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>318</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="D57" s="5" t="s">
         <v>269</v>
@@ -12699,13 +12693,13 @@
         <v>11</v>
       </c>
       <c r="H57" s="12" t="s">
+        <v>517</v>
+      </c>
+      <c r="I57" s="12" t="s">
         <v>521</v>
       </c>
-      <c r="I57" s="12" t="s">
-        <v>525</v>
-      </c>
       <c r="J57" s="12" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="K57" s="12" t="s">
         <v>11</v>
@@ -12716,13 +12710,13 @@
         <v>320</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>322</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="E58" s="5">
         <v>3</v>
@@ -12748,13 +12742,13 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" s="5" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="B59" s="5" t="s">
         <v>321</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="D59" s="5" t="s">
         <v>269</v>
@@ -12769,13 +12763,13 @@
         <v>11</v>
       </c>
       <c r="H59" s="12" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="I59" s="12" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="J59" s="12" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="K59" s="12" t="s">
         <v>11</v>
@@ -12786,13 +12780,13 @@
         <v>323</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C60" s="5" t="s">
         <v>324</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="E60" s="5">
         <v>3</v>
@@ -12818,13 +12812,13 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" s="5" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="B61" s="5" t="s">
         <v>327</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="D61" s="5" t="s">
         <v>269</v>
@@ -12839,13 +12833,13 @@
         <v>11</v>
       </c>
       <c r="H61" s="12" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="I61" s="12" t="s">
+        <v>521</v>
+      </c>
+      <c r="J61" s="12" t="s">
         <v>525</v>
-      </c>
-      <c r="J61" s="12" t="s">
-        <v>529</v>
       </c>
       <c r="K61" s="12" t="s">
         <v>11</v>
@@ -12892,10 +12886,10 @@
         <v>325</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="D63" s="5" t="s">
         <v>333</v>
@@ -12904,7 +12898,7 @@
         <v>6</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="G63" s="5" t="s">
         <v>11</v>
@@ -12919,7 +12913,7 @@
         <v>11</v>
       </c>
       <c r="K63" s="12" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update lock file - change results file. increase replicability
</commit_message>
<xml_diff>
--- a/scoring/EDGI_exercise_scoresheet.xlsx
+++ b/scoring/EDGI_exercise_scoresheet.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kschaumb/Dropbox/Wisconsin/Papers (External)/EDGI_Exercise/scoring/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kschaumberg/Dropbox/Wisconsin/Papers (External)/EDGI_Exercise/scoring/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F61B2125-CF7B-8E4E-853A-8CDEB740F5CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D89A0ED7-ED6C-7340-A110-E89D86DEEBCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="43180" windowHeight="19900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4960" yWindow="760" windowWidth="24980" windowHeight="13860" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ED100k" sheetId="1" r:id="rId1"/>
-    <sheet name="OCIR" sheetId="4" r:id="rId2"/>
-    <sheet name="Perfectionism" sheetId="5" r:id="rId3"/>
+    <sheet name="OCI12" sheetId="4" r:id="rId2"/>
+    <sheet name="FrostMPS" sheetId="5" r:id="rId3"/>
     <sheet name="EDEQ" sheetId="3" r:id="rId4"/>
     <sheet name="CET" sheetId="2" r:id="rId5"/>
   </sheets>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2756" uniqueCount="639">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2891" uniqueCount="686">
   <si>
     <t>raw_vars</t>
   </si>
@@ -1316,15 +1316,6 @@
     <t>oci18</t>
   </si>
   <si>
-    <t>oci_complete</t>
-  </si>
-  <si>
-    <t>ocimiss_ct</t>
-  </si>
-  <si>
-    <t>oci_total</t>
-  </si>
-  <si>
     <t>I have saved up so many things that they get in the way.</t>
   </si>
   <si>
@@ -1382,12 +1373,6 @@
     <t>ocir status</t>
   </si>
   <si>
-    <t>Missing Count</t>
-  </si>
-  <si>
-    <t>Total Score</t>
-  </si>
-  <si>
     <t>mps4_ps</t>
   </si>
   <si>
@@ -1424,18 +1409,6 @@
     <t>mps33_da</t>
   </si>
   <si>
-    <t>perfectionism_complete</t>
-  </si>
-  <si>
-    <t>da_total</t>
-  </si>
-  <si>
-    <t>cm_total</t>
-  </si>
-  <si>
-    <t>ps_total</t>
-  </si>
-  <si>
     <t>If I do not set the highest standards for myself, I am likely to end up a second rate person</t>
   </si>
   <si>
@@ -1472,9 +1445,6 @@
     <t>It takes me a long time to dosomething "right.</t>
   </si>
   <si>
-    <t>Perfectionism Status</t>
-  </si>
-  <si>
     <t>Doubts About Actions Subscale Total</t>
   </si>
   <si>
@@ -1556,15 +1526,6 @@
     <t>Weight concerns subscale of EDEQ - 25% or less missing</t>
   </si>
   <si>
-    <t>mps_total</t>
-  </si>
-  <si>
-    <t>da_total, cm_total, ps_total</t>
-  </si>
-  <si>
-    <t>Total score combining da, cm, and ps subscales</t>
-  </si>
-  <si>
     <t>be_icb___5</t>
   </si>
   <si>
@@ -1953,13 +1914,193 @@
   </si>
   <si>
     <t>reports any compulsive OR any compensatory exercise</t>
+  </si>
+  <si>
+    <t>oci12_wash</t>
+  </si>
+  <si>
+    <t>OCI-12 washing subscale</t>
+  </si>
+  <si>
+    <t>oci2, oci8, oci14</t>
+  </si>
+  <si>
+    <t>oci12_check</t>
+  </si>
+  <si>
+    <t>OCI-12 checking subscale</t>
+  </si>
+  <si>
+    <t>oci6, oci12, oci18</t>
+  </si>
+  <si>
+    <t>oci12_obsess</t>
+  </si>
+  <si>
+    <t>oci3, oci9, oci15</t>
+  </si>
+  <si>
+    <t>oci12_order</t>
+  </si>
+  <si>
+    <t>OCI-12 obsessions</t>
+  </si>
+  <si>
+    <t>OCI-12 order subscale sum</t>
+  </si>
+  <si>
+    <t>oci12_wash, oci12_check, oci12_obsess, oci12_order</t>
+  </si>
+  <si>
+    <t>oci12_total</t>
+  </si>
+  <si>
+    <t>OCI-12 total score</t>
+  </si>
+  <si>
+    <t>mps_ps</t>
+  </si>
+  <si>
+    <t>mps_cm</t>
+  </si>
+  <si>
+    <t>mps4_ps, mps6_ps, mps16_ps, mps19_ps</t>
+  </si>
+  <si>
+    <t>mps_da</t>
+  </si>
+  <si>
+    <t>mps9_cm, mps14_cm, mps18_cm, mps21_cm</t>
+  </si>
+  <si>
+    <t>mps17_da, mps28_da,  mps32_da, mps33_da</t>
+  </si>
+  <si>
+    <t>oci12_wash_raw</t>
+  </si>
+  <si>
+    <t>mps_ps_raw</t>
+  </si>
+  <si>
+    <t>mps_cm_raw</t>
+  </si>
+  <si>
+    <t>mps_da_raw</t>
+  </si>
+  <si>
+    <t>Personal Standards Subscale Total - 25% or less missing</t>
+  </si>
+  <si>
+    <t>Concern over Mistakes Subscale Total - 25% or less missing</t>
+  </si>
+  <si>
+    <t>Doubts About Actions Subscale Total - 25% or less missing</t>
+  </si>
+  <si>
+    <t>mps_ps_raw_NA_percent &gt; 25</t>
+  </si>
+  <si>
+    <t>mps_cm_raw_NA_percent &gt; 25</t>
+  </si>
+  <si>
+    <t>mps_da_raw_NA_percent &gt; 25</t>
+  </si>
+  <si>
+    <t>oci12_cutoff</t>
+  </si>
+  <si>
+    <t>oci12_benchmarks</t>
+  </si>
+  <si>
+    <t>OCI-12 total cutoff met</t>
+  </si>
+  <si>
+    <t>OCI-12 benchmark scores</t>
+  </si>
+  <si>
+    <t>mild/none = 0, moderate = 1, severe = 2</t>
+  </si>
+  <si>
+    <t>oci12_check_raw</t>
+  </si>
+  <si>
+    <t>oci12_obsess_raw</t>
+  </si>
+  <si>
+    <t>oci12_order_raw</t>
+  </si>
+  <si>
+    <t>oci12_total_raw</t>
+  </si>
+  <si>
+    <t>oci12_order_raw_NA_percent &gt; 34</t>
+  </si>
+  <si>
+    <t>oci12_check_raw_NA_percent &gt; 34</t>
+  </si>
+  <si>
+    <t>oci12_total_raw_NA_percent &gt; 25</t>
+  </si>
+  <si>
+    <t>oci12_total &lt; 11 ~ 0, oci12_total &gt;= 11 ~1</t>
+  </si>
+  <si>
+    <t>as.numeric (oci12_total_raw_weighted_sum)</t>
+  </si>
+  <si>
+    <t>as.numeric (oci12_order_raw_weighted_sum)</t>
+  </si>
+  <si>
+    <t>as.numeric (oci12_obsess_raw_weighted_sum)</t>
+  </si>
+  <si>
+    <t>as.numeric (oci12_check_raw_weighted_sum)</t>
+  </si>
+  <si>
+    <t>as.numeric (mps_ps_raw_weighted_sum)</t>
+  </si>
+  <si>
+    <t>as.numeric (mps_cm_raw_weighted_sum)</t>
+  </si>
+  <si>
+    <t>as.numeric (mps_da_raw_weighted_sum)</t>
+  </si>
+  <si>
+    <t>ED100k_ex_compulsive_current2</t>
+  </si>
+  <si>
+    <t>No Current compulsive exercise = 0, current compulsive exercise = 1</t>
+  </si>
+  <si>
+    <t>ED100k_ex_compulsive == 0 ~ 0, ED100k_ex_compulsive == 1 &amp; ED100k_ex_compulsive_current == 0 ~ 1, ED100k_ex_compulsive_current == 1 ~ 2</t>
+  </si>
+  <si>
+    <t>ocir_complete</t>
+  </si>
+  <si>
+    <t>oci5, oci11, oci17</t>
+  </si>
+  <si>
+    <t>oci12_wash_raw_NA_percent &gt; 34</t>
+  </si>
+  <si>
+    <t>as.numeric (oci12_wash_raw_weighted_sum)</t>
+  </si>
+  <si>
+    <t>oci12_obsess_raw_NA_percent &gt; 34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oci12_total &lt; 13 ~ 0, oci12_total &gt; 12 &amp; oci12_total &lt;= 21 ~ 2, oci12_total &gt; 21 ~3 </t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2183,6 +2324,13 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -3076,10 +3224,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L141"/>
+  <dimension ref="A1:L142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="119" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C128" sqref="C128"/>
+    <sheetView zoomScale="119" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="A119" sqref="A119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3203,7 +3351,7 @@
     </row>
     <row r="4" spans="1:11" s="15" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
-        <v>510</v>
+        <v>497</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>11</v>
@@ -3413,13 +3561,13 @@
     </row>
     <row r="10" spans="1:11" s="28" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="26" t="s">
-        <v>607</v>
+        <v>594</v>
       </c>
       <c r="B10" s="26" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>608</v>
+        <v>595</v>
       </c>
       <c r="D10" s="26" t="s">
         <v>11</v>
@@ -3428,7 +3576,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="26" t="s">
-        <v>609</v>
+        <v>596</v>
       </c>
       <c r="G10" s="13" t="s">
         <v>11</v>
@@ -3448,13 +3596,13 @@
     </row>
     <row r="11" spans="1:11" s="28" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="26" t="s">
-        <v>610</v>
+        <v>597</v>
       </c>
       <c r="B11" s="26" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>611</v>
+        <v>598</v>
       </c>
       <c r="D11" s="26" t="s">
         <v>11</v>
@@ -3463,7 +3611,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="26" t="s">
-        <v>609</v>
+        <v>596</v>
       </c>
       <c r="G11" s="13" t="s">
         <v>11</v>
@@ -3483,13 +3631,13 @@
     </row>
     <row r="12" spans="1:11" s="28" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="26" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="B12" s="26" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>605</v>
+        <v>592</v>
       </c>
       <c r="D12" s="26" t="s">
         <v>12</v>
@@ -3498,7 +3646,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="26" t="s">
-        <v>606</v>
+        <v>593</v>
       </c>
       <c r="G12" s="13" t="s">
         <v>11</v>
@@ -3518,7 +3666,7 @@
     </row>
     <row r="13" spans="1:11" s="15" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
-        <v>509</v>
+        <v>496</v>
       </c>
       <c r="B13" s="13" t="s">
         <v>11</v>
@@ -5584,7 +5732,7 @@
     </row>
     <row r="72" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="9" t="s">
-        <v>509</v>
+        <v>496</v>
       </c>
       <c r="B72" s="9" t="s">
         <v>357</v>
@@ -5599,10 +5747,10 @@
         <v>2</v>
       </c>
       <c r="F72" s="9" t="s">
+        <v>528</v>
+      </c>
+      <c r="G72" t="s">
         <v>541</v>
-      </c>
-      <c r="G72" t="s">
-        <v>554</v>
       </c>
       <c r="H72" s="9" t="s">
         <v>11</v>
@@ -5634,10 +5782,10 @@
         <v>2</v>
       </c>
       <c r="F73" s="9" t="s">
-        <v>540</v>
+        <v>527</v>
       </c>
       <c r="G73" s="9" t="s">
-        <v>559</v>
+        <v>546</v>
       </c>
       <c r="H73" s="9" t="s">
         <v>11</v>
@@ -5669,10 +5817,10 @@
         <v>2</v>
       </c>
       <c r="F74" s="9" t="s">
-        <v>540</v>
+        <v>527</v>
       </c>
       <c r="G74" s="9" t="s">
-        <v>559</v>
+        <v>546</v>
       </c>
       <c r="H74" s="9" t="s">
         <v>11</v>
@@ -5704,10 +5852,10 @@
         <v>2</v>
       </c>
       <c r="F75" s="9" t="s">
-        <v>540</v>
+        <v>527</v>
       </c>
       <c r="G75" s="9" t="s">
-        <v>559</v>
+        <v>546</v>
       </c>
       <c r="H75" s="9" t="s">
         <v>11</v>
@@ -5739,10 +5887,10 @@
         <v>2</v>
       </c>
       <c r="F76" s="9" t="s">
-        <v>540</v>
+        <v>527</v>
       </c>
       <c r="G76" s="9" t="s">
-        <v>559</v>
+        <v>546</v>
       </c>
       <c r="H76" s="9" t="s">
         <v>11</v>
@@ -5774,10 +5922,10 @@
         <v>2</v>
       </c>
       <c r="F77" s="9" t="s">
-        <v>540</v>
+        <v>527</v>
       </c>
       <c r="G77" s="9" t="s">
-        <v>559</v>
+        <v>546</v>
       </c>
       <c r="H77" s="9" t="s">
         <v>11</v>
@@ -5809,10 +5957,10 @@
         <v>2</v>
       </c>
       <c r="F78" s="9" t="s">
-        <v>562</v>
+        <v>549</v>
       </c>
       <c r="G78" s="9" t="s">
-        <v>560</v>
+        <v>547</v>
       </c>
       <c r="H78" s="9" t="s">
         <v>11</v>
@@ -5844,10 +5992,10 @@
         <v>2</v>
       </c>
       <c r="F79" s="9" t="s">
-        <v>563</v>
+        <v>550</v>
       </c>
       <c r="G79" s="9" t="s">
-        <v>561</v>
+        <v>548</v>
       </c>
       <c r="H79" s="9" t="s">
         <v>11</v>
@@ -5879,10 +6027,10 @@
         <v>2</v>
       </c>
       <c r="F80" s="9" t="s">
-        <v>540</v>
+        <v>527</v>
       </c>
       <c r="G80" s="9" t="s">
-        <v>559</v>
+        <v>546</v>
       </c>
       <c r="H80" s="9" t="s">
         <v>11</v>
@@ -5902,10 +6050,10 @@
         <v>40</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>622</v>
+        <v>609</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>623</v>
+        <v>610</v>
       </c>
       <c r="D81" s="9" t="s">
         <v>14</v>
@@ -5914,10 +6062,10 @@
         <v>2</v>
       </c>
       <c r="F81" s="30" t="s">
-        <v>624</v>
+        <v>611</v>
       </c>
       <c r="G81" s="9" t="s">
-        <v>625</v>
+        <v>612</v>
       </c>
       <c r="H81" s="9" t="s">
         <v>11</v>
@@ -5934,13 +6082,13 @@
     </row>
     <row r="82" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="9" t="s">
-        <v>626</v>
+        <v>613</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>619</v>
+        <v>606</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>620</v>
+        <v>607</v>
       </c>
       <c r="D82" s="9" t="s">
         <v>333</v>
@@ -5949,7 +6097,7 @@
         <v>3</v>
       </c>
       <c r="F82" s="9" t="s">
-        <v>541</v>
+        <v>528</v>
       </c>
       <c r="G82" s="9" t="s">
         <v>11</v>
@@ -5964,7 +6112,7 @@
         <v>11</v>
       </c>
       <c r="K82" s="9" t="s">
-        <v>627</v>
+        <v>614</v>
       </c>
     </row>
     <row r="83" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -6130,7 +6278,7 @@
         <v>11</v>
       </c>
       <c r="H87" s="9" t="s">
-        <v>511</v>
+        <v>498</v>
       </c>
       <c r="I87" s="9">
         <v>0</v>
@@ -6171,7 +6319,7 @@
         <v>0</v>
       </c>
       <c r="J88" s="9" t="s">
-        <v>630</v>
+        <v>617</v>
       </c>
       <c r="K88" s="9" t="s">
         <v>11</v>
@@ -6182,7 +6330,7 @@
         <v>36</v>
       </c>
       <c r="B89" s="9" t="s">
-        <v>602</v>
+        <v>589</v>
       </c>
       <c r="C89" s="6" t="s">
         <v>236</v>
@@ -6194,7 +6342,7 @@
         <v>3</v>
       </c>
       <c r="F89" s="9" t="s">
-        <v>603</v>
+        <v>590</v>
       </c>
       <c r="G89" s="9" t="s">
         <v>11</v>
@@ -6206,7 +6354,7 @@
         <v>0</v>
       </c>
       <c r="J89" s="9" t="s">
-        <v>601</v>
+        <v>588</v>
       </c>
       <c r="K89" s="9" t="s">
         <v>11</v>
@@ -6217,10 +6365,10 @@
         <v>245</v>
       </c>
       <c r="B90" s="9" t="s">
-        <v>612</v>
+        <v>599</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>613</v>
+        <v>600</v>
       </c>
       <c r="D90" s="9" t="s">
         <v>269</v>
@@ -6229,7 +6377,7 @@
         <v>3</v>
       </c>
       <c r="F90" s="9" t="s">
-        <v>603</v>
+        <v>590</v>
       </c>
       <c r="G90" s="9" t="s">
         <v>11</v>
@@ -6241,127 +6389,127 @@
         <v>0</v>
       </c>
       <c r="J90" s="9" t="s">
-        <v>629</v>
+        <v>616</v>
       </c>
       <c r="K90" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="91" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="29" t="s">
+      <c r="A91" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="B91" s="9" t="s">
+        <v>603</v>
+      </c>
+      <c r="C91" s="6" t="s">
         <v>604</v>
       </c>
-      <c r="B91" s="29" t="s">
-        <v>614</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>615</v>
-      </c>
-      <c r="D91" s="29" t="s">
+      <c r="D91" s="9" t="s">
         <v>269</v>
       </c>
-      <c r="E91" s="29">
-        <v>4</v>
-      </c>
-      <c r="F91" s="29" t="s">
-        <v>603</v>
-      </c>
-      <c r="G91" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="H91" s="29" t="s">
-        <v>621</v>
-      </c>
-      <c r="I91" s="29">
-        <v>0</v>
-      </c>
-      <c r="J91" s="29" t="s">
-        <v>628</v>
-      </c>
-      <c r="K91" s="29" t="s">
+      <c r="E91" s="9">
+        <v>3</v>
+      </c>
+      <c r="F91" s="9" t="s">
+        <v>590</v>
+      </c>
+      <c r="G91" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H91" s="9" t="s">
+        <v>605</v>
+      </c>
+      <c r="I91" s="9">
+        <v>0</v>
+      </c>
+      <c r="J91" s="9" t="s">
+        <v>618</v>
+      </c>
+      <c r="K91" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="92" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="29" t="s">
-        <v>614</v>
-      </c>
-      <c r="B92" s="29" t="s">
-        <v>632</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>633</v>
-      </c>
-      <c r="D92" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="E92" s="29">
-        <v>5</v>
-      </c>
-      <c r="F92" s="29" t="s">
-        <v>634</v>
-      </c>
-      <c r="G92" s="29" t="s">
-        <v>635</v>
-      </c>
-      <c r="H92" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="I92" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="J92" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="K92" s="29" t="s">
-        <v>11</v>
+      <c r="A92" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="B92" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="C92" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="D92" s="9" t="s">
+        <v>333</v>
+      </c>
+      <c r="E92" s="9">
+        <v>3</v>
+      </c>
+      <c r="F92" s="9" t="s">
+        <v>529</v>
+      </c>
+      <c r="G92" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H92" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I92" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J92" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K92" s="9" t="s">
+        <v>556</v>
       </c>
       <c r="L92" s="29"/>
     </row>
     <row r="93" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="9" t="s">
-        <v>244</v>
+      <c r="A93" s="7" t="s">
+        <v>268</v>
       </c>
       <c r="B93" s="9" t="s">
-        <v>616</v>
+        <v>273</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>617</v>
+        <v>406</v>
       </c>
       <c r="D93" s="9" t="s">
-        <v>269</v>
+        <v>333</v>
       </c>
       <c r="E93" s="9">
         <v>3</v>
       </c>
       <c r="F93" s="9" t="s">
-        <v>603</v>
+        <v>555</v>
       </c>
       <c r="G93" s="9" t="s">
         <v>11</v>
       </c>
       <c r="H93" s="9" t="s">
-        <v>618</v>
-      </c>
-      <c r="I93" s="9">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="I93" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="J93" s="9" t="s">
-        <v>631</v>
+        <v>11</v>
       </c>
       <c r="K93" s="9" t="s">
-        <v>11</v>
+        <v>554</v>
       </c>
     </row>
     <row r="94" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="7" t="s">
-        <v>268</v>
+        <v>17</v>
       </c>
       <c r="B94" s="9" t="s">
-        <v>272</v>
+        <v>572</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>407</v>
+        <v>573</v>
       </c>
       <c r="D94" s="9" t="s">
         <v>333</v>
@@ -6370,7 +6518,7 @@
         <v>3</v>
       </c>
       <c r="F94" s="9" t="s">
-        <v>542</v>
+        <v>574</v>
       </c>
       <c r="G94" s="9" t="s">
         <v>11</v>
@@ -6385,144 +6533,144 @@
         <v>11</v>
       </c>
       <c r="K94" s="9" t="s">
-        <v>569</v>
+        <v>575</v>
       </c>
     </row>
     <row r="95" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="7" t="s">
-        <v>268</v>
+      <c r="A95" s="9" t="s">
+        <v>53</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>273</v>
+        <v>382</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>406</v>
+        <v>109</v>
       </c>
       <c r="D95" s="9" t="s">
-        <v>333</v>
+        <v>269</v>
       </c>
       <c r="E95" s="9">
         <v>3</v>
       </c>
       <c r="F95" s="9" t="s">
-        <v>568</v>
+        <v>11</v>
       </c>
       <c r="G95" s="9" t="s">
         <v>11</v>
       </c>
       <c r="H95" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="I95" s="9" t="s">
-        <v>11</v>
+        <v>499</v>
+      </c>
+      <c r="I95" s="9">
+        <v>0</v>
       </c>
       <c r="J95" s="9" t="s">
-        <v>11</v>
+        <v>385</v>
       </c>
       <c r="K95" s="9" t="s">
-        <v>567</v>
+        <v>11</v>
       </c>
     </row>
     <row r="96" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="7" t="s">
-        <v>17</v>
+      <c r="A96" s="9" t="s">
+        <v>56</v>
       </c>
       <c r="B96" s="9" t="s">
-        <v>585</v>
+        <v>370</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>586</v>
+        <v>114</v>
       </c>
       <c r="D96" s="9" t="s">
-        <v>333</v>
+        <v>269</v>
       </c>
       <c r="E96" s="9">
         <v>3</v>
       </c>
       <c r="F96" s="9" t="s">
-        <v>587</v>
+        <v>11</v>
       </c>
       <c r="G96" s="9" t="s">
         <v>11</v>
       </c>
       <c r="H96" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="I96" s="9" t="s">
-        <v>11</v>
+        <v>372</v>
+      </c>
+      <c r="I96" s="9">
+        <v>0</v>
       </c>
       <c r="J96" s="9" t="s">
-        <v>11</v>
+        <v>378</v>
       </c>
       <c r="K96" s="9" t="s">
-        <v>588</v>
+        <v>11</v>
       </c>
     </row>
     <row r="97" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B97" s="9" t="s">
-        <v>382</v>
-      </c>
-      <c r="C97" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="D97" s="9" t="s">
+      <c r="A97" s="29" t="s">
+        <v>591</v>
+      </c>
+      <c r="B97" s="29" t="s">
+        <v>601</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>602</v>
+      </c>
+      <c r="D97" s="29" t="s">
         <v>269</v>
       </c>
-      <c r="E97" s="9">
-        <v>3</v>
-      </c>
-      <c r="F97" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G97" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="H97" s="9" t="s">
-        <v>512</v>
-      </c>
-      <c r="I97" s="9">
-        <v>0</v>
-      </c>
-      <c r="J97" s="9" t="s">
-        <v>385</v>
-      </c>
-      <c r="K97" s="9" t="s">
+      <c r="E97" s="29">
+        <v>4</v>
+      </c>
+      <c r="F97" s="29" t="s">
+        <v>590</v>
+      </c>
+      <c r="G97" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="H97" s="29" t="s">
+        <v>608</v>
+      </c>
+      <c r="I97" s="29">
+        <v>0</v>
+      </c>
+      <c r="J97" s="29" t="s">
+        <v>615</v>
+      </c>
+      <c r="K97" s="29" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="98" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="9" t="s">
-        <v>56</v>
+        <v>374</v>
       </c>
       <c r="B98" s="9" t="s">
-        <v>370</v>
+        <v>375</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D98" s="9" t="s">
-        <v>269</v>
+        <v>14</v>
       </c>
       <c r="E98" s="9">
-        <v>3</v>
-      </c>
-      <c r="F98" s="9" t="s">
-        <v>11</v>
+        <v>4</v>
+      </c>
+      <c r="F98" s="7" t="s">
+        <v>530</v>
       </c>
       <c r="G98" s="9" t="s">
-        <v>11</v>
+        <v>542</v>
       </c>
       <c r="H98" s="9" t="s">
-        <v>372</v>
-      </c>
-      <c r="I98" s="9">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="I98" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="J98" s="9" t="s">
-        <v>378</v>
+        <v>11</v>
       </c>
       <c r="K98" s="9" t="s">
         <v>11</v>
@@ -6530,13 +6678,13 @@
     </row>
     <row r="99" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="9" t="s">
-        <v>374</v>
+        <v>386</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>375</v>
+        <v>388</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="D99" s="9" t="s">
         <v>14</v>
@@ -6545,10 +6693,10 @@
         <v>4</v>
       </c>
       <c r="F99" s="7" t="s">
+        <v>531</v>
+      </c>
+      <c r="G99" s="9" t="s">
         <v>543</v>
-      </c>
-      <c r="G99" s="9" t="s">
-        <v>555</v>
       </c>
       <c r="H99" s="9" t="s">
         <v>11</v>
@@ -6565,13 +6713,13 @@
     </row>
     <row r="100" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="9" t="s">
-        <v>386</v>
+        <v>328</v>
       </c>
       <c r="B100" s="9" t="s">
-        <v>388</v>
+        <v>336</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="D100" s="9" t="s">
         <v>14</v>
@@ -6579,11 +6727,11 @@
       <c r="E100" s="9">
         <v>4</v>
       </c>
-      <c r="F100" s="7" t="s">
+      <c r="F100" s="9" t="s">
+        <v>528</v>
+      </c>
+      <c r="G100" s="9" t="s">
         <v>544</v>
-      </c>
-      <c r="G100" s="9" t="s">
-        <v>556</v>
       </c>
       <c r="H100" s="9" t="s">
         <v>11</v>
@@ -6600,13 +6748,13 @@
     </row>
     <row r="101" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="9" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B101" s="9" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D101" s="9" t="s">
         <v>14</v>
@@ -6615,10 +6763,10 @@
         <v>4</v>
       </c>
       <c r="F101" s="9" t="s">
-        <v>541</v>
+        <v>576</v>
       </c>
       <c r="G101" s="9" t="s">
-        <v>557</v>
+        <v>544</v>
       </c>
       <c r="H101" s="9" t="s">
         <v>11</v>
@@ -6635,13 +6783,13 @@
     </row>
     <row r="102" spans="1:11" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="9" t="s">
-        <v>329</v>
+        <v>379</v>
       </c>
       <c r="B102" s="9" t="s">
-        <v>337</v>
+        <v>381</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>89</v>
+        <v>120</v>
       </c>
       <c r="D102" s="9" t="s">
         <v>14</v>
@@ -6649,11 +6797,11 @@
       <c r="E102" s="9">
         <v>4</v>
       </c>
-      <c r="F102" s="9" t="s">
-        <v>589</v>
+      <c r="F102" s="7" t="s">
+        <v>535</v>
       </c>
       <c r="G102" s="9" t="s">
-        <v>557</v>
+        <v>542</v>
       </c>
       <c r="H102" s="9" t="s">
         <v>11</v>
@@ -6670,13 +6818,13 @@
     </row>
     <row r="103" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="9" t="s">
-        <v>379</v>
+        <v>368</v>
       </c>
       <c r="B103" s="9" t="s">
-        <v>381</v>
+        <v>369</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="D103" s="9" t="s">
         <v>14</v>
@@ -6685,10 +6833,10 @@
         <v>4</v>
       </c>
       <c r="F103" s="7" t="s">
-        <v>548</v>
+        <v>536</v>
       </c>
       <c r="G103" s="9" t="s">
-        <v>555</v>
+        <v>543</v>
       </c>
       <c r="H103" s="9" t="s">
         <v>11</v>
@@ -6703,15 +6851,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="104" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A104" s="9" t="s">
-        <v>368</v>
+        <v>382</v>
       </c>
       <c r="B104" s="9" t="s">
-        <v>369</v>
+        <v>383</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D104" s="9" t="s">
         <v>14</v>
@@ -6720,10 +6868,10 @@
         <v>4</v>
       </c>
       <c r="F104" s="7" t="s">
-        <v>549</v>
+        <v>537</v>
       </c>
       <c r="G104" s="9" t="s">
-        <v>556</v>
+        <v>542</v>
       </c>
       <c r="H104" s="9" t="s">
         <v>11</v>
@@ -6740,13 +6888,13 @@
     </row>
     <row r="105" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" s="9" t="s">
-        <v>382</v>
+        <v>370</v>
       </c>
       <c r="B105" s="9" t="s">
-        <v>383</v>
+        <v>371</v>
       </c>
       <c r="C105" s="6" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="D105" s="9" t="s">
         <v>14</v>
@@ -6755,10 +6903,10 @@
         <v>4</v>
       </c>
       <c r="F105" s="7" t="s">
-        <v>550</v>
+        <v>538</v>
       </c>
       <c r="G105" s="9" t="s">
-        <v>555</v>
+        <v>543</v>
       </c>
       <c r="H105" s="9" t="s">
         <v>11</v>
@@ -6774,37 +6922,37 @@
       </c>
     </row>
     <row r="106" spans="1:11" ht="17" x14ac:dyDescent="0.2">
-      <c r="A106" s="9" t="s">
-        <v>370</v>
-      </c>
-      <c r="B106" s="9" t="s">
-        <v>371</v>
-      </c>
-      <c r="C106" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D106" s="9" t="s">
+      <c r="A106" s="29" t="s">
+        <v>601</v>
+      </c>
+      <c r="B106" s="29" t="s">
+        <v>619</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>620</v>
+      </c>
+      <c r="D106" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="E106" s="9">
-        <v>4</v>
-      </c>
-      <c r="F106" s="7" t="s">
-        <v>551</v>
-      </c>
-      <c r="G106" s="9" t="s">
-        <v>556</v>
-      </c>
-      <c r="H106" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="I106" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="J106" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="K106" s="9" t="s">
+      <c r="E106" s="29">
+        <v>5</v>
+      </c>
+      <c r="F106" s="29" t="s">
+        <v>621</v>
+      </c>
+      <c r="G106" s="29" t="s">
+        <v>622</v>
+      </c>
+      <c r="H106" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="I106" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="J106" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="K106" s="29" t="s">
         <v>11</v>
       </c>
     </row>
@@ -6825,7 +6973,7 @@
         <v>5</v>
       </c>
       <c r="F107" s="9" t="s">
-        <v>541</v>
+        <v>528</v>
       </c>
       <c r="G107" s="9" t="s">
         <v>11</v>
@@ -6840,7 +6988,7 @@
         <v>11</v>
       </c>
       <c r="K107" s="9" t="s">
-        <v>573</v>
+        <v>560</v>
       </c>
     </row>
     <row r="108" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -6866,13 +7014,13 @@
         <v>11</v>
       </c>
       <c r="H108" s="9" t="s">
-        <v>575</v>
+        <v>562</v>
       </c>
       <c r="I108" s="9">
         <v>0</v>
       </c>
       <c r="J108" s="9" t="s">
-        <v>565</v>
+        <v>552</v>
       </c>
       <c r="K108" s="9" t="s">
         <v>11</v>
@@ -6901,13 +7049,13 @@
         <v>11</v>
       </c>
       <c r="H109" s="9" t="s">
-        <v>575</v>
+        <v>562</v>
       </c>
       <c r="I109" s="9">
         <v>0</v>
       </c>
       <c r="J109" s="9" t="s">
-        <v>564</v>
+        <v>551</v>
       </c>
       <c r="K109" s="9" t="s">
         <v>11</v>
@@ -6936,7 +7084,7 @@
         <v>11</v>
       </c>
       <c r="H110" s="9" t="s">
-        <v>575</v>
+        <v>562</v>
       </c>
       <c r="I110" s="9">
         <v>0</v>
@@ -6971,7 +7119,7 @@
         <v>11</v>
       </c>
       <c r="H111" s="9" t="s">
-        <v>575</v>
+        <v>562</v>
       </c>
       <c r="I111" s="9">
         <v>0</v>
@@ -7006,7 +7154,7 @@
         <v>11</v>
       </c>
       <c r="H112" s="9" t="s">
-        <v>575</v>
+        <v>562</v>
       </c>
       <c r="I112" s="9">
         <v>0</v>
@@ -7023,10 +7171,10 @@
         <v>36</v>
       </c>
       <c r="B113" s="9" t="s">
-        <v>578</v>
+        <v>565</v>
       </c>
       <c r="C113" s="6" t="s">
-        <v>576</v>
+        <v>563</v>
       </c>
       <c r="D113" s="9" t="s">
         <v>269</v>
@@ -7035,19 +7183,19 @@
         <v>6</v>
       </c>
       <c r="F113" s="9" t="s">
-        <v>11</v>
+        <v>677</v>
       </c>
       <c r="G113" s="9" t="s">
         <v>11</v>
       </c>
       <c r="H113" s="9" t="s">
-        <v>575</v>
+        <v>562</v>
       </c>
       <c r="I113" s="9">
         <v>0</v>
       </c>
       <c r="J113" s="9" t="s">
-        <v>577</v>
+        <v>564</v>
       </c>
       <c r="K113" s="9"/>
     </row>
@@ -7068,10 +7216,10 @@
         <v>6</v>
       </c>
       <c r="F114" s="7" t="s">
-        <v>545</v>
+        <v>532</v>
       </c>
       <c r="G114" s="9" t="s">
-        <v>556</v>
+        <v>543</v>
       </c>
       <c r="H114" s="9" t="s">
         <v>11</v>
@@ -7086,7 +7234,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="115" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A115" s="9" t="s">
         <v>332</v>
       </c>
@@ -7103,10 +7251,10 @@
         <v>6</v>
       </c>
       <c r="F115" s="9" t="s">
-        <v>546</v>
+        <v>533</v>
       </c>
       <c r="G115" s="9" t="s">
-        <v>558</v>
+        <v>545</v>
       </c>
       <c r="H115" s="9" t="s">
         <v>11</v>
@@ -7121,7 +7269,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="116" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="9" t="s">
         <v>335</v>
       </c>
@@ -7138,10 +7286,10 @@
         <v>6</v>
       </c>
       <c r="F116" s="9" t="s">
-        <v>547</v>
+        <v>534</v>
       </c>
       <c r="G116" s="9" t="s">
-        <v>557</v>
+        <v>544</v>
       </c>
       <c r="H116" s="9" t="s">
         <v>11</v>
@@ -7156,7 +7304,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="117" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="9" t="s">
         <v>331</v>
       </c>
@@ -7173,10 +7321,10 @@
         <v>6</v>
       </c>
       <c r="F117" s="9" t="s">
-        <v>541</v>
+        <v>528</v>
       </c>
       <c r="G117" s="9" t="s">
-        <v>557</v>
+        <v>544</v>
       </c>
       <c r="H117" s="9" t="s">
         <v>11</v>
@@ -7191,27 +7339,25 @@
         <v>11</v>
       </c>
     </row>
-    <row r="118" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="9" t="s">
-        <v>343</v>
-      </c>
+    <row r="118" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A118" s="9"/>
       <c r="B118" s="9" t="s">
-        <v>344</v>
-      </c>
-      <c r="C118" s="5" t="s">
-        <v>342</v>
+        <v>676</v>
+      </c>
+      <c r="C118" s="6" t="s">
+        <v>563</v>
       </c>
       <c r="D118" s="9" t="s">
-        <v>14</v>
+        <v>333</v>
       </c>
       <c r="E118" s="9">
         <v>7</v>
       </c>
       <c r="F118" s="9" t="s">
-        <v>541</v>
+        <v>621</v>
       </c>
       <c r="G118" s="9" t="s">
-        <v>557</v>
+        <v>11</v>
       </c>
       <c r="H118" s="9" t="s">
         <v>11</v>
@@ -7223,30 +7369,30 @@
         <v>11</v>
       </c>
       <c r="K118" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="119" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="9" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B119" s="9" t="s">
-        <v>360</v>
-      </c>
-      <c r="C119" s="6" t="s">
-        <v>348</v>
+        <v>344</v>
+      </c>
+      <c r="C119" s="5" t="s">
+        <v>342</v>
       </c>
       <c r="D119" s="9" t="s">
-        <v>311</v>
+        <v>14</v>
       </c>
       <c r="E119" s="9">
         <v>7</v>
       </c>
       <c r="F119" s="9" t="s">
-        <v>11</v>
+        <v>528</v>
       </c>
       <c r="G119" s="9" t="s">
-        <v>11</v>
+        <v>544</v>
       </c>
       <c r="H119" s="9" t="s">
         <v>11</v>
@@ -7261,24 +7407,24 @@
         <v>11</v>
       </c>
     </row>
-    <row r="120" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="9" t="s">
-        <v>366</v>
+        <v>345</v>
       </c>
       <c r="B120" s="9" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C120" s="6" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D120" s="9" t="s">
-        <v>333</v>
+        <v>311</v>
       </c>
       <c r="E120" s="9">
         <v>7</v>
       </c>
       <c r="F120" s="9" t="s">
-        <v>541</v>
+        <v>11</v>
       </c>
       <c r="G120" s="9" t="s">
         <v>11</v>
@@ -7293,18 +7439,18 @@
         <v>11</v>
       </c>
       <c r="K120" s="9" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="121" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="9" t="s">
-        <v>345</v>
+        <v>366</v>
       </c>
       <c r="B121" s="9" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C121" s="6" t="s">
-        <v>346</v>
+        <v>351</v>
       </c>
       <c r="D121" s="9" t="s">
         <v>333</v>
@@ -7313,7 +7459,7 @@
         <v>7</v>
       </c>
       <c r="F121" s="9" t="s">
-        <v>541</v>
+        <v>528</v>
       </c>
       <c r="G121" s="9" t="s">
         <v>11</v>
@@ -7328,27 +7474,27 @@
         <v>11</v>
       </c>
       <c r="K121" s="9" t="s">
-        <v>347</v>
+        <v>561</v>
       </c>
     </row>
     <row r="122" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="9" t="s">
-        <v>367</v>
+        <v>345</v>
       </c>
       <c r="B122" s="9" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="C122" s="6" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="D122" s="9" t="s">
         <v>333</v>
       </c>
       <c r="E122" s="9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F122" s="9" t="s">
-        <v>11</v>
+        <v>528</v>
       </c>
       <c r="G122" s="9" t="s">
         <v>11</v>
@@ -7363,30 +7509,30 @@
         <v>11</v>
       </c>
       <c r="K122" s="9" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="123" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="9" t="s">
-        <v>29</v>
+        <v>367</v>
       </c>
       <c r="B123" s="9" t="s">
-        <v>570</v>
-      </c>
-      <c r="C123" s="9" t="s">
-        <v>571</v>
+        <v>358</v>
+      </c>
+      <c r="C123" s="6" t="s">
+        <v>350</v>
       </c>
       <c r="D123" s="9" t="s">
-        <v>14</v>
+        <v>333</v>
       </c>
       <c r="E123" s="9">
         <v>8</v>
       </c>
       <c r="F123" s="9" t="s">
-        <v>541</v>
+        <v>11</v>
       </c>
       <c r="G123" s="9" t="s">
-        <v>572</v>
+        <v>11</v>
       </c>
       <c r="H123" s="9" t="s">
         <v>11</v>
@@ -7398,30 +7544,30 @@
         <v>11</v>
       </c>
       <c r="K123" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="124" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A124" s="9" t="s">
-        <v>591</v>
+        <v>29</v>
       </c>
       <c r="B124" s="9" t="s">
-        <v>592</v>
-      </c>
-      <c r="C124" s="6" t="s">
-        <v>590</v>
+        <v>557</v>
+      </c>
+      <c r="C124" s="9" t="s">
+        <v>558</v>
       </c>
       <c r="D124" s="9" t="s">
-        <v>333</v>
+        <v>14</v>
       </c>
       <c r="E124" s="9">
         <v>8</v>
       </c>
       <c r="F124" s="9" t="s">
-        <v>541</v>
+        <v>528</v>
       </c>
       <c r="G124" s="9" t="s">
-        <v>11</v>
+        <v>559</v>
       </c>
       <c r="H124" s="9" t="s">
         <v>11</v>
@@ -7433,27 +7579,27 @@
         <v>11</v>
       </c>
       <c r="K124" s="9" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="125" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A125" s="9" t="s">
-        <v>366</v>
+        <v>578</v>
       </c>
       <c r="B125" s="9" t="s">
-        <v>594</v>
+        <v>579</v>
       </c>
       <c r="C125" s="6" t="s">
-        <v>596</v>
+        <v>577</v>
       </c>
       <c r="D125" s="9" t="s">
         <v>333</v>
       </c>
       <c r="E125" s="9">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F125" s="9" t="s">
-        <v>541</v>
+        <v>528</v>
       </c>
       <c r="G125" s="9" t="s">
         <v>11</v>
@@ -7468,27 +7614,27 @@
         <v>11</v>
       </c>
       <c r="K125" s="9" t="s">
-        <v>595</v>
+        <v>580</v>
       </c>
     </row>
     <row r="126" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="9" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="B126" s="9" t="s">
-        <v>359</v>
+        <v>581</v>
       </c>
       <c r="C126" s="6" t="s">
-        <v>539</v>
+        <v>583</v>
       </c>
       <c r="D126" s="9" t="s">
         <v>333</v>
       </c>
       <c r="E126" s="9">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F126" s="9" t="s">
-        <v>11</v>
+        <v>528</v>
       </c>
       <c r="G126" s="9" t="s">
         <v>11</v>
@@ -7503,18 +7649,18 @@
         <v>11</v>
       </c>
       <c r="K126" s="9" t="s">
-        <v>597</v>
+        <v>582</v>
       </c>
     </row>
     <row r="127" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="9" t="s">
-        <v>356</v>
+        <v>363</v>
       </c>
       <c r="B127" s="9" t="s">
-        <v>600</v>
+        <v>359</v>
       </c>
       <c r="C127" s="6" t="s">
-        <v>598</v>
+        <v>526</v>
       </c>
       <c r="D127" s="9" t="s">
         <v>333</v>
@@ -7538,7 +7684,7 @@
         <v>11</v>
       </c>
       <c r="K127" s="9" t="s">
-        <v>599</v>
+        <v>584</v>
       </c>
     </row>
     <row r="128" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
@@ -7546,10 +7692,10 @@
         <v>356</v>
       </c>
       <c r="B128" s="9" t="s">
-        <v>637</v>
+        <v>587</v>
       </c>
       <c r="C128" s="6" t="s">
-        <v>638</v>
+        <v>585</v>
       </c>
       <c r="D128" s="9" t="s">
         <v>333</v>
@@ -7573,30 +7719,65 @@
         <v>11</v>
       </c>
       <c r="K128" s="9" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="136" spans="2:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="B136" s="9"/>
-    </row>
-    <row r="137" spans="2:2" ht="16" x14ac:dyDescent="0.2">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A129" s="9" t="s">
+        <v>356</v>
+      </c>
+      <c r="B129" s="9" t="s">
+        <v>624</v>
+      </c>
+      <c r="C129" s="6" t="s">
+        <v>625</v>
+      </c>
+      <c r="D129" s="9" t="s">
+        <v>333</v>
+      </c>
+      <c r="E129" s="9">
+        <v>10</v>
+      </c>
+      <c r="F129" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G129" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H129" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I129" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J129" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K129" s="9" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="B137" s="9"/>
     </row>
-    <row r="138" spans="2:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="B138" s="9"/>
     </row>
-    <row r="139" spans="2:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="B139" s="9"/>
     </row>
-    <row r="140" spans="2:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="B140" s="9"/>
     </row>
-    <row r="141" spans="2:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="B141" s="9"/>
+    </row>
+    <row r="142" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="B142" s="9"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K142">
-    <sortCondition ref="E2:E142"/>
+    <sortCondition ref="E108:E142"/>
   </sortState>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7605,10 +7786,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD2BB35C-6E91-D84D-9754-DDB7ED14C6B4}">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7648,50 +7829,50 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
-        <v>408</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="25" t="s">
-        <v>429</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="25" t="s">
-        <v>484</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" t="s">
+    <row r="2" spans="1:11" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="9">
+        <v>0</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>685</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
@@ -7700,7 +7881,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="25" t="s">
-        <v>484</v>
+        <v>474</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
@@ -7720,13 +7901,13 @@
     </row>
     <row r="4" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="25" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
@@ -7735,7 +7916,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="25" t="s">
-        <v>484</v>
+        <v>474</v>
       </c>
       <c r="G4" t="s">
         <v>11</v>
@@ -7755,13 +7936,13 @@
     </row>
     <row r="5" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
@@ -7770,7 +7951,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="25" t="s">
-        <v>484</v>
+        <v>474</v>
       </c>
       <c r="G5" t="s">
         <v>11</v>
@@ -7790,13 +7971,13 @@
     </row>
     <row r="6" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
@@ -7805,7 +7986,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="25" t="s">
-        <v>484</v>
+        <v>474</v>
       </c>
       <c r="G6" t="s">
         <v>11</v>
@@ -7825,13 +8006,13 @@
     </row>
     <row r="7" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="25" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="D7" t="s">
         <v>11</v>
@@ -7840,7 +8021,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="25" t="s">
-        <v>484</v>
+        <v>474</v>
       </c>
       <c r="G7" t="s">
         <v>11</v>
@@ -7860,13 +8041,13 @@
     </row>
     <row r="8" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="25" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="D8" t="s">
         <v>11</v>
@@ -7875,7 +8056,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="25" t="s">
-        <v>484</v>
+        <v>474</v>
       </c>
       <c r="G8" t="s">
         <v>11</v>
@@ -7895,13 +8076,13 @@
     </row>
     <row r="9" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -7910,7 +8091,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="25" t="s">
-        <v>484</v>
+        <v>474</v>
       </c>
       <c r="G9" t="s">
         <v>11</v>
@@ -7930,13 +8111,13 @@
     </row>
     <row r="10" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="D10" t="s">
         <v>11</v>
@@ -7945,7 +8126,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="25" t="s">
-        <v>484</v>
+        <v>474</v>
       </c>
       <c r="G10" t="s">
         <v>11</v>
@@ -7965,13 +8146,13 @@
     </row>
     <row r="11" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="25" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="D11" t="s">
         <v>11</v>
@@ -7980,7 +8161,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="25" t="s">
-        <v>484</v>
+        <v>474</v>
       </c>
       <c r="G11" t="s">
         <v>11</v>
@@ -8000,13 +8181,13 @@
     </row>
     <row r="12" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="25" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D12" t="s">
         <v>11</v>
@@ -8015,7 +8196,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="25" t="s">
-        <v>484</v>
+        <v>474</v>
       </c>
       <c r="G12" t="s">
         <v>11</v>
@@ -8035,13 +8216,13 @@
     </row>
     <row r="13" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="25" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="D13" t="s">
         <v>11</v>
@@ -8050,7 +8231,7 @@
         <v>0</v>
       </c>
       <c r="F13" s="25" t="s">
-        <v>484</v>
+        <v>474</v>
       </c>
       <c r="G13" t="s">
         <v>11</v>
@@ -8070,13 +8251,13 @@
     </row>
     <row r="14" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="25" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="D14" t="s">
         <v>11</v>
@@ -8085,7 +8266,7 @@
         <v>0</v>
       </c>
       <c r="F14" s="25" t="s">
-        <v>484</v>
+        <v>474</v>
       </c>
       <c r="G14" t="s">
         <v>11</v>
@@ -8105,13 +8286,13 @@
     </row>
     <row r="15" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="25" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B15" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="D15" t="s">
         <v>11</v>
@@ -8120,7 +8301,7 @@
         <v>0</v>
       </c>
       <c r="F15" s="25" t="s">
-        <v>484</v>
+        <v>474</v>
       </c>
       <c r="G15" t="s">
         <v>11</v>
@@ -8140,13 +8321,13 @@
     </row>
     <row r="16" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="25" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B16" t="s">
         <v>11</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="D16" t="s">
         <v>11</v>
@@ -8155,7 +8336,7 @@
         <v>0</v>
       </c>
       <c r="F16" s="25" t="s">
-        <v>484</v>
+        <v>474</v>
       </c>
       <c r="G16" t="s">
         <v>11</v>
@@ -8175,13 +8356,13 @@
     </row>
     <row r="17" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="25" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B17" t="s">
         <v>11</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="D17" t="s">
         <v>11</v>
@@ -8190,7 +8371,7 @@
         <v>0</v>
       </c>
       <c r="F17" s="25" t="s">
-        <v>484</v>
+        <v>474</v>
       </c>
       <c r="G17" t="s">
         <v>11</v>
@@ -8210,13 +8391,13 @@
     </row>
     <row r="18" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="25" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B18" t="s">
         <v>11</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="D18" t="s">
         <v>11</v>
@@ -8225,7 +8406,7 @@
         <v>0</v>
       </c>
       <c r="F18" s="25" t="s">
-        <v>484</v>
+        <v>474</v>
       </c>
       <c r="G18" t="s">
         <v>11</v>
@@ -8245,13 +8426,13 @@
     </row>
     <row r="19" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="25" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B19" t="s">
         <v>11</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="D19" t="s">
         <v>11</v>
@@ -8260,7 +8441,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="25" t="s">
-        <v>484</v>
+        <v>474</v>
       </c>
       <c r="G19" t="s">
         <v>11</v>
@@ -8280,13 +8461,13 @@
     </row>
     <row r="20" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="25" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B20" t="s">
         <v>11</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="D20" t="s">
         <v>11</v>
@@ -8295,7 +8476,7 @@
         <v>0</v>
       </c>
       <c r="F20" s="25" t="s">
-        <v>483</v>
+        <v>474</v>
       </c>
       <c r="G20" t="s">
         <v>11</v>
@@ -8315,13 +8496,13 @@
     </row>
     <row r="21" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="25" t="s">
-        <v>427</v>
+        <v>679</v>
       </c>
       <c r="B21" t="s">
         <v>11</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="D21" t="s">
         <v>11</v>
@@ -8330,7 +8511,7 @@
         <v>0</v>
       </c>
       <c r="F21" s="25" t="s">
-        <v>11</v>
+        <v>473</v>
       </c>
       <c r="G21" t="s">
         <v>11</v>
@@ -8349,20 +8530,21 @@
       </c>
     </row>
     <row r="22" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="25" t="s">
-        <v>428</v>
+      <c r="A22" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE, A2:A21)</f>
+        <v>record_id,oci1,oci2,oci3,oci4,oci5,oci6,oci7,oci8,oci9,oci10,oci11,oci12,oci13,oci14,oci15,oci16,oci17,oci18,ocir_complete</v>
       </c>
       <c r="B22" t="s">
         <v>11</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="D22" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22" s="25" t="s">
         <v>11</v>
@@ -8384,52 +8566,429 @@
       </c>
     </row>
     <row r="23" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE, A2:A22)</f>
-        <v>oci1,oci2,oci3,oci4,oci5,oci6,oci7,oci8,oci9,oci10,oci11,oci12,oci13,oci14,oci15,oci16,oci17,oci18,oci_complete,ocimiss_ct,oci_total</v>
+      <c r="A23" s="25" t="s">
+        <v>680</v>
       </c>
       <c r="B23" t="s">
-        <v>11</v>
+        <v>646</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>11</v>
+        <v>627</v>
       </c>
       <c r="D23" t="s">
-        <v>13</v>
+        <v>311</v>
       </c>
       <c r="E23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F23" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="G23" t="s">
-        <v>11</v>
-      </c>
-      <c r="H23" t="s">
-        <v>11</v>
-      </c>
-      <c r="I23" t="s">
-        <v>11</v>
-      </c>
-      <c r="J23" t="s">
-        <v>11</v>
-      </c>
-      <c r="K23" t="s">
-        <v>11</v>
+      <c r="G23" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H23" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="I23" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="J23" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="K23" s="25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="25" t="s">
+        <v>628</v>
+      </c>
+      <c r="B24" t="s">
+        <v>661</v>
+      </c>
+      <c r="C24" s="25" t="s">
+        <v>630</v>
+      </c>
+      <c r="D24" t="s">
+        <v>311</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+      <c r="F24" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H24" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="I24" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="J24" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="K24" s="25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="25" t="s">
+        <v>631</v>
+      </c>
+      <c r="B25" t="s">
+        <v>662</v>
+      </c>
+      <c r="C25" s="25" t="s">
+        <v>635</v>
+      </c>
+      <c r="D25" t="s">
+        <v>311</v>
+      </c>
+      <c r="E25">
+        <v>2</v>
+      </c>
+      <c r="F25" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H25" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="I25" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="J25" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="K25" s="25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="25" t="s">
+        <v>633</v>
+      </c>
+      <c r="B26" t="s">
+        <v>663</v>
+      </c>
+      <c r="C26" s="25" t="s">
+        <v>636</v>
+      </c>
+      <c r="D26" t="s">
+        <v>311</v>
+      </c>
+      <c r="E26">
+        <v>2</v>
+      </c>
+      <c r="F26" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H26" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="I26" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="J26" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="K26" s="25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>646</v>
+      </c>
+      <c r="B27" t="s">
+        <v>626</v>
+      </c>
+      <c r="C27" s="25" t="s">
+        <v>627</v>
+      </c>
+      <c r="D27" t="s">
+        <v>269</v>
+      </c>
+      <c r="E27">
+        <v>3</v>
+      </c>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>681</v>
+      </c>
+      <c r="I27" s="12" t="s">
+        <v>508</v>
+      </c>
+      <c r="J27" s="12" t="s">
+        <v>682</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>661</v>
+      </c>
+      <c r="B28" t="s">
+        <v>629</v>
+      </c>
+      <c r="C28" s="25" t="s">
+        <v>630</v>
+      </c>
+      <c r="D28" t="s">
+        <v>269</v>
+      </c>
+      <c r="E28">
+        <v>3</v>
+      </c>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H28" s="12" t="s">
+        <v>666</v>
+      </c>
+      <c r="I28" s="12" t="s">
+        <v>508</v>
+      </c>
+      <c r="J28" s="12" t="s">
+        <v>672</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>662</v>
+      </c>
+      <c r="B29" t="s">
+        <v>632</v>
+      </c>
+      <c r="C29" s="25" t="s">
+        <v>635</v>
+      </c>
+      <c r="D29" t="s">
+        <v>269</v>
+      </c>
+      <c r="E29">
+        <v>3</v>
+      </c>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H29" s="12" t="s">
+        <v>683</v>
+      </c>
+      <c r="I29" s="12" t="s">
+        <v>508</v>
+      </c>
+      <c r="J29" s="12" t="s">
+        <v>671</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>663</v>
+      </c>
+      <c r="B30" t="s">
+        <v>634</v>
+      </c>
+      <c r="C30" s="25" t="s">
+        <v>636</v>
+      </c>
+      <c r="D30" t="s">
+        <v>269</v>
+      </c>
+      <c r="E30">
+        <v>3</v>
+      </c>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H30" s="12" t="s">
+        <v>665</v>
+      </c>
+      <c r="I30" s="12" t="s">
+        <v>508</v>
+      </c>
+      <c r="J30" s="12" t="s">
+        <v>670</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A31" s="25" t="s">
+        <v>637</v>
+      </c>
+      <c r="B31" t="s">
+        <v>664</v>
+      </c>
+      <c r="C31" s="25" t="s">
+        <v>639</v>
+      </c>
+      <c r="D31" t="s">
+        <v>311</v>
+      </c>
+      <c r="E31">
+        <v>4</v>
+      </c>
+      <c r="F31" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="G31" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H31" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="I31" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="J31" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="K31" s="25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A32" s="25" t="s">
+        <v>664</v>
+      </c>
+      <c r="B32" t="s">
+        <v>638</v>
+      </c>
+      <c r="C32" s="25" t="s">
+        <v>639</v>
+      </c>
+      <c r="D32" t="s">
+        <v>269</v>
+      </c>
+      <c r="E32">
+        <v>5</v>
+      </c>
+      <c r="F32" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="G32" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H32" s="12" t="s">
+        <v>667</v>
+      </c>
+      <c r="I32" s="25" t="s">
+        <v>508</v>
+      </c>
+      <c r="J32" s="12" t="s">
+        <v>669</v>
+      </c>
+      <c r="K32" s="25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A33" s="25" t="s">
+        <v>638</v>
+      </c>
+      <c r="B33" t="s">
+        <v>656</v>
+      </c>
+      <c r="C33" s="25" t="s">
+        <v>658</v>
+      </c>
+      <c r="D33" t="s">
+        <v>333</v>
+      </c>
+      <c r="E33">
+        <v>6</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>528</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H33" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="I33" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="J33" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="K33" s="12" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A34" s="25" t="s">
+        <v>638</v>
+      </c>
+      <c r="B34" t="s">
+        <v>657</v>
+      </c>
+      <c r="C34" s="25" t="s">
+        <v>659</v>
+      </c>
+      <c r="D34" t="s">
+        <v>333</v>
+      </c>
+      <c r="E34">
+        <v>6</v>
+      </c>
+      <c r="F34" s="25" t="s">
+        <v>660</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H34" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="I34" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="J34" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="K34" s="12" t="s">
+        <v>684</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="29" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A5C7946-155C-C64C-B6E6-9BB8EBA62A76}">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8472,50 +9031,50 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
-        <v>450</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="25" t="s">
-        <v>466</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="25" t="s">
-        <v>482</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" t="s">
+    <row r="2" spans="1:11" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="9">
+        <v>0</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>685</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>467</v>
+        <v>457</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
@@ -8524,7 +9083,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="25" t="s">
-        <v>482</v>
+        <v>472</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
@@ -8544,13 +9103,13 @@
     </row>
     <row r="4" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="25" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>468</v>
+        <v>458</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
@@ -8559,7 +9118,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="25" t="s">
-        <v>482</v>
+        <v>472</v>
       </c>
       <c r="G4" t="s">
         <v>11</v>
@@ -8579,13 +9138,13 @@
     </row>
     <row r="5" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>469</v>
+        <v>459</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -8594,7 +9153,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="25" t="s">
-        <v>482</v>
+        <v>472</v>
       </c>
       <c r="G5" t="s">
         <v>11</v>
@@ -8614,13 +9173,13 @@
     </row>
     <row r="6" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>470</v>
+        <v>460</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -8629,7 +9188,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="25" t="s">
-        <v>482</v>
+        <v>472</v>
       </c>
       <c r="G6" t="s">
         <v>11</v>
@@ -8649,13 +9208,13 @@
     </row>
     <row r="7" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="25" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>471</v>
+        <v>461</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
@@ -8664,7 +9223,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="25" t="s">
-        <v>482</v>
+        <v>472</v>
       </c>
       <c r="G7" t="s">
         <v>11</v>
@@ -8684,13 +9243,13 @@
     </row>
     <row r="8" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="25" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>472</v>
+        <v>462</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
@@ -8699,7 +9258,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="25" t="s">
-        <v>482</v>
+        <v>472</v>
       </c>
       <c r="G8" t="s">
         <v>11</v>
@@ -8719,13 +9278,13 @@
     </row>
     <row r="9" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>473</v>
+        <v>463</v>
       </c>
       <c r="D9" t="s">
         <v>12</v>
@@ -8734,7 +9293,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="25" t="s">
-        <v>482</v>
+        <v>472</v>
       </c>
       <c r="G9" t="s">
         <v>11</v>
@@ -8754,13 +9313,13 @@
     </row>
     <row r="10" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>474</v>
+        <v>464</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -8769,7 +9328,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="25" t="s">
-        <v>482</v>
+        <v>472</v>
       </c>
       <c r="G10" t="s">
         <v>11</v>
@@ -8789,13 +9348,13 @@
     </row>
     <row r="11" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="25" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>475</v>
+        <v>465</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
@@ -8804,7 +9363,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="25" t="s">
-        <v>482</v>
+        <v>472</v>
       </c>
       <c r="G11" t="s">
         <v>11</v>
@@ -8824,13 +9383,13 @@
     </row>
     <row r="12" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="25" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>476</v>
+        <v>466</v>
       </c>
       <c r="D12" t="s">
         <v>12</v>
@@ -8839,7 +9398,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="25" t="s">
-        <v>482</v>
+        <v>472</v>
       </c>
       <c r="G12" t="s">
         <v>11</v>
@@ -8859,13 +9418,13 @@
     </row>
     <row r="13" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="25" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>477</v>
+        <v>467</v>
       </c>
       <c r="D13" t="s">
         <v>12</v>
@@ -8874,7 +9433,7 @@
         <v>0</v>
       </c>
       <c r="F13" s="25" t="s">
-        <v>482</v>
+        <v>472</v>
       </c>
       <c r="G13" t="s">
         <v>11</v>
@@ -8894,13 +9453,13 @@
     </row>
     <row r="14" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="25" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>478</v>
+        <v>468</v>
       </c>
       <c r="D14" t="s">
         <v>12</v>
@@ -8909,7 +9468,7 @@
         <v>0</v>
       </c>
       <c r="F14" s="25" t="s">
-        <v>483</v>
+        <v>472</v>
       </c>
       <c r="G14" t="s">
         <v>11</v>
@@ -8928,126 +9487,126 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="25" t="s">
-        <v>463</v>
+      <c r="A15" s="25" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE, A2:A14)</f>
+        <v>record_id,mps4_ps,mps6_ps,mps9_cm,mps14_cm,mps16_ps,mps17_da,mps18_cm,mps19_ps,mps21_cm,mps28_da,mps32_da,mps33_da</v>
       </c>
       <c r="B15" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>479</v>
+        <v>11</v>
       </c>
       <c r="D15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="G15" t="s">
-        <v>11</v>
-      </c>
-      <c r="H15" t="s">
-        <v>11</v>
-      </c>
-      <c r="I15" t="s">
-        <v>11</v>
-      </c>
-      <c r="J15" t="s">
-        <v>11</v>
-      </c>
-      <c r="K15" t="s">
+      <c r="G15" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="K15" s="25" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="25" t="s">
-        <v>464</v>
+        <v>642</v>
       </c>
       <c r="B16" t="s">
-        <v>11</v>
+        <v>647</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>480</v>
+        <v>471</v>
       </c>
       <c r="D16" t="s">
-        <v>12</v>
+        <v>311</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F16" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="G16" t="s">
-        <v>11</v>
-      </c>
-      <c r="H16" t="s">
-        <v>11</v>
-      </c>
-      <c r="I16" t="s">
-        <v>11</v>
-      </c>
-      <c r="J16" t="s">
-        <v>11</v>
-      </c>
-      <c r="K16" t="s">
+      <c r="G16" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="J16" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="K16" s="25" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="25" t="s">
-        <v>465</v>
+        <v>644</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
+        <v>648</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>481</v>
+        <v>470</v>
       </c>
       <c r="D17" t="s">
-        <v>12</v>
+        <v>311</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F17" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="G17" t="s">
-        <v>11</v>
-      </c>
-      <c r="H17" t="s">
-        <v>11</v>
-      </c>
-      <c r="I17" t="s">
-        <v>11</v>
-      </c>
-      <c r="J17" t="s">
-        <v>11</v>
-      </c>
-      <c r="K17" t="s">
+      <c r="G17" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="I17" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="J17" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="K17" s="25" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="25" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE, A2:A17)</f>
-        <v>mps4_ps,mps6_ps,mps9_cm,mps14_cm,mps16_ps,mps17_da,mps18_cm,mps19_ps,mps21_cm,mps28_da,mps32_da,mps33_da,perfectionism_complete,da_total,cm_total,ps_total</v>
+      <c r="A18" s="25" t="s">
+        <v>645</v>
       </c>
       <c r="B18" t="s">
-        <v>11</v>
+        <v>649</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>11</v>
+        <v>469</v>
       </c>
       <c r="D18" t="s">
-        <v>13</v>
+        <v>311</v>
       </c>
       <c r="E18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F18" s="25" t="s">
         <v>11</v>
@@ -9068,38 +9627,108 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="25" t="s">
-        <v>507</v>
+    <row r="19" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>647</v>
       </c>
       <c r="B19" t="s">
-        <v>506</v>
+        <v>640</v>
       </c>
       <c r="C19" s="25" t="s">
+        <v>650</v>
+      </c>
+      <c r="D19" t="s">
+        <v>269</v>
+      </c>
+      <c r="E19">
+        <v>3</v>
+      </c>
+      <c r="F19" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>653</v>
+      </c>
+      <c r="I19" s="12" t="s">
         <v>508</v>
       </c>
-      <c r="D19" t="s">
-        <v>311</v>
-      </c>
-      <c r="E19">
-        <v>2</v>
-      </c>
-      <c r="F19" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="G19" t="s">
-        <v>11</v>
-      </c>
-      <c r="H19" t="s">
-        <v>11</v>
-      </c>
-      <c r="I19" t="s">
-        <v>11</v>
-      </c>
-      <c r="J19" t="s">
-        <v>11</v>
-      </c>
-      <c r="K19" t="s">
+      <c r="J19" s="12" t="s">
+        <v>673</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>648</v>
+      </c>
+      <c r="B20" t="s">
+        <v>641</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>651</v>
+      </c>
+      <c r="D20" t="s">
+        <v>269</v>
+      </c>
+      <c r="E20">
+        <v>3</v>
+      </c>
+      <c r="F20" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>654</v>
+      </c>
+      <c r="I20" s="12" t="s">
+        <v>508</v>
+      </c>
+      <c r="J20" s="12" t="s">
+        <v>674</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>649</v>
+      </c>
+      <c r="B21" t="s">
+        <v>643</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>652</v>
+      </c>
+      <c r="D21" t="s">
+        <v>269</v>
+      </c>
+      <c r="E21">
+        <v>3</v>
+      </c>
+      <c r="F21" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>655</v>
+      </c>
+      <c r="I21" s="12" t="s">
+        <v>508</v>
+      </c>
+      <c r="J21" s="12" t="s">
+        <v>675</v>
+      </c>
+      <c r="K21" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -9112,8 +9741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A674610-18BE-F241-9D23-4CA806F45B9D}">
   <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="A45" sqref="A1:XFD45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10177,7 +10806,7 @@
     </row>
     <row r="31" spans="1:11" s="19" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="22" t="s">
-        <v>537</v>
+        <v>524</v>
       </c>
       <c r="B31" s="19" t="s">
         <v>11</v>
@@ -10212,10 +10841,10 @@
     </row>
     <row r="32" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>533</v>
+        <v>520</v>
       </c>
       <c r="B32" t="s">
-        <v>497</v>
+        <v>487</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>391</v>
@@ -10247,10 +10876,10 @@
     </row>
     <row r="33" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>534</v>
+        <v>521</v>
       </c>
       <c r="B33" t="s">
-        <v>498</v>
+        <v>488</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>395</v>
@@ -10282,10 +10911,10 @@
     </row>
     <row r="34" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>536</v>
+        <v>523</v>
       </c>
       <c r="B34" t="s">
-        <v>499</v>
+        <v>489</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>396</v>
@@ -10317,10 +10946,10 @@
     </row>
     <row r="35" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>535</v>
+        <v>522</v>
       </c>
       <c r="B35" t="s">
-        <v>500</v>
+        <v>490</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>398</v>
@@ -10373,13 +11002,13 @@
         <v>11</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>583</v>
+        <v>570</v>
       </c>
       <c r="I36" s="2">
         <v>0</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>584</v>
+        <v>571</v>
       </c>
       <c r="K36" s="2" t="s">
         <v>11</v>
@@ -10507,7 +11136,7 @@
         <v>3</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>552</v>
+        <v>539</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>11</v>
@@ -10527,13 +11156,13 @@
     </row>
     <row r="41" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>497</v>
+        <v>487</v>
       </c>
       <c r="B41" t="s">
         <v>390</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>502</v>
+        <v>492</v>
       </c>
       <c r="D41" t="s">
         <v>269</v>
@@ -10545,13 +11174,13 @@
         <v>11</v>
       </c>
       <c r="H41" s="12" t="s">
-        <v>527</v>
+        <v>514</v>
       </c>
       <c r="I41" s="12" t="s">
-        <v>521</v>
+        <v>508</v>
       </c>
       <c r="J41" s="12" t="s">
-        <v>528</v>
+        <v>515</v>
       </c>
       <c r="K41" s="2" t="s">
         <v>11</v>
@@ -10559,13 +11188,13 @@
     </row>
     <row r="42" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>498</v>
+        <v>488</v>
       </c>
       <c r="B42" t="s">
         <v>393</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>503</v>
+        <v>493</v>
       </c>
       <c r="D42" t="s">
         <v>269</v>
@@ -10577,13 +11206,13 @@
         <v>11</v>
       </c>
       <c r="H42" s="12" t="s">
-        <v>529</v>
+        <v>516</v>
       </c>
       <c r="I42" s="12" t="s">
-        <v>521</v>
+        <v>508</v>
       </c>
       <c r="J42" s="12" t="s">
-        <v>530</v>
+        <v>517</v>
       </c>
       <c r="K42" s="2" t="s">
         <v>11</v>
@@ -10591,13 +11220,13 @@
     </row>
     <row r="43" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>499</v>
+        <v>489</v>
       </c>
       <c r="B43" t="s">
         <v>394</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>504</v>
+        <v>494</v>
       </c>
       <c r="D43" t="s">
         <v>269</v>
@@ -10609,13 +11238,13 @@
         <v>11</v>
       </c>
       <c r="H43" s="12" t="s">
-        <v>531</v>
+        <v>518</v>
       </c>
       <c r="I43" s="12" t="s">
-        <v>521</v>
+        <v>508</v>
       </c>
       <c r="J43" s="12" t="s">
-        <v>532</v>
+        <v>519</v>
       </c>
       <c r="K43" s="2" t="s">
         <v>11</v>
@@ -10623,13 +11252,13 @@
     </row>
     <row r="44" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>500</v>
+        <v>490</v>
       </c>
       <c r="B44" t="s">
         <v>397</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>505</v>
+        <v>495</v>
       </c>
       <c r="D44" t="s">
         <v>269</v>
@@ -10641,13 +11270,13 @@
         <v>11</v>
       </c>
       <c r="H44" s="12" t="s">
-        <v>538</v>
+        <v>525</v>
       </c>
       <c r="I44" s="12" t="s">
-        <v>521</v>
+        <v>508</v>
       </c>
       <c r="J44" s="12" t="s">
-        <v>528</v>
+        <v>515</v>
       </c>
       <c r="K44" s="2" t="s">
         <v>11</v>
@@ -10655,7 +11284,7 @@
     </row>
     <row r="45" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>501</v>
+        <v>491</v>
       </c>
       <c r="B45" t="s">
         <v>399</v>
@@ -10700,8 +11329,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F526704-404D-A742-B160-DD024D64BBA1}">
   <dimension ref="A1:K63"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63"/>
+    <sheetView topLeftCell="C49" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11698,7 +12327,7 @@
         <v>185</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>513</v>
+        <v>500</v>
       </c>
       <c r="C29" s="12" t="s">
         <v>209</v>
@@ -11908,7 +12537,7 @@
         <v>191</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>581</v>
+        <v>568</v>
       </c>
       <c r="C35" s="12" t="s">
         <v>353</v>
@@ -11920,7 +12549,7 @@
         <v>2</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>553</v>
+        <v>540</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>312</v>
@@ -12060,7 +12689,7 @@
         <v>2</v>
       </c>
       <c r="F39" s="12" t="s">
-        <v>553</v>
+        <v>540</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>312</v>
@@ -12153,7 +12782,7 @@
         <v>198</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>579</v>
+        <v>566</v>
       </c>
       <c r="C42" s="12" t="s">
         <v>222</v>
@@ -12363,7 +12992,7 @@
         <v>204</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>515</v>
+        <v>502</v>
       </c>
       <c r="C48" s="12" t="s">
         <v>228</v>
@@ -12468,7 +13097,7 @@
         <v>207</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>514</v>
+        <v>501</v>
       </c>
       <c r="C51" s="12" t="s">
         <v>231</v>
@@ -12500,10 +13129,10 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
-        <v>580</v>
+        <v>567</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>485</v>
+        <v>475</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>314</v>
@@ -12535,13 +13164,13 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
-        <v>485</v>
+        <v>475</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>313</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>494</v>
+        <v>484</v>
       </c>
       <c r="D53" s="5" t="s">
         <v>269</v>
@@ -12556,13 +13185,13 @@
         <v>11</v>
       </c>
       <c r="H53" s="12" t="s">
-        <v>495</v>
+        <v>485</v>
       </c>
       <c r="I53" s="12" t="s">
-        <v>521</v>
+        <v>508</v>
       </c>
       <c r="J53" s="12" t="s">
-        <v>520</v>
+        <v>507</v>
       </c>
       <c r="K53" s="12" t="s">
         <v>11</v>
@@ -12570,10 +13199,10 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
-        <v>582</v>
+        <v>569</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>486</v>
+        <v>476</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>316</v>
@@ -12605,13 +13234,13 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="5" t="s">
-        <v>486</v>
+        <v>476</v>
       </c>
       <c r="B55" s="5" t="s">
         <v>315</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>493</v>
+        <v>483</v>
       </c>
       <c r="D55" s="5" t="s">
         <v>269</v>
@@ -12626,13 +13255,13 @@
         <v>11</v>
       </c>
       <c r="H55" s="12" t="s">
-        <v>516</v>
+        <v>503</v>
       </c>
       <c r="I55" s="12" t="s">
-        <v>521</v>
+        <v>508</v>
       </c>
       <c r="J55" s="12" t="s">
-        <v>522</v>
+        <v>509</v>
       </c>
       <c r="K55" s="12" t="s">
         <v>11</v>
@@ -12643,7 +13272,7 @@
         <v>317</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>487</v>
+        <v>477</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>319</v>
@@ -12675,13 +13304,13 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="5" t="s">
-        <v>487</v>
+        <v>477</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>318</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>492</v>
+        <v>482</v>
       </c>
       <c r="D57" s="5" t="s">
         <v>269</v>
@@ -12696,13 +13325,13 @@
         <v>11</v>
       </c>
       <c r="H57" s="12" t="s">
-        <v>517</v>
+        <v>504</v>
       </c>
       <c r="I57" s="12" t="s">
-        <v>521</v>
+        <v>508</v>
       </c>
       <c r="J57" s="12" t="s">
-        <v>523</v>
+        <v>510</v>
       </c>
       <c r="K57" s="12" t="s">
         <v>11</v>
@@ -12713,7 +13342,7 @@
         <v>320</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>488</v>
+        <v>478</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>322</v>
@@ -12745,13 +13374,13 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" s="5" t="s">
-        <v>488</v>
+        <v>478</v>
       </c>
       <c r="B59" s="5" t="s">
         <v>321</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>491</v>
+        <v>481</v>
       </c>
       <c r="D59" s="5" t="s">
         <v>269</v>
@@ -12766,13 +13395,13 @@
         <v>11</v>
       </c>
       <c r="H59" s="12" t="s">
-        <v>518</v>
+        <v>505</v>
       </c>
       <c r="I59" s="12" t="s">
-        <v>521</v>
+        <v>508</v>
       </c>
       <c r="J59" s="12" t="s">
-        <v>524</v>
+        <v>511</v>
       </c>
       <c r="K59" s="12" t="s">
         <v>11</v>
@@ -12783,7 +13412,7 @@
         <v>323</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>489</v>
+        <v>479</v>
       </c>
       <c r="C60" s="5" t="s">
         <v>324</v>
@@ -12815,13 +13444,13 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" s="5" t="s">
-        <v>489</v>
+        <v>479</v>
       </c>
       <c r="B61" s="5" t="s">
         <v>327</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>490</v>
+        <v>480</v>
       </c>
       <c r="D61" s="5" t="s">
         <v>269</v>
@@ -12836,13 +13465,13 @@
         <v>11</v>
       </c>
       <c r="H61" s="12" t="s">
-        <v>519</v>
+        <v>506</v>
       </c>
       <c r="I61" s="12" t="s">
-        <v>521</v>
+        <v>508</v>
       </c>
       <c r="J61" s="12" t="s">
-        <v>525</v>
+        <v>512</v>
       </c>
       <c r="K61" s="12" t="s">
         <v>11</v>
@@ -12892,7 +13521,7 @@
         <v>354</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>496</v>
+        <v>486</v>
       </c>
       <c r="D63" s="5" t="s">
         <v>333</v>
@@ -12901,7 +13530,7 @@
         <v>6</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>541</v>
+        <v>528</v>
       </c>
       <c r="G63" s="5" t="s">
         <v>11</v>
@@ -12916,7 +13545,7 @@
         <v>11</v>
       </c>
       <c r="K63" s="12" t="s">
-        <v>526</v>
+        <v>513</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update - new defs
</commit_message>
<xml_diff>
--- a/scoring/EDGI_exercise_scoresheet.xlsx
+++ b/scoring/EDGI_exercise_scoresheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kschaumberg/Dropbox/Wisconsin/Papers (External)/EDGI_Exercise/scoring/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kschaumberg/Library/CloudStorage/Dropbox/Papers/EDGI_Exercise/scoring/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D89A0ED7-ED6C-7340-A110-E89D86DEEBCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5304A0B6-3447-E942-9FEF-F77AF1581D9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4960" yWindow="760" windowWidth="24980" windowHeight="13860" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="24980" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ED100k" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2891" uniqueCount="686">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2899" uniqueCount="689">
   <si>
     <t>raw_vars</t>
   </si>
@@ -1103,21 +1103,9 @@
     <t>cet_clinical</t>
   </si>
   <si>
-    <t>ED100k_ex_compulsive</t>
-  </si>
-  <si>
     <t>ED100k_ex_compulsive_1mo, ED100k_ex_compensatory</t>
   </si>
   <si>
-    <t>ED100k_ex_compensatory</t>
-  </si>
-  <si>
-    <t>ED100k_ex_excessive</t>
-  </si>
-  <si>
-    <t>ED100k_ex_addictive</t>
-  </si>
-  <si>
     <t>ED100k_ex_interfere_sum</t>
   </si>
   <si>
@@ -1697,9 +1685,6 @@
     <t>as.numeric(ex_diet)</t>
   </si>
   <si>
-    <t>ED100k_ex_compulsive_1mo == 1 &amp; ED100k_ex_freq == 4 ~ 1, ED100k_ex_compulsive_1mo  == 1 &amp; ED100k_ex_freq &lt; 4 ~ 0, ED100k_ex_compulsive_1mo == 0 ~0</t>
-  </si>
-  <si>
     <t xml:space="preserve">ethnicity == 1 ~3, ED100k_race_dummy_1 == 0 &amp; ethnicity == 2~0, ED100k_race_dummy_2 == 1 ~ 1, ED100k_race_dummy_2 == 2 &amp; ethnicity == 2 ~ 2, ED100k_race_dummy_2 == 3 &amp; ethnicity == 2 ~4 </t>
   </si>
   <si>
@@ -1709,33 +1694,18 @@
     <t>ED100k_race_dummy_1 == 0 &amp; ethnicity == 2 ~ 0, ED100k_race_dummy_1 ==1 | ethnicity == 1 ~ 1</t>
   </si>
   <si>
-    <t>ED100k_ex_any</t>
-  </si>
-  <si>
     <t>Any Intentional Exercise to Control Weight and Shape</t>
   </si>
   <si>
-    <t>1= 0, 2= 1, 3 = 1</t>
-  </si>
-  <si>
     <t>ex_compel_2 == 0 &amp; ex_distress_2 == 0 ~ 0, ex_compel_2 == 1 | ex_distress_2 == 1 ~ 1</t>
   </si>
   <si>
-    <t>ED100k_ex_compulsive == 1 &amp; ED100k_ex_dur &lt;= 1 | ED100k_ex_compulsive == 0 ~ 0, ED100k_ex_compulsive == 1 &amp; ED100k_ex_dur &gt; 1 ~ 1</t>
-  </si>
-  <si>
-    <t>ED100k_ex_compulsive == 0</t>
-  </si>
-  <si>
     <t xml:space="preserve">Does participant report current compuslive exercise </t>
   </si>
   <si>
     <t>as.numeric(ex_current)</t>
   </si>
   <si>
-    <t>ED100k_ex_compulsive_current</t>
-  </si>
-  <si>
     <t>cet_15_makeup</t>
   </si>
   <si>
@@ -1775,18 +1745,12 @@
     <t>ED100k_ex_compulsive, ED100k_exercise_icb</t>
   </si>
   <si>
-    <t>ED100k_ex_compulsive_strict</t>
-  </si>
-  <si>
     <t>ED100k_exercise_icb &lt; 2 | ex_compel_2  + ex_distress_2 == 0 ~ 0, ED100k_exercise_icb == 2 &amp; ex_compel_2 == 1  | ED100k_exercise_icb == 2 &amp; ex_distress_2 == 1 ~ 1</t>
   </si>
   <si>
     <t>ED100k_ex_compulsive_strict_3mo</t>
   </si>
   <si>
-    <t>ED100k_ex_compulsive_strict == 1 &amp; ED100k_ex_dur &lt;= 2 | ED100k_ex_compulsive_strict == 0 ~ 0, ED100k_ex_compulsive_strict == 1 &amp; ED100k_ex_dur &gt; 2 ~ 1</t>
-  </si>
-  <si>
     <t>Compulsive/Driven Exercise that lasted for at least three months and weight/shape exercise endorsed 'more often'</t>
   </si>
   <si>
@@ -1796,12 +1760,6 @@
     <t>reports regular driven exercise for at least 3 months OR any compensatory exercise</t>
   </si>
   <si>
-    <t>ED100k_ex_compulsive_strict_3mo == 0 ~ 0, ED100k_ex_compensatory == 0 ~ 0, ED100k_ex_compulsive_strict_3mo == 1 | ED100k_ex_compensatory ==1 ~ 1</t>
-  </si>
-  <si>
-    <t>ED100k_ex_maladaptive</t>
-  </si>
-  <si>
     <t>as.numeric(ex_current)+1</t>
   </si>
   <si>
@@ -1907,15 +1865,6 @@
     <t>0=0, 1=1, 2=2, -8 = NaN</t>
   </si>
   <si>
-    <t>ED100k_ex_compulsive == 0 ~ 0, ED100k_ex_compensatory == 0 ~ 0, ED100k_ex_compulsive == 1 | ED100k_ex_compensatory ==1 ~ 1</t>
-  </si>
-  <si>
-    <t>ED100k_ex_maladaptive_1</t>
-  </si>
-  <si>
-    <t>reports any compulsive OR any compensatory exercise</t>
-  </si>
-  <si>
     <t>oci12_wash</t>
   </si>
   <si>
@@ -2069,12 +2018,6 @@
     <t>ED100k_ex_compulsive_current2</t>
   </si>
   <si>
-    <t>No Current compulsive exercise = 0, current compulsive exercise = 1</t>
-  </si>
-  <si>
-    <t>ED100k_ex_compulsive == 0 ~ 0, ED100k_ex_compulsive == 1 &amp; ED100k_ex_compulsive_current == 0 ~ 1, ED100k_ex_compulsive_current == 1 ~ 2</t>
-  </si>
-  <si>
     <t>ocir_complete</t>
   </si>
   <si>
@@ -2094,6 +2037,72 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Does participant report current maladaptive exercise </t>
+  </si>
+  <si>
+    <t>No History, History (not current) or current maladaptive exercise</t>
+  </si>
+  <si>
+    <t>ED100k_exercise_icb == 2 &amp; ED100k_ex_compulsive_1mo == 1 &amp; ED100k_ex_freq == 4 ~ 1, ED100k_exercise_icb &lt; 2 | ED100k_ex_compulsive_1mo  == 0 | ED100k_ex_freq &lt; 4 ~ 0  ~0</t>
+  </si>
+  <si>
+    <t>ED100k_ex_maladaptive_old</t>
+  </si>
+  <si>
+    <t>0= 0, 1= 1, 2 = 1</t>
+  </si>
+  <si>
+    <t>0= 0, 1= 0, 2 = 1</t>
+  </si>
+  <si>
+    <t>ED100k_ex4_compulsive_narrow</t>
+  </si>
+  <si>
+    <t>ED100k_ex5_addictive</t>
+  </si>
+  <si>
+    <t>ED100k_ex8_maladaptive_current</t>
+  </si>
+  <si>
+    <t>No Current maladaptive exercise = 0, current maladaptive exercise = 1</t>
+  </si>
+  <si>
+    <t>ED100k_ex7_compensatory</t>
+  </si>
+  <si>
+    <t>ED100k_ex6_excessive</t>
+  </si>
+  <si>
+    <t>ED100k_ex3_compulsive_broad</t>
+  </si>
+  <si>
+    <t>ED100k_ex3_compulsive_broad == 1 &amp; ED100k_ex_dur &lt;= 1 | ED100k_ex3_compulsive_broad == 0 ~ 0, ED100k_ex3_compulsive_broad == 1 &amp; ED100k_ex_dur &gt; 1 ~ 1</t>
+  </si>
+  <si>
+    <t>ED100k_ex9_maladaptive_hxplusc</t>
+  </si>
+  <si>
+    <t>ED100k_ex1_Q1_broad</t>
+  </si>
+  <si>
+    <t>ED100k_ex2_Q1_narrow</t>
+  </si>
+  <si>
+    <t>ED100k_ex3_compulsive_broad == 0</t>
+  </si>
+  <si>
+    <t>ED100k_ex3_compulsive_broad == 0 ~ 0, ED100k_ex3_compulsive_broad == 1 &amp; ED100k_ex8_maladaptive_current == 0 ~ 1, ED100k_ex8_maladaptive_current == 1 ~ 2</t>
+  </si>
+  <si>
+    <t>ED100k_exercise_icb == 0 ~ 0, ED100k_exercise_icb &gt;= 1 &amp; ED100k_ex8_maladaptive_current == 0 ~ 1, ED100k_ex8_maladaptive_current == 1 ~ 2</t>
+  </si>
+  <si>
+    <t>ED100k_ex_compulsive_strict_3mo == 0 ~ 0, ED100k_ex7_compensatory == 0 ~ 0, ED100k_ex_compulsive_strict_3mo == 1 | ED100k_ex7_compensatory ==1 ~ 1</t>
+  </si>
+  <si>
+    <t>ED100k_ex4_compulsive_narrow == 1 &amp; ED100k_ex_dur &lt;= 2 | ED100k_ex4_compulsive_narrow == 0 ~ 0, ED100k_ex4_compulsive_narrow == 1 &amp; ED100k_ex_dur &gt; 2 ~ 1</t>
   </si>
 </sst>
 </file>
@@ -3224,10 +3233,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L142"/>
+  <dimension ref="A1:L143"/>
   <sheetViews>
-    <sheetView zoomScale="119" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A119" sqref="A119"/>
+    <sheetView tabSelected="1" topLeftCell="C119" zoomScale="119" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="F126" sqref="F126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3351,7 +3360,7 @@
     </row>
     <row r="4" spans="1:11" s="15" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>11</v>
@@ -3561,13 +3570,13 @@
     </row>
     <row r="10" spans="1:11" s="28" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="26" t="s">
-        <v>594</v>
+        <v>580</v>
       </c>
       <c r="B10" s="26" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>595</v>
+        <v>581</v>
       </c>
       <c r="D10" s="26" t="s">
         <v>11</v>
@@ -3576,7 +3585,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="26" t="s">
-        <v>596</v>
+        <v>582</v>
       </c>
       <c r="G10" s="13" t="s">
         <v>11</v>
@@ -3596,13 +3605,13 @@
     </row>
     <row r="11" spans="1:11" s="28" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="26" t="s">
-        <v>597</v>
+        <v>583</v>
       </c>
       <c r="B11" s="26" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>598</v>
+        <v>584</v>
       </c>
       <c r="D11" s="26" t="s">
         <v>11</v>
@@ -3611,7 +3620,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="26" t="s">
-        <v>596</v>
+        <v>582</v>
       </c>
       <c r="G11" s="13" t="s">
         <v>11</v>
@@ -3631,13 +3640,13 @@
     </row>
     <row r="12" spans="1:11" s="28" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="26" t="s">
-        <v>591</v>
+        <v>577</v>
       </c>
       <c r="B12" s="26" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>592</v>
+        <v>578</v>
       </c>
       <c r="D12" s="26" t="s">
         <v>12</v>
@@ -3646,7 +3655,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="26" t="s">
-        <v>593</v>
+        <v>579</v>
       </c>
       <c r="G12" s="13" t="s">
         <v>11</v>
@@ -3666,7 +3675,7 @@
     </row>
     <row r="13" spans="1:11" s="15" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="B13" s="13" t="s">
         <v>11</v>
@@ -5732,13 +5741,13 @@
     </row>
     <row r="72" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="9" t="s">
-        <v>496</v>
+        <v>40</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>357</v>
+        <v>595</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>96</v>
+        <v>596</v>
       </c>
       <c r="D72" s="9" t="s">
         <v>14</v>
@@ -5746,11 +5755,11 @@
       <c r="E72" s="9">
         <v>2</v>
       </c>
-      <c r="F72" s="9" t="s">
-        <v>528</v>
-      </c>
-      <c r="G72" t="s">
-        <v>541</v>
+      <c r="F72" s="30" t="s">
+        <v>597</v>
+      </c>
+      <c r="G72" s="9" t="s">
+        <v>598</v>
       </c>
       <c r="H72" s="9" t="s">
         <v>11</v>
@@ -5782,10 +5791,10 @@
         <v>2</v>
       </c>
       <c r="F73" s="9" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="G73" s="9" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="H73" s="9" t="s">
         <v>11</v>
@@ -5817,10 +5826,10 @@
         <v>2</v>
       </c>
       <c r="F74" s="9" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="G74" s="9" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="H74" s="9" t="s">
         <v>11</v>
@@ -5837,13 +5846,13 @@
     </row>
     <row r="75" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="9" t="s">
-        <v>29</v>
+        <v>492</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>275</v>
-      </c>
-      <c r="C75" s="9" t="s">
-        <v>280</v>
+        <v>677</v>
+      </c>
+      <c r="C75" s="6" t="s">
+        <v>96</v>
       </c>
       <c r="D75" s="9" t="s">
         <v>14</v>
@@ -5852,10 +5861,10 @@
         <v>2</v>
       </c>
       <c r="F75" s="9" t="s">
-        <v>527</v>
-      </c>
-      <c r="G75" s="9" t="s">
-        <v>546</v>
+        <v>524</v>
+      </c>
+      <c r="G75" t="s">
+        <v>537</v>
       </c>
       <c r="H75" s="9" t="s">
         <v>11</v>
@@ -5872,13 +5881,13 @@
     </row>
     <row r="76" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="9" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D76" s="9" t="s">
         <v>14</v>
@@ -5887,10 +5896,10 @@
         <v>2</v>
       </c>
       <c r="F76" s="9" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="G76" s="9" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="H76" s="9" t="s">
         <v>11</v>
@@ -5907,13 +5916,13 @@
     </row>
     <row r="77" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="9" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="D77" s="9" t="s">
         <v>14</v>
@@ -5922,10 +5931,10 @@
         <v>2</v>
       </c>
       <c r="F77" s="9" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="G77" s="9" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="H77" s="9" t="s">
         <v>11</v>
@@ -5940,15 +5949,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="78" spans="1:11" ht="17" x14ac:dyDescent="0.2">
-      <c r="A78" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B78" s="7" t="s">
-        <v>270</v>
-      </c>
-      <c r="C78" s="6" t="s">
-        <v>266</v>
+    <row r="78" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A78" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B78" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="C78" s="9" t="s">
+        <v>281</v>
       </c>
       <c r="D78" s="9" t="s">
         <v>14</v>
@@ -5957,10 +5966,10 @@
         <v>2</v>
       </c>
       <c r="F78" s="9" t="s">
-        <v>549</v>
+        <v>523</v>
       </c>
       <c r="G78" s="9" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
       <c r="H78" s="9" t="s">
         <v>11</v>
@@ -5979,11 +5988,11 @@
       <c r="A79" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B79" s="9" t="s">
-        <v>271</v>
+      <c r="B79" s="7" t="s">
+        <v>270</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D79" s="9" t="s">
         <v>14</v>
@@ -5992,10 +6001,10 @@
         <v>2</v>
       </c>
       <c r="F79" s="9" t="s">
-        <v>550</v>
+        <v>545</v>
       </c>
       <c r="G79" s="9" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="H79" s="9" t="s">
         <v>11</v>
@@ -6011,14 +6020,14 @@
       </c>
     </row>
     <row r="80" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="9" t="s">
-        <v>43</v>
+      <c r="A80" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>384</v>
+        <v>271</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>101</v>
+        <v>267</v>
       </c>
       <c r="D80" s="9" t="s">
         <v>14</v>
@@ -6027,10 +6036,10 @@
         <v>2</v>
       </c>
       <c r="F80" s="9" t="s">
-        <v>527</v>
+        <v>546</v>
       </c>
       <c r="G80" s="9" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="H80" s="9" t="s">
         <v>11</v>
@@ -6047,13 +6056,13 @@
     </row>
     <row r="81" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="9" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>609</v>
+        <v>380</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>610</v>
+        <v>101</v>
       </c>
       <c r="D81" s="9" t="s">
         <v>14</v>
@@ -6061,11 +6070,11 @@
       <c r="E81" s="9">
         <v>2</v>
       </c>
-      <c r="F81" s="30" t="s">
-        <v>611</v>
+      <c r="F81" s="9" t="s">
+        <v>523</v>
       </c>
       <c r="G81" s="9" t="s">
-        <v>612</v>
+        <v>542</v>
       </c>
       <c r="H81" s="9" t="s">
         <v>11</v>
@@ -6082,37 +6091,37 @@
     </row>
     <row r="82" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="9" t="s">
-        <v>613</v>
+        <v>42</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>606</v>
+        <v>382</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>607</v>
+        <v>100</v>
       </c>
       <c r="D82" s="9" t="s">
-        <v>333</v>
+        <v>269</v>
       </c>
       <c r="E82" s="9">
         <v>3</v>
       </c>
       <c r="F82" s="9" t="s">
-        <v>528</v>
+        <v>11</v>
       </c>
       <c r="G82" s="9" t="s">
         <v>11</v>
       </c>
       <c r="H82" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="I82" s="9" t="s">
-        <v>11</v>
+        <v>385</v>
+      </c>
+      <c r="I82" s="9">
+        <v>0</v>
       </c>
       <c r="J82" s="9" t="s">
-        <v>11</v>
+        <v>383</v>
       </c>
       <c r="K82" s="9" t="s">
-        <v>614</v>
+        <v>11</v>
       </c>
     </row>
     <row r="83" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -6120,7 +6129,7 @@
         <v>59</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="C83" s="6" t="s">
         <v>117</v>
@@ -6138,13 +6147,13 @@
         <v>11</v>
       </c>
       <c r="H83" s="9" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="I83" s="9">
         <v>0</v>
       </c>
       <c r="J83" s="9" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="K83" s="9" t="s">
         <v>11</v>
@@ -6152,118 +6161,118 @@
     </row>
     <row r="84" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="9" t="s">
-        <v>42</v>
+        <v>599</v>
       </c>
       <c r="B84" s="9" t="s">
-        <v>386</v>
+        <v>592</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>100</v>
+        <v>593</v>
       </c>
       <c r="D84" s="9" t="s">
-        <v>269</v>
+        <v>333</v>
       </c>
       <c r="E84" s="9">
         <v>3</v>
       </c>
       <c r="F84" s="9" t="s">
-        <v>11</v>
+        <v>524</v>
       </c>
       <c r="G84" s="9" t="s">
         <v>11</v>
       </c>
       <c r="H84" s="9" t="s">
-        <v>389</v>
-      </c>
-      <c r="I84" s="9">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="I84" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="J84" s="9" t="s">
-        <v>387</v>
+        <v>11</v>
       </c>
       <c r="K84" s="9" t="s">
-        <v>11</v>
+        <v>600</v>
       </c>
     </row>
     <row r="85" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="9" t="s">
-        <v>30</v>
+      <c r="A85" s="7" t="s">
+        <v>268</v>
       </c>
       <c r="B85" s="9" t="s">
-        <v>328</v>
+        <v>272</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>88</v>
+        <v>403</v>
       </c>
       <c r="D85" s="9" t="s">
-        <v>269</v>
+        <v>333</v>
       </c>
       <c r="E85" s="9">
         <v>3</v>
       </c>
       <c r="F85" s="9" t="s">
-        <v>11</v>
+        <v>525</v>
       </c>
       <c r="G85" s="9" t="s">
         <v>11</v>
       </c>
       <c r="H85" s="9" t="s">
-        <v>285</v>
-      </c>
-      <c r="I85" s="9">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="I85" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="J85" s="9" t="s">
-        <v>286</v>
+        <v>11</v>
       </c>
       <c r="K85" s="9" t="s">
-        <v>11</v>
+        <v>551</v>
       </c>
     </row>
     <row r="86" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="9" t="s">
-        <v>31</v>
+      <c r="A86" s="7" t="s">
+        <v>268</v>
       </c>
       <c r="B86" s="9" t="s">
-        <v>329</v>
+        <v>273</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>89</v>
+        <v>402</v>
       </c>
       <c r="D86" s="9" t="s">
-        <v>269</v>
+        <v>333</v>
       </c>
       <c r="E86" s="9">
         <v>3</v>
       </c>
       <c r="F86" s="9" t="s">
-        <v>11</v>
+        <v>550</v>
       </c>
       <c r="G86" s="9" t="s">
         <v>11</v>
       </c>
       <c r="H86" s="9" t="s">
-        <v>285</v>
-      </c>
-      <c r="I86" s="9">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="I86" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="J86" s="9" t="s">
-        <v>287</v>
+        <v>11</v>
       </c>
       <c r="K86" s="9" t="s">
-        <v>11</v>
+        <v>549</v>
       </c>
     </row>
     <row r="87" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="9" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>379</v>
+        <v>575</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>120</v>
+        <v>236</v>
       </c>
       <c r="D87" s="9" t="s">
         <v>269</v>
@@ -6272,68 +6281,68 @@
         <v>3</v>
       </c>
       <c r="F87" s="9" t="s">
-        <v>11</v>
+        <v>576</v>
       </c>
       <c r="G87" s="9" t="s">
         <v>11</v>
       </c>
       <c r="H87" s="9" t="s">
-        <v>498</v>
+        <v>285</v>
       </c>
       <c r="I87" s="9">
         <v>0</v>
       </c>
       <c r="J87" s="9" t="s">
-        <v>380</v>
+        <v>574</v>
       </c>
       <c r="K87" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="88" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="9" t="s">
-        <v>54</v>
+      <c r="A88" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="B88" s="9" t="s">
-        <v>368</v>
+        <v>562</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>111</v>
+        <v>563</v>
       </c>
       <c r="D88" s="9" t="s">
-        <v>269</v>
+        <v>333</v>
       </c>
       <c r="E88" s="9">
         <v>3</v>
       </c>
       <c r="F88" s="9" t="s">
-        <v>11</v>
+        <v>564</v>
       </c>
       <c r="G88" s="9" t="s">
         <v>11</v>
       </c>
       <c r="H88" s="9" t="s">
-        <v>373</v>
-      </c>
-      <c r="I88" s="9">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="I88" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="J88" s="9" t="s">
-        <v>617</v>
+        <v>11</v>
       </c>
       <c r="K88" s="9" t="s">
-        <v>11</v>
+        <v>565</v>
       </c>
     </row>
     <row r="89" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="9" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B89" s="9" t="s">
-        <v>589</v>
+        <v>328</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>236</v>
+        <v>88</v>
       </c>
       <c r="D89" s="9" t="s">
         <v>269</v>
@@ -6342,7 +6351,7 @@
         <v>3</v>
       </c>
       <c r="F89" s="9" t="s">
-        <v>590</v>
+        <v>11</v>
       </c>
       <c r="G89" s="9" t="s">
         <v>11</v>
@@ -6354,7 +6363,7 @@
         <v>0</v>
       </c>
       <c r="J89" s="9" t="s">
-        <v>588</v>
+        <v>286</v>
       </c>
       <c r="K89" s="9" t="s">
         <v>11</v>
@@ -6362,13 +6371,13 @@
     </row>
     <row r="90" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="9" t="s">
-        <v>245</v>
+        <v>31</v>
       </c>
       <c r="B90" s="9" t="s">
-        <v>599</v>
+        <v>329</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>600</v>
+        <v>89</v>
       </c>
       <c r="D90" s="9" t="s">
         <v>269</v>
@@ -6377,19 +6386,19 @@
         <v>3</v>
       </c>
       <c r="F90" s="9" t="s">
-        <v>590</v>
+        <v>11</v>
       </c>
       <c r="G90" s="9" t="s">
         <v>11</v>
       </c>
       <c r="H90" s="9" t="s">
-        <v>373</v>
+        <v>285</v>
       </c>
       <c r="I90" s="9">
         <v>0</v>
       </c>
       <c r="J90" s="9" t="s">
-        <v>616</v>
+        <v>287</v>
       </c>
       <c r="K90" s="9" t="s">
         <v>11</v>
@@ -6397,13 +6406,13 @@
     </row>
     <row r="91" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="9" t="s">
-        <v>244</v>
+        <v>62</v>
       </c>
       <c r="B91" s="9" t="s">
-        <v>603</v>
+        <v>375</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>604</v>
+        <v>120</v>
       </c>
       <c r="D91" s="9" t="s">
         <v>269</v>
@@ -6412,128 +6421,128 @@
         <v>3</v>
       </c>
       <c r="F91" s="9" t="s">
-        <v>590</v>
+        <v>11</v>
       </c>
       <c r="G91" s="9" t="s">
         <v>11</v>
       </c>
       <c r="H91" s="9" t="s">
-        <v>605</v>
+        <v>494</v>
       </c>
       <c r="I91" s="9">
         <v>0</v>
       </c>
       <c r="J91" s="9" t="s">
-        <v>618</v>
+        <v>376</v>
       </c>
       <c r="K91" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="92" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="7" t="s">
-        <v>268</v>
+      <c r="A92" s="9" t="s">
+        <v>245</v>
       </c>
       <c r="B92" s="9" t="s">
-        <v>272</v>
+        <v>585</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>407</v>
+        <v>586</v>
       </c>
       <c r="D92" s="9" t="s">
-        <v>333</v>
+        <v>269</v>
       </c>
       <c r="E92" s="9">
         <v>3</v>
       </c>
       <c r="F92" s="9" t="s">
-        <v>529</v>
+        <v>576</v>
       </c>
       <c r="G92" s="9" t="s">
         <v>11</v>
       </c>
       <c r="H92" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="I92" s="9" t="s">
-        <v>11</v>
+        <v>369</v>
+      </c>
+      <c r="I92" s="9">
+        <v>0</v>
       </c>
       <c r="J92" s="9" t="s">
-        <v>11</v>
+        <v>602</v>
       </c>
       <c r="K92" s="9" t="s">
-        <v>556</v>
+        <v>11</v>
       </c>
       <c r="L92" s="29"/>
     </row>
     <row r="93" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="7" t="s">
-        <v>268</v>
+      <c r="A93" s="9" t="s">
+        <v>54</v>
       </c>
       <c r="B93" s="9" t="s">
-        <v>273</v>
+        <v>364</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>406</v>
+        <v>111</v>
       </c>
       <c r="D93" s="9" t="s">
-        <v>333</v>
+        <v>269</v>
       </c>
       <c r="E93" s="9">
         <v>3</v>
       </c>
       <c r="F93" s="9" t="s">
-        <v>555</v>
+        <v>11</v>
       </c>
       <c r="G93" s="9" t="s">
         <v>11</v>
       </c>
       <c r="H93" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="I93" s="9" t="s">
-        <v>11</v>
+        <v>369</v>
+      </c>
+      <c r="I93" s="9">
+        <v>0</v>
       </c>
       <c r="J93" s="9" t="s">
-        <v>11</v>
+        <v>603</v>
       </c>
       <c r="K93" s="9" t="s">
-        <v>554</v>
+        <v>11</v>
       </c>
     </row>
     <row r="94" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="7" t="s">
-        <v>17</v>
+      <c r="A94" s="9" t="s">
+        <v>244</v>
       </c>
       <c r="B94" s="9" t="s">
-        <v>572</v>
+        <v>589</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>573</v>
+        <v>590</v>
       </c>
       <c r="D94" s="9" t="s">
-        <v>333</v>
+        <v>269</v>
       </c>
       <c r="E94" s="9">
         <v>3</v>
       </c>
       <c r="F94" s="9" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
       <c r="G94" s="9" t="s">
         <v>11</v>
       </c>
       <c r="H94" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="I94" s="9" t="s">
-        <v>11</v>
+        <v>591</v>
+      </c>
+      <c r="I94" s="9">
+        <v>0</v>
       </c>
       <c r="J94" s="9" t="s">
-        <v>11</v>
+        <v>604</v>
       </c>
       <c r="K94" s="9" t="s">
-        <v>575</v>
+        <v>11</v>
       </c>
     </row>
     <row r="95" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -6541,7 +6550,7 @@
         <v>53</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="C95" s="6" t="s">
         <v>109</v>
@@ -6559,13 +6568,13 @@
         <v>11</v>
       </c>
       <c r="H95" s="9" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="I95" s="9">
         <v>0</v>
       </c>
       <c r="J95" s="9" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="K95" s="9" t="s">
         <v>11</v>
@@ -6576,7 +6585,7 @@
         <v>56</v>
       </c>
       <c r="B96" s="9" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="C96" s="6" t="s">
         <v>114</v>
@@ -6594,13 +6603,13 @@
         <v>11</v>
       </c>
       <c r="H96" s="9" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="I96" s="9">
         <v>0</v>
       </c>
       <c r="J96" s="9" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="K96" s="9" t="s">
         <v>11</v>
@@ -6608,13 +6617,13 @@
     </row>
     <row r="97" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="29" t="s">
-        <v>591</v>
+        <v>577</v>
       </c>
       <c r="B97" s="29" t="s">
-        <v>601</v>
+        <v>587</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>602</v>
+        <v>588</v>
       </c>
       <c r="D97" s="29" t="s">
         <v>269</v>
@@ -6623,19 +6632,19 @@
         <v>4</v>
       </c>
       <c r="F97" s="29" t="s">
-        <v>590</v>
+        <v>576</v>
       </c>
       <c r="G97" s="29" t="s">
         <v>11</v>
       </c>
       <c r="H97" s="29" t="s">
-        <v>608</v>
+        <v>594</v>
       </c>
       <c r="I97" s="29">
         <v>0</v>
       </c>
       <c r="J97" s="29" t="s">
-        <v>615</v>
+        <v>601</v>
       </c>
       <c r="K97" s="29" t="s">
         <v>11</v>
@@ -6643,13 +6652,13 @@
     </row>
     <row r="98" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="9" t="s">
-        <v>374</v>
+        <v>382</v>
       </c>
       <c r="B98" s="9" t="s">
-        <v>375</v>
+        <v>384</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="D98" s="9" t="s">
         <v>14</v>
@@ -6658,10 +6667,10 @@
         <v>4</v>
       </c>
       <c r="F98" s="7" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="G98" s="9" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="H98" s="9" t="s">
         <v>11</v>
@@ -6678,13 +6687,13 @@
     </row>
     <row r="99" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="9" t="s">
-        <v>386</v>
+        <v>370</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>388</v>
+        <v>371</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>100</v>
+        <v>117</v>
       </c>
       <c r="D99" s="9" t="s">
         <v>14</v>
@@ -6693,10 +6702,10 @@
         <v>4</v>
       </c>
       <c r="F99" s="7" t="s">
-        <v>531</v>
+        <v>526</v>
       </c>
       <c r="G99" s="9" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="H99" s="9" t="s">
         <v>11</v>
@@ -6713,13 +6722,13 @@
     </row>
     <row r="100" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="9" t="s">
-        <v>328</v>
+        <v>366</v>
       </c>
       <c r="B100" s="9" t="s">
-        <v>336</v>
+        <v>367</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>88</v>
+        <v>114</v>
       </c>
       <c r="D100" s="9" t="s">
         <v>14</v>
@@ -6727,11 +6736,11 @@
       <c r="E100" s="9">
         <v>4</v>
       </c>
-      <c r="F100" s="9" t="s">
-        <v>528</v>
+      <c r="F100" s="7" t="s">
+        <v>534</v>
       </c>
       <c r="G100" s="9" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="H100" s="9" t="s">
         <v>11</v>
@@ -6748,13 +6757,13 @@
     </row>
     <row r="101" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="9" t="s">
-        <v>329</v>
+        <v>375</v>
       </c>
       <c r="B101" s="9" t="s">
-        <v>337</v>
+        <v>377</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>89</v>
+        <v>120</v>
       </c>
       <c r="D101" s="9" t="s">
         <v>14</v>
@@ -6762,11 +6771,11 @@
       <c r="E101" s="9">
         <v>4</v>
       </c>
-      <c r="F101" s="9" t="s">
-        <v>576</v>
+      <c r="F101" s="7" t="s">
+        <v>531</v>
       </c>
       <c r="G101" s="9" t="s">
-        <v>544</v>
+        <v>538</v>
       </c>
       <c r="H101" s="9" t="s">
         <v>11</v>
@@ -6783,13 +6792,13 @@
     </row>
     <row r="102" spans="1:11" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="9" t="s">
-        <v>379</v>
+        <v>364</v>
       </c>
       <c r="B102" s="9" t="s">
-        <v>381</v>
+        <v>365</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="D102" s="9" t="s">
         <v>14</v>
@@ -6798,10 +6807,10 @@
         <v>4</v>
       </c>
       <c r="F102" s="7" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="G102" s="9" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="H102" s="9" t="s">
         <v>11</v>
@@ -6818,13 +6827,13 @@
     </row>
     <row r="103" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="9" t="s">
-        <v>368</v>
+        <v>378</v>
       </c>
       <c r="B103" s="9" t="s">
-        <v>369</v>
+        <v>379</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D103" s="9" t="s">
         <v>14</v>
@@ -6833,10 +6842,10 @@
         <v>4</v>
       </c>
       <c r="F103" s="7" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="G103" s="9" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="H103" s="9" t="s">
         <v>11</v>
@@ -6851,15 +6860,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="104" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A104" s="9" t="s">
-        <v>382</v>
+        <v>328</v>
       </c>
       <c r="B104" s="9" t="s">
-        <v>383</v>
+        <v>336</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="D104" s="9" t="s">
         <v>14</v>
@@ -6867,11 +6876,11 @@
       <c r="E104" s="9">
         <v>4</v>
       </c>
-      <c r="F104" s="7" t="s">
-        <v>537</v>
+      <c r="F104" s="9" t="s">
+        <v>524</v>
       </c>
       <c r="G104" s="9" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="H104" s="9" t="s">
         <v>11</v>
@@ -6886,15 +6895,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="105" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A105" s="9" t="s">
-        <v>370</v>
+        <v>329</v>
       </c>
       <c r="B105" s="9" t="s">
-        <v>371</v>
+        <v>337</v>
       </c>
       <c r="C105" s="6" t="s">
-        <v>114</v>
+        <v>89</v>
       </c>
       <c r="D105" s="9" t="s">
         <v>14</v>
@@ -6902,11 +6911,11 @@
       <c r="E105" s="9">
         <v>4</v>
       </c>
-      <c r="F105" s="7" t="s">
-        <v>538</v>
+      <c r="F105" s="9" t="s">
+        <v>566</v>
       </c>
       <c r="G105" s="9" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="H105" s="9" t="s">
         <v>11</v>
@@ -6923,13 +6932,13 @@
     </row>
     <row r="106" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="29" t="s">
-        <v>601</v>
+        <v>587</v>
       </c>
       <c r="B106" s="29" t="s">
-        <v>619</v>
+        <v>605</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>620</v>
+        <v>606</v>
       </c>
       <c r="D106" s="29" t="s">
         <v>14</v>
@@ -6938,10 +6947,10 @@
         <v>5</v>
       </c>
       <c r="F106" s="29" t="s">
-        <v>621</v>
+        <v>607</v>
       </c>
       <c r="G106" s="29" t="s">
-        <v>622</v>
+        <v>608</v>
       </c>
       <c r="H106" s="29" t="s">
         <v>11</v>
@@ -6961,7 +6970,7 @@
         <v>340</v>
       </c>
       <c r="B107" s="9" t="s">
-        <v>355</v>
+        <v>679</v>
       </c>
       <c r="C107" s="6" t="s">
         <v>334</v>
@@ -6973,7 +6982,7 @@
         <v>5</v>
       </c>
       <c r="F107" s="9" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="G107" s="9" t="s">
         <v>11</v>
@@ -6988,39 +6997,39 @@
         <v>11</v>
       </c>
       <c r="K107" s="9" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="108" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A108" s="9" t="s">
-        <v>341</v>
+        <v>330</v>
       </c>
       <c r="B108" s="9" t="s">
-        <v>343</v>
-      </c>
-      <c r="C108" s="5" t="s">
-        <v>342</v>
+        <v>361</v>
+      </c>
+      <c r="C108" s="6" t="s">
+        <v>93</v>
       </c>
       <c r="D108" s="9" t="s">
-        <v>269</v>
+        <v>14</v>
       </c>
       <c r="E108" s="9">
         <v>6</v>
       </c>
-      <c r="F108" s="9" t="s">
-        <v>11</v>
+      <c r="F108" s="7" t="s">
+        <v>528</v>
       </c>
       <c r="G108" s="9" t="s">
-        <v>11</v>
+        <v>539</v>
       </c>
       <c r="H108" s="9" t="s">
-        <v>562</v>
-      </c>
-      <c r="I108" s="9">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="I108" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="J108" s="9" t="s">
-        <v>552</v>
+        <v>11</v>
       </c>
       <c r="K108" s="9" t="s">
         <v>11</v>
@@ -7028,48 +7037,48 @@
     </row>
     <row r="109" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A109" s="9" t="s">
-        <v>349</v>
+        <v>332</v>
       </c>
       <c r="B109" s="9" t="s">
-        <v>330</v>
+        <v>360</v>
       </c>
       <c r="C109" s="6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D109" s="9" t="s">
-        <v>269</v>
+        <v>14</v>
       </c>
       <c r="E109" s="9">
         <v>6</v>
       </c>
       <c r="F109" s="9" t="s">
-        <v>11</v>
+        <v>529</v>
       </c>
       <c r="G109" s="9" t="s">
-        <v>11</v>
+        <v>541</v>
       </c>
       <c r="H109" s="9" t="s">
-        <v>562</v>
-      </c>
-      <c r="I109" s="9">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="I109" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="J109" s="9" t="s">
-        <v>551</v>
+        <v>11</v>
       </c>
       <c r="K109" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="110" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A110" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B110" s="9" t="s">
-        <v>332</v>
+        <v>675</v>
       </c>
       <c r="C110" s="6" t="s">
-        <v>94</v>
+        <v>667</v>
       </c>
       <c r="D110" s="9" t="s">
         <v>269</v>
@@ -7078,33 +7087,31 @@
         <v>6</v>
       </c>
       <c r="F110" s="9" t="s">
-        <v>11</v>
+        <v>676</v>
       </c>
       <c r="G110" s="9" t="s">
         <v>11</v>
       </c>
       <c r="H110" s="9" t="s">
-        <v>562</v>
+        <v>684</v>
       </c>
       <c r="I110" s="9">
         <v>0</v>
       </c>
       <c r="J110" s="9" t="s">
-        <v>290</v>
-      </c>
-      <c r="K110" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="111" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+        <v>555</v>
+      </c>
+      <c r="K110" s="9"/>
+    </row>
+    <row r="111" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A111" s="9" t="s">
-        <v>32</v>
+        <v>341</v>
       </c>
       <c r="B111" s="9" t="s">
-        <v>335</v>
-      </c>
-      <c r="C111" s="6" t="s">
-        <v>90</v>
+        <v>343</v>
+      </c>
+      <c r="C111" s="5" t="s">
+        <v>342</v>
       </c>
       <c r="D111" s="9" t="s">
         <v>269</v>
@@ -7119,13 +7126,13 @@
         <v>11</v>
       </c>
       <c r="H111" s="9" t="s">
-        <v>562</v>
+        <v>684</v>
       </c>
       <c r="I111" s="9">
         <v>0</v>
       </c>
       <c r="J111" s="9" t="s">
-        <v>288</v>
+        <v>548</v>
       </c>
       <c r="K111" s="9" t="s">
         <v>11</v>
@@ -7133,13 +7140,13 @@
     </row>
     <row r="112" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A112" s="9" t="s">
-        <v>33</v>
+        <v>349</v>
       </c>
       <c r="B112" s="9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D112" s="9" t="s">
         <v>269</v>
@@ -7154,27 +7161,27 @@
         <v>11</v>
       </c>
       <c r="H112" s="9" t="s">
-        <v>562</v>
+        <v>684</v>
       </c>
       <c r="I112" s="9">
         <v>0</v>
       </c>
       <c r="J112" s="9" t="s">
-        <v>289</v>
+        <v>547</v>
       </c>
       <c r="K112" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="113" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A113" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B113" s="9" t="s">
-        <v>565</v>
+        <v>332</v>
       </c>
       <c r="C113" s="6" t="s">
-        <v>563</v>
+        <v>94</v>
       </c>
       <c r="D113" s="9" t="s">
         <v>269</v>
@@ -7183,52 +7190,54 @@
         <v>6</v>
       </c>
       <c r="F113" s="9" t="s">
-        <v>677</v>
+        <v>11</v>
       </c>
       <c r="G113" s="9" t="s">
         <v>11</v>
       </c>
       <c r="H113" s="9" t="s">
-        <v>562</v>
+        <v>684</v>
       </c>
       <c r="I113" s="9">
         <v>0</v>
       </c>
       <c r="J113" s="9" t="s">
-        <v>564</v>
-      </c>
-      <c r="K113" s="9"/>
+        <v>290</v>
+      </c>
+      <c r="K113" s="9" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="114" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A114" s="9" t="s">
-        <v>330</v>
+        <v>32</v>
       </c>
       <c r="B114" s="9" t="s">
-        <v>365</v>
+        <v>335</v>
       </c>
       <c r="C114" s="6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D114" s="9" t="s">
-        <v>14</v>
+        <v>269</v>
       </c>
       <c r="E114" s="9">
         <v>6</v>
       </c>
-      <c r="F114" s="7" t="s">
-        <v>532</v>
+      <c r="F114" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="G114" s="9" t="s">
-        <v>543</v>
+        <v>11</v>
       </c>
       <c r="H114" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="I114" s="9" t="s">
-        <v>11</v>
+        <v>684</v>
+      </c>
+      <c r="I114" s="9">
+        <v>0</v>
       </c>
       <c r="J114" s="9" t="s">
-        <v>11</v>
+        <v>288</v>
       </c>
       <c r="K114" s="9" t="s">
         <v>11</v>
@@ -7236,13 +7245,13 @@
     </row>
     <row r="115" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A115" s="9" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="B115" s="9" t="s">
-        <v>364</v>
+        <v>338</v>
       </c>
       <c r="C115" s="6" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D115" s="9" t="s">
         <v>14</v>
@@ -7251,10 +7260,10 @@
         <v>6</v>
       </c>
       <c r="F115" s="9" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="G115" s="9" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="H115" s="9" t="s">
         <v>11</v>
@@ -7271,34 +7280,34 @@
     </row>
     <row r="116" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="9" t="s">
-        <v>335</v>
+        <v>33</v>
       </c>
       <c r="B116" s="9" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="C116" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D116" s="9" t="s">
-        <v>14</v>
+        <v>269</v>
       </c>
       <c r="E116" s="9">
         <v>6</v>
       </c>
       <c r="F116" s="9" t="s">
-        <v>534</v>
+        <v>11</v>
       </c>
       <c r="G116" s="9" t="s">
-        <v>544</v>
+        <v>11</v>
       </c>
       <c r="H116" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="I116" s="9" t="s">
-        <v>11</v>
+        <v>684</v>
+      </c>
+      <c r="I116" s="9">
+        <v>0</v>
       </c>
       <c r="J116" s="9" t="s">
-        <v>11</v>
+        <v>289</v>
       </c>
       <c r="K116" s="9" t="s">
         <v>11</v>
@@ -7321,10 +7330,10 @@
         <v>6</v>
       </c>
       <c r="F117" s="9" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="G117" s="9" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="H117" s="9" t="s">
         <v>11</v>
@@ -7340,12 +7349,14 @@
       </c>
     </row>
     <row r="118" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="9"/>
+      <c r="A118" s="9" t="s">
+        <v>362</v>
+      </c>
       <c r="B118" s="9" t="s">
-        <v>676</v>
+        <v>358</v>
       </c>
       <c r="C118" s="6" t="s">
-        <v>563</v>
+        <v>351</v>
       </c>
       <c r="D118" s="9" t="s">
         <v>333</v>
@@ -7354,7 +7365,7 @@
         <v>7</v>
       </c>
       <c r="F118" s="9" t="s">
-        <v>621</v>
+        <v>524</v>
       </c>
       <c r="G118" s="9" t="s">
         <v>11</v>
@@ -7369,30 +7380,28 @@
         <v>11</v>
       </c>
       <c r="K118" s="9" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="119" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A119" s="9" t="s">
-        <v>343</v>
-      </c>
+        <v>680</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A119" s="9"/>
       <c r="B119" s="9" t="s">
-        <v>344</v>
-      </c>
-      <c r="C119" s="5" t="s">
-        <v>342</v>
+        <v>659</v>
+      </c>
+      <c r="C119" s="6" t="s">
+        <v>554</v>
       </c>
       <c r="D119" s="9" t="s">
-        <v>14</v>
+        <v>333</v>
       </c>
       <c r="E119" s="9">
         <v>7</v>
       </c>
       <c r="F119" s="9" t="s">
-        <v>528</v>
+        <v>607</v>
       </c>
       <c r="G119" s="9" t="s">
-        <v>544</v>
+        <v>11</v>
       </c>
       <c r="H119" s="9" t="s">
         <v>11</v>
@@ -7404,27 +7413,27 @@
         <v>11</v>
       </c>
       <c r="K119" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="120" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="9" t="s">
         <v>345</v>
       </c>
       <c r="B120" s="9" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C120" s="6" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D120" s="9" t="s">
-        <v>311</v>
+        <v>333</v>
       </c>
       <c r="E120" s="9">
         <v>7</v>
       </c>
       <c r="F120" s="9" t="s">
-        <v>11</v>
+        <v>524</v>
       </c>
       <c r="G120" s="9" t="s">
         <v>11</v>
@@ -7439,27 +7448,27 @@
         <v>11</v>
       </c>
       <c r="K120" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="121" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="9" t="s">
-        <v>366</v>
+        <v>345</v>
       </c>
       <c r="B121" s="9" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="C121" s="6" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D121" s="9" t="s">
-        <v>333</v>
+        <v>311</v>
       </c>
       <c r="E121" s="9">
         <v>7</v>
       </c>
       <c r="F121" s="9" t="s">
-        <v>528</v>
+        <v>11</v>
       </c>
       <c r="G121" s="9" t="s">
         <v>11</v>
@@ -7474,18 +7483,16 @@
         <v>11</v>
       </c>
       <c r="K121" s="9" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="122" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="9" t="s">
-        <v>345</v>
-      </c>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A122" s="9"/>
       <c r="B122" s="9" t="s">
-        <v>361</v>
+        <v>681</v>
       </c>
       <c r="C122" s="6" t="s">
-        <v>346</v>
+        <v>668</v>
       </c>
       <c r="D122" s="9" t="s">
         <v>333</v>
@@ -7494,7 +7501,7 @@
         <v>7</v>
       </c>
       <c r="F122" s="9" t="s">
-        <v>528</v>
+        <v>607</v>
       </c>
       <c r="G122" s="9" t="s">
         <v>11</v>
@@ -7509,30 +7516,30 @@
         <v>11</v>
       </c>
       <c r="K122" s="9" t="s">
-        <v>347</v>
+        <v>686</v>
       </c>
     </row>
     <row r="123" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="9" t="s">
-        <v>367</v>
+        <v>343</v>
       </c>
       <c r="B123" s="9" t="s">
-        <v>358</v>
-      </c>
-      <c r="C123" s="6" t="s">
-        <v>350</v>
+        <v>344</v>
+      </c>
+      <c r="C123" s="5" t="s">
+        <v>342</v>
       </c>
       <c r="D123" s="9" t="s">
-        <v>333</v>
+        <v>14</v>
       </c>
       <c r="E123" s="9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F123" s="9" t="s">
-        <v>11</v>
+        <v>524</v>
       </c>
       <c r="G123" s="9" t="s">
-        <v>11</v>
+        <v>540</v>
       </c>
       <c r="H123" s="9" t="s">
         <v>11</v>
@@ -7544,18 +7551,18 @@
         <v>11</v>
       </c>
       <c r="K123" s="9" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="124" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="9" t="s">
-        <v>29</v>
+        <v>275</v>
       </c>
       <c r="B124" s="9" t="s">
-        <v>557</v>
+        <v>682</v>
       </c>
       <c r="C124" s="9" t="s">
-        <v>558</v>
+        <v>552</v>
       </c>
       <c r="D124" s="9" t="s">
         <v>14</v>
@@ -7564,10 +7571,10 @@
         <v>8</v>
       </c>
       <c r="F124" s="9" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="G124" s="9" t="s">
-        <v>559</v>
+        <v>671</v>
       </c>
       <c r="H124" s="9" t="s">
         <v>11</v>
@@ -7582,27 +7589,25 @@
         <v>11</v>
       </c>
     </row>
-    <row r="125" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A125" s="9" t="s">
-        <v>578</v>
+        <v>275</v>
       </c>
       <c r="B125" s="9" t="s">
-        <v>579</v>
-      </c>
-      <c r="C125" s="6" t="s">
-        <v>577</v>
-      </c>
+        <v>683</v>
+      </c>
+      <c r="C125" s="6"/>
       <c r="D125" s="9" t="s">
-        <v>333</v>
+        <v>14</v>
       </c>
       <c r="E125" s="9">
         <v>8</v>
       </c>
       <c r="F125" s="9" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="G125" s="9" t="s">
-        <v>11</v>
+        <v>672</v>
       </c>
       <c r="H125" s="9" t="s">
         <v>11</v>
@@ -7614,27 +7619,27 @@
         <v>11</v>
       </c>
       <c r="K125" s="9" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="126" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A126" s="9" t="s">
-        <v>366</v>
+        <v>568</v>
       </c>
       <c r="B126" s="9" t="s">
-        <v>581</v>
+        <v>673</v>
       </c>
       <c r="C126" s="6" t="s">
-        <v>583</v>
+        <v>567</v>
       </c>
       <c r="D126" s="9" t="s">
         <v>333</v>
       </c>
       <c r="E126" s="9">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F126" s="9" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="G126" s="9" t="s">
         <v>11</v>
@@ -7649,7 +7654,7 @@
         <v>11</v>
       </c>
       <c r="K126" s="9" t="s">
-        <v>582</v>
+        <v>569</v>
       </c>
     </row>
     <row r="127" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
@@ -7657,16 +7662,16 @@
         <v>363</v>
       </c>
       <c r="B127" s="9" t="s">
-        <v>359</v>
+        <v>678</v>
       </c>
       <c r="C127" s="6" t="s">
-        <v>526</v>
+        <v>350</v>
       </c>
       <c r="D127" s="9" t="s">
         <v>333</v>
       </c>
       <c r="E127" s="9">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F127" s="9" t="s">
         <v>11</v>
@@ -7684,27 +7689,27 @@
         <v>11</v>
       </c>
       <c r="K127" s="9" t="s">
-        <v>584</v>
+        <v>669</v>
       </c>
     </row>
     <row r="128" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="9" t="s">
-        <v>356</v>
+        <v>362</v>
       </c>
       <c r="B128" s="9" t="s">
-        <v>587</v>
+        <v>570</v>
       </c>
       <c r="C128" s="6" t="s">
-        <v>585</v>
+        <v>571</v>
       </c>
       <c r="D128" s="9" t="s">
         <v>333</v>
       </c>
       <c r="E128" s="9">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F128" s="9" t="s">
-        <v>11</v>
+        <v>524</v>
       </c>
       <c r="G128" s="9" t="s">
         <v>11</v>
@@ -7719,18 +7724,18 @@
         <v>11</v>
       </c>
       <c r="K128" s="9" t="s">
-        <v>586</v>
+        <v>688</v>
       </c>
     </row>
     <row r="129" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="9" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B129" s="9" t="s">
-        <v>624</v>
+        <v>670</v>
       </c>
       <c r="C129" s="6" t="s">
-        <v>625</v>
+        <v>573</v>
       </c>
       <c r="D129" s="9" t="s">
         <v>333</v>
@@ -7754,11 +7759,43 @@
         <v>11</v>
       </c>
       <c r="K129" s="9" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="137" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="B137" s="9"/>
+        <v>687</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A130" s="9" t="s">
+        <v>359</v>
+      </c>
+      <c r="B130" s="9" t="s">
+        <v>674</v>
+      </c>
+      <c r="C130" s="6" t="s">
+        <v>522</v>
+      </c>
+      <c r="D130" s="9" t="s">
+        <v>333</v>
+      </c>
+      <c r="E130" s="9">
+        <v>10</v>
+      </c>
+      <c r="F130" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G130" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H130" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I130" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J130" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K130" s="9" t="s">
+        <v>572</v>
+      </c>
     </row>
     <row r="138" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="B138" s="9"/>
@@ -7775,9 +7812,12 @@
     <row r="142" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="B142" s="9"/>
     </row>
+    <row r="143" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="B143" s="9"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K142">
-    <sortCondition ref="E108:E142"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K146">
+    <sortCondition ref="E14:E146"/>
   </sortState>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7855,7 +7895,7 @@
         <v>11</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>685</v>
+        <v>666</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>11</v>
@@ -7866,13 +7906,13 @@
     </row>
     <row r="3" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
@@ -7881,7 +7921,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="25" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
@@ -7901,13 +7941,13 @@
     </row>
     <row r="4" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="25" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
@@ -7916,7 +7956,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="25" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="G4" t="s">
         <v>11</v>
@@ -7936,13 +7976,13 @@
     </row>
     <row r="5" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
@@ -7951,7 +7991,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="25" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="G5" t="s">
         <v>11</v>
@@ -7971,13 +8011,13 @@
     </row>
     <row r="6" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
@@ -7986,7 +8026,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="25" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="G6" t="s">
         <v>11</v>
@@ -8006,13 +8046,13 @@
     </row>
     <row r="7" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="25" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="D7" t="s">
         <v>11</v>
@@ -8021,7 +8061,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="25" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="G7" t="s">
         <v>11</v>
@@ -8041,13 +8081,13 @@
     </row>
     <row r="8" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="25" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="D8" t="s">
         <v>11</v>
@@ -8056,7 +8096,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="25" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="G8" t="s">
         <v>11</v>
@@ -8076,13 +8116,13 @@
     </row>
     <row r="9" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -8091,7 +8131,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="25" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="G9" t="s">
         <v>11</v>
@@ -8111,13 +8151,13 @@
     </row>
     <row r="10" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="D10" t="s">
         <v>11</v>
@@ -8126,7 +8166,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="25" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="G10" t="s">
         <v>11</v>
@@ -8146,13 +8186,13 @@
     </row>
     <row r="11" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="25" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="D11" t="s">
         <v>11</v>
@@ -8161,7 +8201,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="25" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="G11" t="s">
         <v>11</v>
@@ -8181,13 +8221,13 @@
     </row>
     <row r="12" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="25" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="D12" t="s">
         <v>11</v>
@@ -8196,7 +8236,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="25" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="G12" t="s">
         <v>11</v>
@@ -8216,13 +8256,13 @@
     </row>
     <row r="13" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="25" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="D13" t="s">
         <v>11</v>
@@ -8231,7 +8271,7 @@
         <v>0</v>
       </c>
       <c r="F13" s="25" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="G13" t="s">
         <v>11</v>
@@ -8251,13 +8291,13 @@
     </row>
     <row r="14" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="25" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="D14" t="s">
         <v>11</v>
@@ -8266,7 +8306,7 @@
         <v>0</v>
       </c>
       <c r="F14" s="25" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="G14" t="s">
         <v>11</v>
@@ -8286,13 +8326,13 @@
     </row>
     <row r="15" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="25" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="B15" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="D15" t="s">
         <v>11</v>
@@ -8301,7 +8341,7 @@
         <v>0</v>
       </c>
       <c r="F15" s="25" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="G15" t="s">
         <v>11</v>
@@ -8321,13 +8361,13 @@
     </row>
     <row r="16" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="25" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="B16" t="s">
         <v>11</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D16" t="s">
         <v>11</v>
@@ -8336,7 +8376,7 @@
         <v>0</v>
       </c>
       <c r="F16" s="25" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="G16" t="s">
         <v>11</v>
@@ -8356,13 +8396,13 @@
     </row>
     <row r="17" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="25" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="B17" t="s">
         <v>11</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="D17" t="s">
         <v>11</v>
@@ -8371,7 +8411,7 @@
         <v>0</v>
       </c>
       <c r="F17" s="25" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="G17" t="s">
         <v>11</v>
@@ -8391,13 +8431,13 @@
     </row>
     <row r="18" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="25" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="B18" t="s">
         <v>11</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="D18" t="s">
         <v>11</v>
@@ -8406,7 +8446,7 @@
         <v>0</v>
       </c>
       <c r="F18" s="25" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="G18" t="s">
         <v>11</v>
@@ -8426,13 +8466,13 @@
     </row>
     <row r="19" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="25" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="B19" t="s">
         <v>11</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="D19" t="s">
         <v>11</v>
@@ -8441,7 +8481,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="25" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="G19" t="s">
         <v>11</v>
@@ -8461,13 +8501,13 @@
     </row>
     <row r="20" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="25" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B20" t="s">
         <v>11</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="D20" t="s">
         <v>11</v>
@@ -8476,7 +8516,7 @@
         <v>0</v>
       </c>
       <c r="F20" s="25" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="G20" t="s">
         <v>11</v>
@@ -8496,13 +8536,13 @@
     </row>
     <row r="21" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="25" t="s">
-        <v>679</v>
+        <v>660</v>
       </c>
       <c r="B21" t="s">
         <v>11</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="D21" t="s">
         <v>11</v>
@@ -8511,7 +8551,7 @@
         <v>0</v>
       </c>
       <c r="F21" s="25" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="G21" t="s">
         <v>11</v>
@@ -8567,13 +8607,13 @@
     </row>
     <row r="23" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="25" t="s">
-        <v>680</v>
+        <v>661</v>
       </c>
       <c r="B23" t="s">
-        <v>646</v>
+        <v>629</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>627</v>
+        <v>610</v>
       </c>
       <c r="D23" t="s">
         <v>311</v>
@@ -8602,13 +8642,13 @@
     </row>
     <row r="24" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="25" t="s">
-        <v>628</v>
+        <v>611</v>
       </c>
       <c r="B24" t="s">
-        <v>661</v>
+        <v>644</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>630</v>
+        <v>613</v>
       </c>
       <c r="D24" t="s">
         <v>311</v>
@@ -8637,13 +8677,13 @@
     </row>
     <row r="25" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="25" t="s">
-        <v>631</v>
+        <v>614</v>
       </c>
       <c r="B25" t="s">
-        <v>662</v>
+        <v>645</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>635</v>
+        <v>618</v>
       </c>
       <c r="D25" t="s">
         <v>311</v>
@@ -8672,13 +8712,13 @@
     </row>
     <row r="26" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="25" t="s">
-        <v>633</v>
+        <v>616</v>
       </c>
       <c r="B26" t="s">
-        <v>663</v>
+        <v>646</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>636</v>
+        <v>619</v>
       </c>
       <c r="D26" t="s">
         <v>311</v>
@@ -8707,13 +8747,13 @@
     </row>
     <row r="27" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>646</v>
+        <v>629</v>
       </c>
       <c r="B27" t="s">
-        <v>626</v>
+        <v>609</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>627</v>
+        <v>610</v>
       </c>
       <c r="D27" t="s">
         <v>269</v>
@@ -8726,13 +8766,13 @@
         <v>11</v>
       </c>
       <c r="H27" s="12" t="s">
-        <v>681</v>
+        <v>662</v>
       </c>
       <c r="I27" s="12" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="J27" s="12" t="s">
-        <v>682</v>
+        <v>663</v>
       </c>
       <c r="K27" s="2" t="s">
         <v>11</v>
@@ -8740,13 +8780,13 @@
     </row>
     <row r="28" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>661</v>
+        <v>644</v>
       </c>
       <c r="B28" t="s">
-        <v>629</v>
+        <v>612</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>630</v>
+        <v>613</v>
       </c>
       <c r="D28" t="s">
         <v>269</v>
@@ -8759,13 +8799,13 @@
         <v>11</v>
       </c>
       <c r="H28" s="12" t="s">
-        <v>666</v>
+        <v>649</v>
       </c>
       <c r="I28" s="12" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="J28" s="12" t="s">
-        <v>672</v>
+        <v>655</v>
       </c>
       <c r="K28" s="2" t="s">
         <v>11</v>
@@ -8773,13 +8813,13 @@
     </row>
     <row r="29" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>662</v>
+        <v>645</v>
       </c>
       <c r="B29" t="s">
-        <v>632</v>
+        <v>615</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>635</v>
+        <v>618</v>
       </c>
       <c r="D29" t="s">
         <v>269</v>
@@ -8792,13 +8832,13 @@
         <v>11</v>
       </c>
       <c r="H29" s="12" t="s">
-        <v>683</v>
+        <v>664</v>
       </c>
       <c r="I29" s="12" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="J29" s="12" t="s">
-        <v>671</v>
+        <v>654</v>
       </c>
       <c r="K29" s="2" t="s">
         <v>11</v>
@@ -8806,13 +8846,13 @@
     </row>
     <row r="30" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>663</v>
+        <v>646</v>
       </c>
       <c r="B30" t="s">
-        <v>634</v>
+        <v>617</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>636</v>
+        <v>619</v>
       </c>
       <c r="D30" t="s">
         <v>269</v>
@@ -8825,13 +8865,13 @@
         <v>11</v>
       </c>
       <c r="H30" s="12" t="s">
-        <v>665</v>
+        <v>648</v>
       </c>
       <c r="I30" s="12" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="J30" s="12" t="s">
-        <v>670</v>
+        <v>653</v>
       </c>
       <c r="K30" s="2" t="s">
         <v>11</v>
@@ -8839,13 +8879,13 @@
     </row>
     <row r="31" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="25" t="s">
-        <v>637</v>
+        <v>620</v>
       </c>
       <c r="B31" t="s">
-        <v>664</v>
+        <v>647</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>639</v>
+        <v>622</v>
       </c>
       <c r="D31" t="s">
         <v>311</v>
@@ -8874,13 +8914,13 @@
     </row>
     <row r="32" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="25" t="s">
-        <v>664</v>
+        <v>647</v>
       </c>
       <c r="B32" t="s">
-        <v>638</v>
+        <v>621</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>639</v>
+        <v>622</v>
       </c>
       <c r="D32" t="s">
         <v>269</v>
@@ -8895,13 +8935,13 @@
         <v>11</v>
       </c>
       <c r="H32" s="12" t="s">
-        <v>667</v>
+        <v>650</v>
       </c>
       <c r="I32" s="25" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="J32" s="12" t="s">
-        <v>669</v>
+        <v>652</v>
       </c>
       <c r="K32" s="25" t="s">
         <v>11</v>
@@ -8909,13 +8949,13 @@
     </row>
     <row r="33" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="25" t="s">
-        <v>638</v>
+        <v>621</v>
       </c>
       <c r="B33" t="s">
-        <v>656</v>
+        <v>639</v>
       </c>
       <c r="C33" s="25" t="s">
-        <v>658</v>
+        <v>641</v>
       </c>
       <c r="D33" t="s">
         <v>333</v>
@@ -8924,7 +8964,7 @@
         <v>6</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>11</v>
@@ -8939,18 +8979,18 @@
         <v>11</v>
       </c>
       <c r="K33" s="12" t="s">
-        <v>668</v>
+        <v>651</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="25" t="s">
-        <v>638</v>
+        <v>621</v>
       </c>
       <c r="B34" t="s">
-        <v>657</v>
+        <v>640</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>659</v>
+        <v>642</v>
       </c>
       <c r="D34" t="s">
         <v>333</v>
@@ -8959,7 +8999,7 @@
         <v>6</v>
       </c>
       <c r="F34" s="25" t="s">
-        <v>660</v>
+        <v>643</v>
       </c>
       <c r="G34" s="5" t="s">
         <v>11</v>
@@ -8974,7 +9014,7 @@
         <v>11</v>
       </c>
       <c r="K34" s="12" t="s">
-        <v>684</v>
+        <v>665</v>
       </c>
     </row>
   </sheetData>
@@ -9057,7 +9097,7 @@
         <v>11</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>685</v>
+        <v>666</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>11</v>
@@ -9068,13 +9108,13 @@
     </row>
     <row r="3" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
@@ -9083,7 +9123,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="25" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
@@ -9103,13 +9143,13 @@
     </row>
     <row r="4" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="25" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
@@ -9118,7 +9158,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="25" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="G4" t="s">
         <v>11</v>
@@ -9138,13 +9178,13 @@
     </row>
     <row r="5" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -9153,7 +9193,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="25" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="G5" t="s">
         <v>11</v>
@@ -9173,13 +9213,13 @@
     </row>
     <row r="6" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -9188,7 +9228,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="25" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="G6" t="s">
         <v>11</v>
@@ -9208,13 +9248,13 @@
     </row>
     <row r="7" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="25" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
@@ -9223,7 +9263,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="25" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="G7" t="s">
         <v>11</v>
@@ -9243,13 +9283,13 @@
     </row>
     <row r="8" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="25" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
@@ -9258,7 +9298,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="25" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="G8" t="s">
         <v>11</v>
@@ -9278,13 +9318,13 @@
     </row>
     <row r="9" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="D9" t="s">
         <v>12</v>
@@ -9293,7 +9333,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="25" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="G9" t="s">
         <v>11</v>
@@ -9313,13 +9353,13 @@
     </row>
     <row r="10" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -9328,7 +9368,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="25" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="G10" t="s">
         <v>11</v>
@@ -9348,13 +9388,13 @@
     </row>
     <row r="11" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="25" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
@@ -9363,7 +9403,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="25" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="G11" t="s">
         <v>11</v>
@@ -9383,13 +9423,13 @@
     </row>
     <row r="12" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="25" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="D12" t="s">
         <v>12</v>
@@ -9398,7 +9438,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="25" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="G12" t="s">
         <v>11</v>
@@ -9418,13 +9458,13 @@
     </row>
     <row r="13" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="25" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="D13" t="s">
         <v>12</v>
@@ -9433,7 +9473,7 @@
         <v>0</v>
       </c>
       <c r="F13" s="25" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="G13" t="s">
         <v>11</v>
@@ -9453,13 +9493,13 @@
     </row>
     <row r="14" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="25" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="D14" t="s">
         <v>12</v>
@@ -9468,7 +9508,7 @@
         <v>0</v>
       </c>
       <c r="F14" s="25" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="G14" t="s">
         <v>11</v>
@@ -9524,13 +9564,13 @@
     </row>
     <row r="16" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="25" t="s">
-        <v>642</v>
+        <v>625</v>
       </c>
       <c r="B16" t="s">
-        <v>647</v>
+        <v>630</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="D16" t="s">
         <v>311</v>
@@ -9559,13 +9599,13 @@
     </row>
     <row r="17" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="25" t="s">
-        <v>644</v>
+        <v>627</v>
       </c>
       <c r="B17" t="s">
-        <v>648</v>
+        <v>631</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="D17" t="s">
         <v>311</v>
@@ -9594,13 +9634,13 @@
     </row>
     <row r="18" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="25" t="s">
-        <v>645</v>
+        <v>628</v>
       </c>
       <c r="B18" t="s">
-        <v>649</v>
+        <v>632</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="D18" t="s">
         <v>311</v>
@@ -9629,13 +9669,13 @@
     </row>
     <row r="19" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>647</v>
+        <v>630</v>
       </c>
       <c r="B19" t="s">
-        <v>640</v>
+        <v>623</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>650</v>
+        <v>633</v>
       </c>
       <c r="D19" t="s">
         <v>269</v>
@@ -9650,13 +9690,13 @@
         <v>11</v>
       </c>
       <c r="H19" s="12" t="s">
-        <v>653</v>
+        <v>636</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="J19" s="12" t="s">
-        <v>673</v>
+        <v>656</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>11</v>
@@ -9664,13 +9704,13 @@
     </row>
     <row r="20" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>648</v>
+        <v>631</v>
       </c>
       <c r="B20" t="s">
-        <v>641</v>
+        <v>624</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>651</v>
+        <v>634</v>
       </c>
       <c r="D20" t="s">
         <v>269</v>
@@ -9685,13 +9725,13 @@
         <v>11</v>
       </c>
       <c r="H20" s="12" t="s">
-        <v>654</v>
+        <v>637</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="J20" s="12" t="s">
-        <v>674</v>
+        <v>657</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>11</v>
@@ -9699,13 +9739,13 @@
     </row>
     <row r="21" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>649</v>
+        <v>632</v>
       </c>
       <c r="B21" t="s">
-        <v>643</v>
+        <v>626</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>652</v>
+        <v>635</v>
       </c>
       <c r="D21" t="s">
         <v>269</v>
@@ -9720,13 +9760,13 @@
         <v>11</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>655</v>
+        <v>638</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="J21" s="12" t="s">
-        <v>675</v>
+        <v>658</v>
       </c>
       <c r="K21" s="2" t="s">
         <v>11</v>
@@ -9741,7 +9781,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A674610-18BE-F241-9D23-4CA806F45B9D}">
   <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A33" workbookViewId="0">
       <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
@@ -10806,7 +10846,7 @@
     </row>
     <row r="31" spans="1:11" s="19" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="22" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="B31" s="19" t="s">
         <v>11</v>
@@ -10841,16 +10881,16 @@
     </row>
     <row r="32" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="B32" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="D32" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="E32">
         <v>2</v>
@@ -10876,16 +10916,16 @@
     </row>
     <row r="33" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="B33" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="D33" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="E33">
         <v>2</v>
@@ -10911,16 +10951,16 @@
     </row>
     <row r="34" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="B34" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="D34" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="E34">
         <v>2</v>
@@ -10946,16 +10986,16 @@
     </row>
     <row r="35" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="B35" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="D35" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="E35">
         <v>2</v>
@@ -10984,7 +11024,7 @@
         <v>136</v>
       </c>
       <c r="B36" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>165</v>
@@ -11002,13 +11042,13 @@
         <v>11</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>570</v>
+        <v>560</v>
       </c>
       <c r="I36" s="2">
         <v>0</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>571</v>
+        <v>561</v>
       </c>
       <c r="K36" s="2" t="s">
         <v>11</v>
@@ -11019,7 +11059,7 @@
         <v>137</v>
       </c>
       <c r="B37" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>166</v>
@@ -11054,7 +11094,7 @@
         <v>138</v>
       </c>
       <c r="B38" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>167</v>
@@ -11089,7 +11129,7 @@
         <v>139</v>
       </c>
       <c r="B39" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>168</v>
@@ -11124,7 +11164,7 @@
         <v>123</v>
       </c>
       <c r="B40" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>152</v>
@@ -11136,7 +11176,7 @@
         <v>3</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>11</v>
@@ -11156,13 +11196,13 @@
     </row>
     <row r="41" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="B41" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="D41" t="s">
         <v>269</v>
@@ -11174,13 +11214,13 @@
         <v>11</v>
       </c>
       <c r="H41" s="12" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="I41" s="12" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="J41" s="12" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="K41" s="2" t="s">
         <v>11</v>
@@ -11188,13 +11228,13 @@
     </row>
     <row r="42" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="B42" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="D42" t="s">
         <v>269</v>
@@ -11206,13 +11246,13 @@
         <v>11</v>
       </c>
       <c r="H42" s="12" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="I42" s="12" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="J42" s="12" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="K42" s="2" t="s">
         <v>11</v>
@@ -11220,13 +11260,13 @@
     </row>
     <row r="43" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="B43" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="D43" t="s">
         <v>269</v>
@@ -11238,13 +11278,13 @@
         <v>11</v>
       </c>
       <c r="H43" s="12" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="I43" s="12" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="J43" s="12" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="K43" s="2" t="s">
         <v>11</v>
@@ -11252,13 +11292,13 @@
     </row>
     <row r="44" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="B44" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="D44" t="s">
         <v>269</v>
@@ -11270,13 +11310,13 @@
         <v>11</v>
       </c>
       <c r="H44" s="12" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="I44" s="12" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="J44" s="12" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="K44" s="2" t="s">
         <v>11</v>
@@ -11284,16 +11324,16 @@
     </row>
     <row r="45" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="B45" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="D45" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="E45">
         <v>5</v>
@@ -12327,7 +12367,7 @@
         <v>185</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C29" s="12" t="s">
         <v>209</v>
@@ -12537,7 +12577,7 @@
         <v>191</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>568</v>
+        <v>558</v>
       </c>
       <c r="C35" s="12" t="s">
         <v>353</v>
@@ -12549,7 +12589,7 @@
         <v>2</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>312</v>
@@ -12689,7 +12729,7 @@
         <v>2</v>
       </c>
       <c r="F39" s="12" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>312</v>
@@ -12782,7 +12822,7 @@
         <v>198</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>566</v>
+        <v>556</v>
       </c>
       <c r="C42" s="12" t="s">
         <v>222</v>
@@ -12992,7 +13032,7 @@
         <v>204</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="C48" s="12" t="s">
         <v>228</v>
@@ -13097,7 +13137,7 @@
         <v>207</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="C51" s="12" t="s">
         <v>231</v>
@@ -13129,16 +13169,16 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
-        <v>567</v>
+        <v>557</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>314</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="E52" s="5">
         <v>3</v>
@@ -13164,13 +13204,13 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>313</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="D53" s="5" t="s">
         <v>269</v>
@@ -13185,13 +13225,13 @@
         <v>11</v>
       </c>
       <c r="H53" s="12" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="I53" s="12" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="J53" s="12" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="K53" s="12" t="s">
         <v>11</v>
@@ -13199,16 +13239,16 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
-        <v>569</v>
+        <v>559</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>316</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="E54" s="5">
         <v>3</v>
@@ -13234,13 +13274,13 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="5" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="B55" s="5" t="s">
         <v>315</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="D55" s="5" t="s">
         <v>269</v>
@@ -13255,13 +13295,13 @@
         <v>11</v>
       </c>
       <c r="H55" s="12" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="I55" s="12" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="J55" s="12" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="K55" s="12" t="s">
         <v>11</v>
@@ -13272,13 +13312,13 @@
         <v>317</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>319</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="E56" s="5">
         <v>3</v>
@@ -13304,13 +13344,13 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="5" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>318</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="D57" s="5" t="s">
         <v>269</v>
@@ -13325,13 +13365,13 @@
         <v>11</v>
       </c>
       <c r="H57" s="12" t="s">
+        <v>500</v>
+      </c>
+      <c r="I57" s="12" t="s">
         <v>504</v>
       </c>
-      <c r="I57" s="12" t="s">
-        <v>508</v>
-      </c>
       <c r="J57" s="12" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="K57" s="12" t="s">
         <v>11</v>
@@ -13342,13 +13382,13 @@
         <v>320</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>322</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="E58" s="5">
         <v>3</v>
@@ -13374,13 +13414,13 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" s="5" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="B59" s="5" t="s">
         <v>321</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="D59" s="5" t="s">
         <v>269</v>
@@ -13395,13 +13435,13 @@
         <v>11</v>
       </c>
       <c r="H59" s="12" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="I59" s="12" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="J59" s="12" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="K59" s="12" t="s">
         <v>11</v>
@@ -13412,13 +13452,13 @@
         <v>323</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="C60" s="5" t="s">
         <v>324</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="E60" s="5">
         <v>3</v>
@@ -13444,13 +13484,13 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" s="5" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="B61" s="5" t="s">
         <v>327</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="D61" s="5" t="s">
         <v>269</v>
@@ -13465,13 +13505,13 @@
         <v>11</v>
       </c>
       <c r="H61" s="12" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="I61" s="12" t="s">
+        <v>504</v>
+      </c>
+      <c r="J61" s="12" t="s">
         <v>508</v>
-      </c>
-      <c r="J61" s="12" t="s">
-        <v>512</v>
       </c>
       <c r="K61" s="12" t="s">
         <v>11</v>
@@ -13521,7 +13561,7 @@
         <v>354</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="D63" s="5" t="s">
         <v>333</v>
@@ -13530,7 +13570,7 @@
         <v>6</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="G63" s="5" t="s">
         <v>11</v>
@@ -13545,7 +13585,7 @@
         <v>11</v>
       </c>
       <c r="K63" s="12" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
     </row>
   </sheetData>

</xml_diff>